<commit_message>
Added more news and updated the data.
This is the most recent version as of June 13.
</commit_message>
<xml_diff>
--- a/data_clean.xlsx
+++ b/data_clean.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/busramarsan/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/onurkeles/Documents/GitHub/complingproject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{192D5057-A755-3047-A068-875BFBC9870F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75F4C8E1-D9D0-7842-B1C6-EB8D87314F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="460" windowWidth="24960" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="672">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1007" uniqueCount="889">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -2857,6 +2857,1058 @@
     <t>Denizli’nin Merkezefendi ilçesinde bayan sürücünün kullandığı otomobilin, yan yol bariyerini aşıp hareket halindeki minibüse çarpması sonucu 7 kişi yaralandı.,  , , 
 Edinilen bilgiye göre; Buket S. idaresindeki 20 EG 483 plakalı otomobil Menderes Bulvarı üzerinde seyir halinde ilerlerken, bir başka aracın sıkıştırması sonrası kontrolden çıktı. Kontrolsüz bir şekilde hareket eden otomobil yan yol bariyerini aştıktan sonra ara yolda seyir halindeki Akın Y. idaresindeki 20 M 0443 plakalı şehiriçi minibüsüne ortadan çarptı. Çarpmanın etkisiyle otomobil içerisindeki sürücü Buket S., yolcu bölümündeki Ayhan D., Müjde K. ve Meryem Ö. ile yolcu minibüsü sürücüsü Akın Y. ve ismi öğrenilemeyen iki yolcu yaralandı.,  , , 
 Kazaya ilk müdahaleyi çevredeki esnaf ve vatandaşlar yaptı. Durum hemen itfaiye ve sağlık ekiplerine bildirildi. Olay yerine gelen itfaiye ekipleri araçların güvenliğini sağlarken, sağlık ekipleri de yaralılara ilk müdahale de bulundu. Kaza sonrası yaralanan 7 yaralı tedbir amaçlı hastaneye kaldırıldı. İki araçta da maddi hasar oluşan kazayla ilgili olarak soruşturma başlatıldı.,</t>
+  </si>
+  <si>
+    <t>http://www.gazetevatan.com/vicdanlari-sizlatan-olay-kadin-surucu-kopege-carpip-kacti-1335201-gundem/</t>
+  </si>
+  <si>
+    <t>http://www.kayserihaber.com.tr/haber/ambulansta-kadin-surucu-goren-soforler-36302.html</t>
+  </si>
+  <si>
+    <t>KAPI ZİLİ, KAYSERİSPOR’DA YASAK NASIL KALKACAK?, DUYGUSAL ŞİDDET’İN ANOTOMİSİ, GÜL SİYASETE DÖNER, ÖZHASEKİ İSE ADAY, VOLEYBOL BÖLGESEL LİG HEYECANI KAYSERİ’DE YAŞANACAK, BİRLİK OLMAYAN YERDE DİRLİK OLMAZ, 19 MAYIS, CEMİL BABA,  ,  KANALIMIZA ABONE OL, YEREL BASINA DESTEK OL,  , ,    , , , , , , , , , , , , , , , , , , , , , , , , , , , , , , , , Kayseri´de 4 yıldır ambulans sürüş teknikleri eğiticisi olarak görev yapan acil tıp teknisyeni İmge Geçener, ambulans şoförlerini eğiterek trafiğe hazırlıyor. Geçener, ?Şoförler ambulansta bir kadın gördüklerinde yol vermiyorlar, yarışmaya kalkışıyorlar? dedi., Kayseri´de daha önceleri ambulans şoförlüğü yapan ve aynı zaman da ambulans sürüş teknikleri eğiticisi olarak şoförler yetiştiren acil tıp teknisyeni İmge Geçener, eğitimlere devam ediyor. Belirli aralıklarla ambulans şoförlerinin trafiğe hazırlanmasında yardımcı olan Geçener, erkek şoförlere de taş çıkarıyor., Eğitimler hakkında bilgiler veren Geçener, ?Birkaç yıldır ambulans sürücülüğü yapmıyorum ama öncesinde 5 sene kadar sürücülük deneyimim de oldu. Bölgede kadın olarak tek ambulans sürücüsüyüm. Eğitmen olarak da sadece ben çalışıyorum. Eğitimlerde sürücüleri trafiğe hazırlıyoruz. Ambulans süren arkadaşlarımızın eğitimlerini tamamlıyoruz. Eğer yeni yönetmelik çıktıya onları tekrarlıyoruz. Eğitimlerde araçların teknik özelliklerini, herhangi bir tehlikeyle karşılaştığımızda neler yapmamız gerektiğini, uygun hızda araç kullanılması gerektiğini, lastik, zincir ve akü takmayı ve aracın ufak tefek motor arızalarını öğretiyoruz? ifadelerini kullandı., Trafikte yaşadığı sıkıntıları anlatan İmge Geçener, ?Kadın olarak sürücülük yapmak gerçekten zor. Özellikle ambulans sürücülüğü yapmak çok zor. İlk başta trafikteki insanlar kadın sürücüleri yadırgıyorlar ama ambulansta bir kadın gördüklerinde daha çok sıkıntılı oluyor. Yol vermiyorlar, yarışmaya kalkışıyorlar. İnsanlardan ambulanslara daha fazla duyarlı olmalarını istiyorum. Ambulansın içerisinde kendi yakınları hatta kendileri bile olabilir? şeklinde konuştu.</t>
+  </si>
+  <si>
+    <t>http://www.pusulagazetesi.com.tr/esine-kizan-kadin-surucu-kocasinin-ayagini-ezdi-150282-haberler.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eşine kızan kadın sürücü, kocasının ayağını ezdi,  10-07-2020 | 21 : 48 43 , Zonguldak'ın Ereğli ilçesinde, iddiaya göre eşine kızan bir kadın, otomobille eşinin ayağının üzerinden geçti.Olay, akşam saatlerinde, Müftü Mahallesi İsmail Sidal Sokak'taki otopark alanında meydana geldi.İddiaya göre; eşine kızan bir kadın, otomobilini eşinin üzerine sürerek ayağının üzerinden geçti. Acı içinde yerde kalan yaralıyı gören vartandaşlar, durumu 112'ye bildirdi. Olay yerine gelen 112 sağlık ekibi, ayağı kırılan yaralıya ilk müdahalesini yaptıktan sonra Özel Anadolu Hastanesi'ne kaldırdı.Olay ile ilgili soruşturma başlatıldı.,  , Haber : Pusula, ETİKETLER : Yazdır, , La arkadaş bu ereğlide teksas gibi hergün ayrı ayrı olaylar bi gün uslu durun ya,  Beğen, , , , Günün Pusula Gazetesi'ni okuyabilirsiniz. PDF formatında indirebilirsiniz., , ETİKET, </t>
+  </si>
+  <si>
+    <t>http://www.yildirimgazetesi.com/gundem/kadin-surucu-kanala-uctu-h61222.html</t>
+  </si>
+  <si>
+    <t>10.1213, 8.3655, 1461, 506.359, , Bursa-Ankara yolunda meydana gelen kazada kontrolden çıkan otomobil su kanalına uçtu, kadın sürücü yaralandı._x000D_
+Kaza Bursa-Ankara yolunun Kestel ilçesi mevkiinde meydana geldi., , Yorumunuz Onaylanmak Üzere Gönderildi, İMSAK, 03:31, 
+_x000D_
+ (adsbygoogle = window.adsbygoogle || ).push({});_x000D_
+, 
+_x000D_
+ (adsbygoogle = window.adsbygoogle || ).push({});_x000D_
+, Yıldırım Gazetesi bir Metropol Ajans kuruluşudur., Tüm Hakları Saklıdır. Yıldırım Gazetesi -  Copyright © 2021</t>
+  </si>
+  <si>
+    <t>https://abcgazetesi.com/antalyada-motosiklet-kullanan-kadin-surucu-epilepsi-nobeti-gecirdi-383097</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antalya'da kullandığı motosikletin üzerinde epilepsi nöbeti geçiren Meltem B. (39), ölümden döndü. Motosikletiyle yaklaşık 500 metre boyunca kontrolsüz bir şekilde ilerleyip demir korkuluklara çarpan Meltem B.'nin araçların altında kalmaktan son anda kurtulduğu anlar, kameraya yansıdı., Olay, sabah saatlerinde Muratpaşa ilçesi Adnan Menderes Bulvarı'nda meydana geldi. Meltem B., motosikletle seyir halindeyken epilepsi nöbeti geçirdi. Meltem B.'nin kontrolünü kaybettiği motosiklet, sürekli şerit değiştirmeye başladı. Bu sırada solundan geçen bir otomobile sıfır mesafede yaklaşan motosiklet, son anda yapılan manevrayla çarpmaktan kurtuldu. Kontrolsüz şekilde ilerlemeye devam eden Meltem B., çift yönlü bulvarda bu kez sol şeride geçerken, motosikletiyle orta bölümde yer alan demir korkuluklara çarptı. Meltem B., çarpmanın etkisiyle ilk olarak korkuluklara, ardından yola savruldu., Meltem B., korkuluklar sayesinde karşı şeritten gelen araçların altında kalmaktan kurtuldu. Arkasından gelen cipin sürücüsünün dikkati sayesinde Meltem B., ölümden döndü., İhbar üzerine bölgeye polis ve sağlık ekipleri sevk edildi. Sağlık ekipleri Meltem B.'ye ilk müdahaleyi ambulansta yaptı. Meltem B., epilepsi nöbeti geçirdiğini ve iyi olduğunu söyleyerek hastaneye gitmeyi kabul etmedi., ARAÇ KAMERASINA YANSIDI, Epilepsi nöbeti sırasında Meltem B.'nin motosikletiyle yaklaşık 500 metrelik yolu kat ettiği anlar araç kamerasına yansıdı. Görüntülerde Meltem B.'nin sürekli şerit değiştirdiği, alt geçitte demir korkuluklara çarptığı, arkasından gelen araçların altında kalmaktan son anda kurtulduğu görüldü. İşte o görüntüler..., , , 
+Kaynak: </t>
+  </si>
+  <si>
+    <t>Üreticiler Ezilmesin, Karanlık Çağ, Deniz Rüyası..., Yoğun Spor Yapmayın, Alternatif, Bedava Gibi Reklamını Yaptırmak ve  Bir Sporcuya Dokunmak İster Misin?     </t>
+  </si>
+  <si>
+    <t>https://dogruhaber.com.tr/haber/626729-kadin-surucu-fren-yerine-gaza-basinca-olanlar-oldu/</t>
+  </si>
+  <si>
+    <t>Olay, Eyüpsultan Çırçır Mahallesi'nde saat 16.20 sıralarında meydana geldi. İddiaya göre, evine gelen yabancı uyruklu kadın sürücü Zınep R., aracını park etmeden önce iki çocuğunu aşağı indirdi. Çocuklarını indirdikten sonra 34 MN 3395 plakalı otomobili park etmek isteyen kadın sürücü, gaz yerine frene bastı. Aracın kontrolünü kaybeden sürücü, yolun karşısında bulunan şantiye alanının sac korumalarına çarptı., Sac korumaları da deviren otomobil yaklaşık 9 metre yükseklikten aşağı uçtu. İnşaat demirlerinin üzerine düşen otomobilin içindeki Zınep R.'yi çevredeki vatandaşlar aracın camını kırarak kurtardı. Yaralanan kadın sürücü olay yerine gelen 112 Acil Servis ekiplerince ambulansla hastaneye kaldırıldı. Kadın sürücünün sağlık durumunun iyi olduğu öğrenilirken, araç ise vinç yardımıyla inşaat alanından çıkartıldı. (İHA), , Milli Eğitim Bakanlığı (MEB), ilkokul, ortaokul ve lise öğrencilerinin karne ve başarı belgelerinin 18 Haziran'da erişime açılacağını bildirildi., Van'ın Muradiye ilçesinde, jandarma ekipleri tarafından yapılan çalışmalarda meyve suyu paketi içerisine gizlenmiş 50 gram metamfetamin ele geçirildi., Sitemizde yayınlanan haberlerin telif hakları gazete ve haber kaynaklarına aittir..</t>
+  </si>
+  <si>
+    <t>Serdivan Eski Kazımpaşa Caddesi’nde iftar saatine az bir süre kala meydana gelen trafik kazasında, motosikleti ile evine giden bir bekçi yaralandı. Kadın sürücü ise kaza sonrası şok yaşadı…
+, Kaza,  Serdivan ilçesi Eski Kazımpaşa Caddesi üzerinde meydana geldi., Edinilen bilgilere göre, M.A. isimli kadın sürücünün kullandığı otomobil ile Göksel B. isimli bekçinin idaresindeki motosiklet çarpıştı., Kazanın şiddetiyle motosiklet ve sürücüsü yola savruldu. Kazayı görenler ilk  yardım için hemen bekçinin yanına koşarken, kazaya karışan otomobilin sürücüsü şok yaşadı., Haber verilmesi ile kaza yerine gelen 112 acil ekipleri, yaralı bekçiye ilk müdahaleyi yaptıktan sonra ambulans ile hastaneye kaldırdı., Kazayla ilgili inceleme başlatıldı., 
+01 May 2021 - 19:53
+Sakarya-
+Güncel
+--- Okunma
+Yazdır
+, medyabar.com son bir ayda 2.843.678 kez ziyaret edildi., Yorumunuz yarım kaldı, devam etmek için üstteki yoruma, silmek için buraya tıklayın, Kırmızı alanlar eksik veya hatalı girildi. Lütfen bu alanları düzeltip tekrar gönderelim, Yorumunuz için teşekkürler, en kısa sürede gözden geçirilip yayınlanacaktır, Yorum yazarak Medyabar Topluluk Kuralları’nı kabul etmiş bulunuyor ve yorumunuzla ilgili doğrudan veya dolaylı tüm sorumluluğu tek başınıza üstleniyorsunuz. Yazılan yorumlardan Medyabar hiçbir şekilde sorumlu tutulamaz., Anadolu Ajansı (AA), İhlas Haber Ajansı (İHA), Demirören Haber Ajansı (DHA) tarafından servis edilen tüm haberler Medyabar editörlerinin hiçbir editöryel müdahalesi olmadan, ajans kanallarından geldiği şekliyle yayınlanmaktadır. Sitemize ajanslar üzerinden aktarılan haberlerin hukuki muhatabı Medyabar değil haberi geçen ajanstır., Şimdi oturum açın, her yorumda isim ve e.posta yazma zahmetinden kurtulun. Oturum açmak için bir hesabınız yoksa, oluşturmak için buraya tıklayın.
+, Yorum yazarak  Medyabar Topluluk Kuralları’nı kabul etmiş bulunuyor ve yorumunuzla ilgili doğrudan veya dolaylı tüm sorumluluğu tek başınıza üstleniyorsunuz. Yazılan yorumlardan Medyabar hiçbir şekilde sorumlu tutulamaz., Anadolu Ajansı (AA), İhlas Haber Ajansı (İHA), Demirören Haber Ajansı (DHA) tarafından servis edilen tüm haberler Medyabar editörlerinin hiçbir editöryel müdahalesi olmadan, ajans kanallarından geldiği şekliyle yayınlanmaktadır. Sitemize ajanslar üzerinden aktarılan haberlerin hukuki muhatabı Medyabar değil haberi geçen ajanstır., Ramazan Keser - bu yasaklarda ne kazasi yav allah askina yeterin da uyun yasaklara markete diye cikiyonuz her yere gidiyonuz yollar full dolu yaziklar olsun ne diyelim, Eyüp İktisatçı - Kazadır , kimse kimseye bilerek vurmaz.Allah beterinden korusun, B - Bu kaza dünya üzerinde gerçekleşen ne ilk kaza olmuş, ne de son kaza olacak. Kadın-erkek üzerine ayrıştırıcı yorumlar yapacağınıza; "herkesin haklıda olsa haksızda olsa başına gelebileceği" bu tür kazaları nasıl en az seviyeye indirgeyebiliriz onu tartışalım. Evet telefon, kemer bu tür şeyler dikkatsizliğe yol açıyor ve kazaya sebep oluyor. Ancak erkekler taş devrinde mi yaşıyorlar da telefondan haberleri yok? Herkesin elinde telefon, müzik.. Her gün evden çıktığımda arabayla yanlayan, hız yapmaktan zevk alan erkeklerle karşılaşıyorum. İki tarafa da geçmiş olsun, Allah beterinden korusun.., Fahrettin Kocaman  - Değerli dostlar kadın sürücü,erkek sürücü yok diye ayrımcılık yapmayalım trafiğe çıkan herkes bilinçli araç kullanırsa kurallara uyarsa sıkıntı yok ama malesef görünen köy kılavuz istemez arabaya oturanın ayranı kabarıyor meskün mahalde ne kadar hızla gidileceği bellidir lakin kazanın yaşandığı cadde yarış pisti gibi herkes bir yarış içinde ne gerek var üç dakka geç gitsen ne kaybedersin sanki. bekçi kardeşimize geçmiş olsun Allah acil şifalar versin inşaallah lütfen birbirimize saygılı olalım , Ellidört - Geçmiş olsun yazacağınıza yazdığınız şeylere bakın , M - Hiçbir haberinizde erkek sürücü diye belirtmiyorsunuz da kadın olunca mı manşete kadın sürücü ibaresini koyuyorsunuz!.. , Sorun sadece imlada değil , zihninizde ., M - @M 05 nolu yoruma cevabı: Çok haklısınız bazı erkek sürücüler de aynı dediğiniz gibi canlı bomba . Bunun cinsiyeti olmadığını kabul etmelisiniz ki eleştirim kazaya değil haberi yapan editöre. Ayrıca şunu da belirtmeliyim ki 12 senede bir defa kazaya karıştım . Haklıydım çünkü ERKEK SÜRÜCÜ sinyal vermeden kulağında telefonuyla sola dönüş yaptı . , Diyeceğim o ki kazadır olur , kadın erkek fark etmez. Ancak haber böyle yapılmaz !.., becks - @M 05 nolu yoruma cevabı: 3 kere kazaya karıştım, 3 kazada da 100%100 haklıyım resmi olarak, 3’üde kadındı. kabul edin artık motor becerileriniz, erkeklere göre daha az çalışıyor. burada kadın erkek kıyaslaması yapmıyorum sadece bazı kadınlar gerçekten canlı bomba gibi trafikte geziyor. , Vatandaş - Yasak var daha yolda yürümeyi beceremeyen bayanlar araç kullanıyor üstelik bir çoğu elinde tel direksiyonda geçmiş olsun , Osman - @Vatandaş 04 nolu yoruma cevabı: Hafız haklı olabilirsin çünkü kadın şok geçirir iken bile telefon elde , Badenur  - elinde telefon ile araba sürme cabası olursa kazalar böyle oluşur , Vatandaş - @Badenur 02 nolu yoruma cevabı: Görmedim ama geneli böle trafikte gördüğümüz birde yasak saati yürüme mesafesi dendi dimi eşofmanla işe de gidilmiyor heralde tabki kimsenin başına gelmesin ama dikkat ve kendinden emin olmadan trafiğe çıkılmaz uyandırayım, Görgüsüz Şahit  - @Badenur 02 nolu yoruma cevabı: Gördün mü???, Egm Bekçi - Çok geçmiş olsun ramazan ayında kazalar dikkat dağınıklığından dolayı daha çok oluyor lütfen yavaş kullanalım şu araçları., Yazılan yorumlardan Medyabar hiçbir şekilde sorumlu tutulamaz. Sitemizin Topluluk Kurallarına uymayan yorumlar yayınlanmaz. Yorumunuzla ilgili doğrudan veya dolaylı tüm sorumluluğu tek başınıza üstleniyorsunuz. , Anadolu Ajansı (AA), İhlas Haber Ajansı (İHA), Demirören Haber Ajansı (DHA) tarafından servis edilen tüm haberler Medyabar editörlerinin hiçbir editöryel müdahalesi olmadan, ajans kanallarından geldiği şekliyle yayınlanmaktadır. Sitemize ajanslar üzerinden aktarılan haberlerin hukuki muhatabı Medyabar değil haberi geçen ajanstır., Sitemizde  online, Reklam seçeneklerimizi inceleyin, 
+©Copyright 2021 Medyabar Tüm Hakları Saklıdır
+-
+Veri PolitikasıKullanım Şartları
++90 (264) 273 53 53
+,  Veri politikasındaki amaçlarla sınırlı ve mevzuata uygun şekilde çerez konumlandırmaktayız. Detaylar için veri politikamızı inceleyebilirsiniz.</t>
+  </si>
+  <si>
+    <t>Reema Juffali’nin dediğine göre kendisi asla böyle bir şeyi beklemezken, geçtiğimiz sene içerisinde Suudi Arabistan’da kadın sürücülere karşı çıkan yasanın kaldırılmasıyla, kendisini bu tecrübeyi yaşarken buldu., Böylesine adrenalin dolu hız sporları, aşırı tutucu bir İslam krallığı olan Suudi Arabistan’da geçtiğimiz Haziran'da kadınlara yönelik araç kullanmayı kısıtlayan yasanın kaldırıldığı zamana kadar düşünülmeyecek bir şeydi. Prens Mohammed bin Salman’ın emirleriyle değiştirilen bu olgu, beraberinde birçok değişikliği de getirmiş gibi gözüküyor. Hadi bu değişim konusunu biraz daha irdeleyelim., Juffali: Yasa geçen sene kalkana kadar böyle bir düşüncem bile yoktu. Direksiyonun arkasına bile geçme fırsatı yakalayamayan, bu tecrübeyi deneyimleyemeyen milyonlarca kadının varlığını bilmek çok üzücü, yarışırken onların hepsi için bunu yapıyorum., Suudi Arabistan Spor Kurumu'nun yetkili sorumlusu olan Prens Abdulaziz bin Turki al-Faisal, bunun krallık için bir dönüm noktası olacağını söylerken, Juffali'nin şimdiden toplumun gözdesi olduğunu da vurguluyor., Ancak genç yaşından beri engelleyemediği ve bunu takip etmesine sebep olan bir tutkusu vardı, hızlı arabalar… Formula 1’i izleyerek büyüdü, birkaç yıl önce okumak için taşındığı Amerika Birleşik Devletleri'nde girdiği sürüş testini başarıyla geçerek, yarışmalara katılabilmek için lisansını aldı. , Fransa'da yapılan ve 24 saat boyunca süren, dünyanın en prestijli ve yorucu yarışlarından biri olan Le Mans’a katılmayı çok istediğini belirtti genç kadın. Riyad'da ise sezonun kıdemlilerine karşı yarışacak, fakat puan kazanmayacak., Ancak reformların yanı sıra, düşüncelerini açıkça belirtmek isteyen insanlara karşı kapsamlı bir baskı başlamıştı ve muhaliflere karşı yürüttüğü bu genel baskı, otoriter imajını da ortaya çıkarıyor., Araba kullanabilme hakkı için uzun süredir eylemler yürüten bir düzine kadın eylemci, geçen yıl tutuklandıktan sonra yargılanmış ve bu, Prens Muhammed’in toplumda geniş çaplı olarak kınanmasına yol açmıştı. Bazıları, sorgulama esnasında işkence gördüklerini ve cinsel tacize uğradıklarını iddia ederken; erkek egemen ve otoriter toplumlarda alışık olduğumuz gibi Suudi yetkililer de iddiaları reddediyor., Kadınların araba tercihlerine yönelik kalıplar da yavaş yavaş toplumdan silinmeye şimdiden başladı. Kadın müşterilerle ilgili röportajlar yapan otomobil galerileri, vişne çürüğü Mini Cooper’ların en çok tercih edilen model olduğunu belirtse de satış uzmanları, “Kadınların çoğu, Chevrolet Camaro veya Mustang gibi üstü açılır ve kaslı otomobiller için sıraya giriyor” diyor., Juffali, “Pek çok insan burada meydana gelen değişimlere karşı hala çok şaşkın, beni bir arabada yarışırken görmeye inanamayan yarışçılara denk geliyorum. Birçok insan için bu sürpriz ama insanları şaşırtmaktan mutluyum. Her şeye rağmen düşüncenizi savunmaya devam edin, bir farklılık olmanız sizi hastalıklı değil daha güçlü birisi yapar” diyor., Demedi demeyin bu araplar hızla gelişiyor çok yakın bir zamanda yallah Arabistana sözü yallah Türkiyeye'ye evrilebilir.., Demedi demeyin bu araplar hızla gelişiyor çok yakın bir zamanda yallah Arabistana sözü yallah Türkiyeye 'ye evrilebilir.., herkese umut mu olacak?!!! ulan niye yasak zaten., onedio.com sosyal içerik platformu, IOS ve ANDROID CİHAZINIZA İNDİRİN</t>
+  </si>
+  <si>
+    <t>Bu içerik Onedio üyesi kullanıcı tarafından üretilmiş, Onedio editör ekibi tarafından müdahale edilmemiştir. Siz de Onedio’da dilediğiniz şekilde içerik üretebilirsiniz., Bu işe bir nokta koymanın vakti gelmişti de geçiyordu bile... , Fikirlerinizi ya da o çok tarafsız 'deneyimlerinizi' bir kenara bırakıyorsunuz şimdi; çünkü gerçekleri, sadece gerçekleri bilimsel verilerle konuşacağız!, Kadın sürücüler konusunda hemen hemen herkesin söyleyecek bir sözü, yapacak bir şakası mutlaka vardır. Bu "kadın sürücü" iddiaları önce zararsız bir şakaymış gibi sunulur, ardından belli başlı anılar anlatılır... Sonuç itibariyle de tüm bu iğrenç düşünce akışı, kadınların erkeklerden daha beceriksiz, daha düşük olduğu algısına hizmet eder. , Kısacası "duyar kasmak" denilip geçilmeyecek kadar ciddi bir mevzu, bu kadın sürücü mevzusu... Bu aşağılayıcı geyikler çocuklarımızın kulaklarına kadar gidiyor ve kız çocuklarının zihnine "Ben yapamam" fikrini kazıyıp öz güvenlerini kırdığı gibi, erkek çocuklara da kadınlardan daha üstün olduğu düşüncesini aşılıyor., Hatırlarsanız Suudi Arabistan'da kadınlara araba kullanabilme hakkı geçtiğimiz yıllarda verilmişti. Bu gelişmeye bir yandan Suudi kadınlar adına sevinmiş, bir yandan da şaşırarak "Böyle bir hakları yok muydu yani?! Ne saçma ve çağ dışı!" diye eleştirmiştik. , Ne saçmaydı değil mi, şu yaşadığımız çağ içerisinde kadınların araba kullanmasının yasak olduğu bir ülke olması..., Peki böyle saçma sapan yasaklara hunharca karşı çıkarken ve uygulanmasını absürt bulurken, neden bir taraftan sık sık 'kadın sürücü' şakaları yapıyoruz ya da bu şakaları tolere ediyoruz? Bu işte bir çelişki var!, Hadi internet alemi zaten ofansif paylaşımlardan geçilmiyor diyeceğiz fakat, dahası da var..., Akıl alır gibi değil!, Kadın sürücünün cinsiyeti daima belirtiliyor. Bunda art niyet fazlasıyla var. Hepsini açıklayacağız şimdi..., Bu noktada "Sizin bir keresinde şahit olduğunuz, gözünüzle gördüğünüz." olaylar değil; bizzat bu araştırmaları tarafsız ve gerçek kayıtlara dayanarak yapan uzmanların rakamları önemli., Dünya genelinde de, ülkemizde de kadın sürücülerin sayısının en hızlı arttığı yıl 2007 olarak gösteriliyor. O yüzden önce 2007 yılına bakalım:, TUİK'e göre ülkemizde o sene: Ölümlü yaralanmalı trafik kazalarına, 133 bin 778 sürücü karıştı. Bu sürücülerin yüzde 93'ünü erkekler, yaklaşık yüzde 7'sini kadınlar oluşturdu. , Bu patlamanın yaşandığı, yani trafikteki kadın sürücü sayısının, erkek sürücü sayısını geçtiği tarihten sonra, 2013'te bile, Yol Güvenliği Sigorta Enstitüsü'nün verilerine göre Amerika'da motorlu taşıt kazalarının %71'ini erkekler yaptı. Kadınlar ise %29'da kaldı. , Türkiye'de mi? Türkiye'de 2006 yılından 2012 yılına kadar trafikteki kazaların %95'inin erkekler tarafından yapıldığı ANKARA Üniversitesi Tıp Fakültesi Halk Sağlığı Ana Bilim Dalı Başkanı Prof. Dr. Recep Akdur’un “Türkiye’deki Trafik Kazalarının Epidemiyolojik İlkeleri Işığında Değerlendirilmesi” çalışmasında gösterildi., Trafikte en çok tehlike oluşturan, kural ihlalinde bulunan sürücüler ise 18-22 yaş arası erkekler olarak açıklandı., Yani trafikte gördüğünüzde sizi tehlikeye atacağından korkmanız, temkinli olmanız gereken kişi, kadın sürücü değil; 20li yaşlardaki bir erkek sürücü., Alkollü araç kullanma, hız limiti aşma gibi kural ihlallerinde de erkek sürücüler, kadın sürücüleri fazlasıyla geçiyor., Erkeklerin trafikte hız aşımı ile kontrolden çıkma gibi ölümcül hataları olurken; kadınların ise çevrelerindeki herkesin hayatından sorumlu hissederek daha temkinli ve yavaş davrandıkları gözlemleniyor., Yani yansıtıldığı ve şakası yapıldığı gibi;, Direksiyon başında aynaya bakarak makyaj yapmaktan,, Telefonda dedikodu yapmaktan,, Gerizekalı oldukları için becerememekten dolayı değil;, İnsan hayatına dair sorumluluk hissettikleri için "makas atan usta sürücü" kategorisine girmiyorlar belki de..., Göz göze gelindiği anda dahi bunu bir mesaj gibi anlayan erkek sürücüler tarafından tacize uğrayan, sıkıştırılan kadın sürücülerin tehlikeli kazalara karışmaları son derece yaygın., Çünkü söz konusu para olunca; cinsiyetçi önyargılara göre değil, gerçek rakamlara göre hareket ediyorlar ve rakamlar, erkeklerin daha çok kaza yapan sürücüler olduğunu gösteriyor., 100 yıl öncesine kadar oy dahi kullanamayan bir cinsin çocukları olarak hayatın her alanına yayılıyoruz. Kurduğumuz yeni dünyada ise "Kadınlar iyi araba kullanamaz, kadınlar trafikten alınsın" gibi hafif cinsiyetçi söylemleri devam ettirenlere dahi yer olmayacak., Trafikte kazan yapan bir erkeği görünce "Salağa bak" deyip geçen ve asla cinsiyete takılmayan, fakat kaza yapan bir kadını görünce "işte bu yüzden kadınlara ehliyet verilmemeli, kadınlar şöyle böyle" diye konuşan gerikafalı insanların algı oyununa düşmeyin., Rakamlar, kazaların çoğunluğunun erkekler tarafından yapıldığını gösteriyor. Hiç kulak asmayın!, Bu içerik Onedio üyesi kullanıcı tarafından üretilmiş, Onedio editör ekibi tarafından müdahale edilmemiştir. Siz de Onedio’da dilediğiniz şekilde içerik üretebilirsiniz., Bu konuyla ilgili bir erotik hikaye anlatiyim.Sene 3000li yillar Dunyaya artik kadinlar egemen olmus yani Anaerkil bir toplum.Isleri kadinlar ve robotlar yapiyor. Kadinlar sadece sperm uretemiyor ve erkegin bu distopik dunyada gorevi sadece sperm uretmek. Tum erkekler hayvan ciftligine benzer bir mekanda sagma makinelerina bagli ve sagiliyor. Sagildiktan sonra uyuyor dinleniyor yine sagiliyor. Bu ergenlikten olunceye kadar devam ediyor.Spermler de insanoglunun nesli icin kullaniliyor. Heleki genetigi iyi biriyseniz iyice sagiliyorsunuz son damlasina kadar. Bu gibi senaryo Blood Drive dizisinde de vardi. Anlayacaginiz gidisat o yonde. Bir gun sagmaya gelecekler bizi., Ben de daha ilk an itibari ile anlıyorum bir sürücünün kadın mı erkek mi olduğunu... _x000D_
+gerektiğinde sinyal veriyor, hatalı sollama yapmıyor, hız sınırına uyuyor vs. vs. yani kurallara uyup ilerliyorsa ''kadın şöfördür''. Biz erkeklerin problemi bu kuralları hiçe sayınca iyi şöför olduğumuzu düşünmemiş. Nereden mi biliyorum? Dün oturumumu uzatmak için evraklarımı teslim ederken yüklü trafik cezaları ile karşılaştım, sinirle kız arkadaşıma bunların hepsi senin eserin dedim ama tarihlere baktığımda tamamının benim olduğu ortaya çıktı., Yani bunun da cinsiyetçi birisi tarafından hazırlandığı çok belli. Kötü erkek sürücülerin olması kadınların trafikte çok acemice davrandığı, kötü araba kullandığı gerçeğini değiştirmez. Tecrübeyle sabit. Ancak yiğidi öldür hakkını yeme demişler. Kadınlar metro ve tramvayları erkeklerden daha iyi kullanıyor. Yine tecrübeyle sabit., Ya şimdi bir kadın sürücü olarak bu hassas bir konu falan da, erkek gibi araba kullanan bir sürücü olarak şunu söyleyebilirim ki, bazı kadınlar da gerçekten aşırı ürkek ve mıymıntı araba kullanıyor. Sol şeridi 70'le işgal eden mi ararsın, kavşaktan dönerken arabanın gaz fren ayarını yapamayıp bir hızlanıp bir yavaşlayarak arkasında beni fıtık eden mi ararsın, arabayı sağa sola yalpalatan mı ararsın, böyle sürüyle örnek sayabilirim. Bu tarz hareketler trafik seyrinde diğer sürücüleri de tehlikeye atıyor, kendi aracınızla normal hareket akışınızda alışılmadık bir kesinti çıkıyor çünkü, yalnızca "sinir olmak" değil yani mevzu. Trafikte ne kadar uyuz hareket eden araç gördüysem onları sollamadan önce "kesin kadın" dedim ve %95 doğru çıkıyor bu tespitlerim. Biraz da özgüven ve atik - çevik araba kullanmayı öğrenin ama artık yani siz de, madem cinsiyetçi yaklaşımdan bıktınız. Buna direksiyon ağzınıza girecek kadar koltuğunuzu öne çekmekten artık vazgeçerek başlayabilirsiniz mesela., simdi bir kadin surucu olayi var ama bunun nedeni cinsiyet degil tecrube kaynakli. turkiyede cok az ailenin birden fazla araci var ve araba kullanmak erkek gorevi gibi goruluyor, cogunlukla erkek kullaniyor, hatta ailenin erkek cocugu erken yasta gorevi alip kullanmaya basliyor. kadinlar nadiren arac kullandiklarindan tecrubeleri az. erken yasta kendi arabalarini alip kullanan kadinlarda gordugum mukemmel kullaniyorlar, eksikleri yok fazlalari var. kaza oranina gelirsek, gayet normal kadinlar sorumluluk sahibi daha dikkatliler, riskli tehlikeli ise kolay kolay girmezler. bu sadece insanda degil tum memelilerde boyle. turun devami olarak disi riskden uzak durur, erkek ise daha fazla riske girerek potansiyel kazancin pesinde kosar. neticede bir populasyonda erkek sayisi yariya inse bile populasyonun gidisi cok sarsilmaz., onedio.com sosyal içerik platformu, IOS ve ANDROID CİHAZINIZA İNDİRİN]</t>
+  </si>
+  <si>
+    <t>ANTALYA’nın Alanya ilçesinde hafif ticari aracıyla köprüden uçan sürücü Nursel Yıldız (39), yaşamını yitirdi.
+Alanya’nın Türkler Mahallesi’nde dün gec..., ANTALYA’nın Alanya ilçesinde hafif ticari aracıyla köprüden uçan sürücü Nursel Yıldız (39), yaşamını yitirdi., Alanya’nın Türkler Mahallesi’nde dün gece meydana gelen kazada Nursel Yıldız’ın kullandığı 07 NLK 65 plakalı hafif ticari araç, sürücünün direksiyon hakimiyetini kaybetmesi sonucu Ali Çavuşoğlu Köprüsü’nden Kargı Çayı’na uçtu. Çevredekilerin ihbarı üzerine olay yerine Alanya İlçe Jandarma Komutanlığı ekipleri, Antalya Büyükşehir Belediyesi itfaiye ekipleri ve 112 ekipleri sevk edildi. İtfaiye ekiplerinin çabasıyla araç içerisinden çıkarılan Nursel Yıldız’ın yaşamını yitirdiği belirlendi. Yıldız’ın cansız bedeni otopsi yapılmak üzere Antalya Adli Tıp Kurumu’na gönderilirken, kazayla ilgili soruşturma başlatıldı., , , 
+25 May 2020 - 09:11
+Antalya-
+Asayiş
+Yazdır
+, akdeniztelgraf.com son bir ayda 59.820 kez ziyaret edildi., Yorumunuz yarım kaldı, devam etmek için üstteki yoruma, silmek için buraya tıklayın, Kırmızı alanlar eksik veya hatalı girildi. Lütfen bu alanları düzeltip tekrar gönderelim, Yorumunuz için teşekkürler, en kısa sürede gözden geçirilip yayınlanacaktır, Yorum yazarak Akdeniz Telgraf Gazetesi Topluluk Kuralları’nı kabul etmiş bulunuyor ve yorumunuzla ilgili doğrudan veya dolaylı tüm sorumluluğu tek başınıza üstleniyorsunuz. Yazılan yorumlardan Akdeniz Telgraf Gazetesi hiçbir şekilde sorumlu tutulamaz., Anadolu Ajansı (AA), İhlas Haber Ajansı (İHA), Demirören Haber Ajansı (DHA) tarafından servis edilen tüm haberler Akdeniz Telgraf Gazetesi editörlerinin hiçbir editöryel müdahalesi olmadan, ajans kanallarından geldiği şekliyle yayınlanmaktadır. Sitemize ajanslar üzerinden aktarılan haberlerin hukuki muhatabı Akdeniz Telgraf Gazetesi değil haberi geçen ajanstır., Şimdi oturum açın, her yorumda isim ve e.posta yazma zahmetinden kurtulun. Oturum açmak için bir hesabınız yoksa, oluşturmak için buraya tıklayın.
+, Yorum yazarak  Akdeniz Telgraf Gazetesi Topluluk Kuralları’nı kabul etmiş bulunuyor ve yorumunuzla ilgili doğrudan veya dolaylı tüm sorumluluğu tek başınıza üstleniyorsunuz. Yazılan yorumlardan Akdeniz Telgraf Gazetesi hiçbir şekilde sorumlu tutulamaz., Anadolu Ajansı (AA), İhlas Haber Ajansı (İHA), Demirören Haber Ajansı (DHA) tarafından servis edilen tüm haberler Akdeniz Telgraf Gazetesi editörlerinin hiçbir editöryel müdahalesi olmadan, ajans kanallarından geldiği şekliyle yayınlanmaktadır. Sitemize ajanslar üzerinden aktarılan haberlerin hukuki muhatabı Akdeniz Telgraf Gazetesi değil haberi geçen ajanstır., Reklamlarla ilgili talepleriniz veya detaylı bilgi almak için email protected adresini kullanarak bizimle iletişime geçebilirsiniz., 
+Seri İlan sayfası için buraya tıklayın.
+Günlük 5 TL den başlayan fiyatlarla ilanınızı şimdi oluşturun
+, Aylık 365₺'den başlayan fiyatlar ile sizleri bekliyor..., +90 (532) 553 36 59  Reklam bilgi, Sitemizde  online, Reklam seçeneklerimizi inceleyin, Gazetemizin üye olduğu kuruluşlar., Gazetemizin üyesi olduğu haber ajansları, 
+©Copyright 2021 Akdeniz Telgraf Gazetesi Tüm Hakları Saklıdır
+-
+Veri PolitikasıKullanım Şartları
++90 (532) 553 36 59
+,  Veri politikasındaki amaçlarla sınırlı ve mevzuata uygun şekilde çerez konumlandırmaktayız. Detaylar için veri politikamızı inceleyebilirsiniz.</t>
+  </si>
+  <si>
+    <t>https://www.aydinhedef.com.tr/motosikletli-kadin-surucu-yaralandi-13181h.htm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AYŞE AKTAŞ- Kaza, Nazilli'nin Cumhuriyet Mahallesi Beşeylül caddesi üzerinde meydana geldi. Alınan bilgiye göre Havva S. Ö. idaresindeki 09 B 2825 plakalı motosiklet ile Kasım Ç. idaresindeki 34 BİC 763 plakalı otomobil çarpıştı. Çarpmanın etkisiyle motosiklet sürücüsü Havva S.Ö. savrularak yaralandı. Çevredekilerin ihbarı üzerine bölgeye 112 Acil Sağlık ve polis ekipleri sevk edildi. Yaralı kadın sürücü, ambulansla Nazilli Devlet Hastanesine kaldırıldı. Olayla ilgili soruşturma başlatılırken kadın sürücünün durumunun iyi olduğu öğrenildi. , </t>
+  </si>
+  <si>
+    <t>https://www.aydinhedef.com.tr/nazillide-2-kadin-surucu-kafa-kafaya-carpisti-20859h.htm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AYŞE AKTAŞ - Kaza, Yeşil Mahalle Atatürk Bulvarı'nda 17:30 sıralarında meydana geldi. Alınan bilgiye göre 654 Sokak'tan Atatürk Bulvarı’na seyreden S.O. idaresindeki 09 RZ 218 plakalı otomobil ile hastane istikametinden Arslanlı Mahallesi istikametine seyreden B.K. idaresindeki 09 CBD 87 plakalı motosiklet kafa kafaya çarpıştı. , Kazayı gören vatandaşlar durumu sağlık ve polis ekiplerine bildirdi. , Çarpışmanın etkisiyle yola savrulan ve yaralanan motosiklet sürücüsü B.K. ambulansla Nazilli Devlet Hastanesi’ne kaldırılırken, sürücünün hayati tehlikesinin bulunmadığı öğrenildi., Polis kazayla ilgili inceleme başlattı., </t>
+  </si>
+  <si>
+    <t>https://www.aynahaber.net/haberler/asayis/denizlide-otomobil-takla-atti-kadin-surucu-yarali/29428/</t>
+  </si>
+  <si>
+    <t>Access to this resource on the server is denied!</t>
+  </si>
+  <si>
+    <t>Please enable Cookies and reload the page., This process is automatic. Your browser will redirect to your requested content shortly., Please allow up to 5 seconds…, Redirecting…</t>
+  </si>
+  <si>
+    <t>https://www.bursa.com/yasli-adama-bu-sekilde-carpti-n458057/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> , Önceki hafta Salı günü saat 14.45 sıralarında Şişli Merkez Mahallesi'nde meydana gelen olayda, edinilen bilgiye göre yabancı uyruklu Widline Erie, arkadaşlarıyla birlikte öğrenci yurduna eşya taşımaya başladı. Bir süre sonra taşıma işlemini bitiren Erie, otomobiline bindi. Yola çıkmaya çalışan kadın fren yerine gaza basınca direksiyon hakimiyetini kaybetti., GÜÇLÜKLE DURABİLDİ, Kontrolden çıkan otomobil kaldırıma çıkarak o esnada kaldırımda bastonuyla yürüyen Sebahattin Özcan'a çarptı. Çarpma sonucu duvara çarpan adam takla atarak yere savruldu. Otomobil ise doğal gaz kutusuna ve havalandırma borularına çarparak durabildi., Dehşet anları ise güvenlik kameralarına saniye saniye yansıdı. Görüntülerde, kadın sürücü otomobiline binerek yola çıkmak istiyor. Ardından sürücünün kontrolünden çıkan araç kaldırıma çıkıyor. Araç kaldırımda bastonuyla yürüyen yaşlı adama çarpıyor. Duvara çarpan adam takla atarak yere savruluyor., , Kazanın ardından ihbar üzerine olay yerine sağlık ve polis ekibi sevk edildi. Kısa sürede olay yerine gelen sağlık ekipleri, direksiyon başında şoke olan sürücü Erie'yi yaptıkları ilk müdahalenin ardından ambulansla Şişli Hamidiye Etfal Eğitim ve Araştırma Hastanesi'ne kaldırılarak tedavi altına aldı., Yaralı halde yerde oturan Özcan'da sağlık ekiplerinin müdahalesinin ardından başka bir ambulansla hastaneye kaldırıldı. Erie ve Özcan'ın durumlarının iyi olduğu ve hayati tehlikelerinin olmadığı öğrenildi., Olayla ilgili konuşan bina sakini Nuran Tüzün, "Garaj önündeki aracın içerisinde çok sayıda siyahi çıktı. Öğrenci yurduna eşya taşıyorlardı, bende burada oturuyordum. İçerisinde direksiyonda kadın varmış. Konuşurken 'güm' diye bir ses duydum, bir baktım bizim apartmana vurmuş. Adamın birisi de yoldan geçiyormuş ona da vurmuş. Siyahi kadın da yaralıydı, adam da yaralıydı sırtüstü yere düşmüştü. Camı açtım ne oluyor diye bir baktım, apartman uçuyor zannettim. Ondan sonra polisler ve ambulans geldi, götürdüler" dedi., Olayın ardından polis ekipleri de kazayla ilgili inceleme yaparak tutanak tuttu. Aracın bina girişindeki doğalgaz kutusuna ve havalandırma borularına çarpması nedeniyle vatandaşlar büyük panik yaşadı. Olay yerine gelen doğal gaz ekipleri de gazı gezerek önlem aldı. Yapılan çalışmaların ardından otomobil çekici yardımıyla emniyet otoparkına götürüldü., , </t>
+  </si>
+  <si>
+    <t>Bursa 28°, İlçeler, Kategoriler, Sosyal Medya, Bursa'da kimliği belirsiz bir kişi, gözüne kestirdiği kadın sürücünün aracını saniyeler içerisinde çalarak kayıplara karıştı. Kadın sürücünün araçtan inmesini fırsat bilen şüpheli, araca binip kaçarken, peşinden koşan sürücüyü de metrelerce sürükledi._x000D_
+, İLGİLİ VİDEO, Olay, merkez Osmangazi ilçesi Sırameşeler Mahallesi'nde meydana geldi. Edinilen bilgiye göre, 45 HC 3642 plakalı hafif ticari aracın sürücüsü Aynur Artık (50), bir yakınlarının nişan cemiyetine katılmak üzere düğün salonunun önüne geldi., Artık, burada aracından inerek arkada bulunan araçtaki kızıyla sohbet etmeye başladı., , Bu sırada yaklaşık 20 metre uzaktan durumu seyreden kimliği belirsiz bir şüpheli, Artık'ın park halindeki aracına gelerek direksiyon koltuğuna oturdu ve aracı çalıştırdı. , Aracının hareket ettiğini fark eden Aynur Artık, aracının kapısına tutundu ancak, şüpheli durmayarak Aynur Artık'ı metrelerce sürükledi., Fenalaşan Aynur Artık, bölgede bulunan vatandaşlar tarafından sakinleştirildi., , İhbar üzerine olay yerine gelen polis ekipleri, güvenlik kameralarını takibe alarak şüpheliyi yakalamak için soruşturma başlattı., , Öte yandan yaşanan panik anları, güvenlik kameraları tarafından an be an görüntülendi. Yaşanan olayın ardından konuşan Aynur Artık, 'Tahmin ediyorum ki arabada 4 kadın olmamızdan kaynaklı bizleri takip ederek aracı gözüne kestirdi. Araçtan inmemizle birlikte arabaya biniyor ve aracı çalıştırıp kaçıyor. Peşinden koşup, kapıyı tuttum ancak durmadı ve beni sürükledi. Aracımızın bir an önce bulunmasını istiyoruz. Aracımızla tehlikeli işler yapılıp başka bir suça karışmasından endişe ediyoruz.' diye konuştu., , , , , Diğer Bursa Haberleri - Bölge Haberleri için tıklayın, ABD ve Çin'den sonra Hollanda: Ülkeler BTC'yi sıkıştırıyor, Doğu Anadolu'dan yapılan ihracat 1 milyar doları aştı, TÜBİTAK Başkanı Prof. Dr. Mandal'dan müsilaj açıklaması , Kapıdağ'ın bir tarafı müsilajdan kahverengi, diğer tarafı pırıl pırıl , G7 ülkeleri 1 milyar Covid-19 aşısı bağışlayacak , Almanya'da Türk genci 2 yıldır kayıp, NASA dev roketleri birleştiriyor: Ay'a ilk kadını taşıyacak , Bursa Mudanya'da bir sorun daha çözüme kavuşuyor , Bursa Yıldırım Medya Akademisi, ilk mezunlarını verdi, Bursa'da kestane ağaçlarını dolu vurdu, Öne Çıkan Galeriler, Öne Çıkan Videolar, En Çok Okunanlar</t>
+  </si>
+  <si>
+    <t>Bursa 28°, İlçeler, Kategoriler, Sosyal Medya, Bursa'da kaza yapan kadın sürücü, yaptığı kazanın ardından kazaya karışan otomobilleri ve kendini görüntüleyen gazeteciye saldırdı., İLGİLİ VİDEO, Kaza, saat 00.00 sıralarında merkez Osmangazi ilçesi Bursa-İzmir yolu Merinos batçığında meydana geldi. , , Edinilen bilgiye göre, İzmir yolu üzerinde seyir halinde olan Ö.Y. yönetimindeki 16 LKM 16 plakalı kadın sürücü, direksiyon hakimiyetini kaybetmesiyle ani fren yaptı. , , İddiaya göre, ani fren yapmasıyla M.A.,yönetimindeki 16 AHS 962 ve H.L.S., yönetimindeki 16 AFF 886 plakalı otomobil sürücüleri 16 LKM 16 plakalı araca çarptı._x000D_
+Vatandaşların ihbarı üzerine olay yerine polis ekipleri sevk edildi. , , Herhangi bir can kaybı yaşamazken, olay yerine gelen ekipler geniş güvenlik önlemi aldı. , , 16 LKM 16 plakalı araç sürücüsü Ö.Y. ise kendisini görüntüleyen gazeteciye "Çekme sende, ne çekiyorsun" diyerek saldırmaya kalkıştı., Kazada nedeniyle bir süre trafiğe kapanan yol, araçların çekilmesiyle tekrar ulaşıma açıldı., Diğer Bursa Haberleri - Bölge Haberleri için tıklayın, ABD ve Çin'den sonra Hollanda: Ülkeler BTC'yi sıkıştırıyor, Doğu Anadolu'dan yapılan ihracat 1 milyar doları aştı, TÜBİTAK Başkanı Prof. Dr. Mandal'dan müsilaj açıklaması , Kapıdağ'ın bir tarafı müsilajdan kahverengi, diğer tarafı pırıl pırıl , G7 ülkeleri 1 milyar Covid-19 aşısı bağışlayacak , Almanya'da Türk genci 2 yıldır kayıp, NASA dev roketleri birleştiriyor: Ay'a ilk kadını taşıyacak , Bursa Mudanya'da bir sorun daha çözüme kavuşuyor , Bursa Yıldırım Medya Akademisi, ilk mezunlarını verdi, Bursa'da kestane ağaçlarını dolu vurdu, Öne Çıkan Galeriler, Öne Çıkan Videolar, En Çok Okunanlar</t>
+  </si>
+  <si>
+    <t>8 Mart Dünya Kadınlar Gününde 'kim demiş kadınlar araba süremez diye?' sloganıyla yola çıkan bir otomobil satış bayisi, trafikte cinsiyet ayrımcılığına dikkat çekmek ve kadınların araba kullanamayacağı yönündeki ön yargıyı kırmak amacıyla Türkiye'nin en genç kadın ralli şampiyonu Burcu Burkut Erenkul ile video hazırladı. Videoda bir sosyal medya fenomenini canlandıran Erenkul, acemi şoför gibi davranarak satış temsilcilerine ilginç sorular sordu. , Daha sonra test sürüşüne çıkan Erenkul ve şakadan habersiz satış temsilcilerinin yaşadığı o anlara kameraya kaydedildi. Test sürüşü sırasında yeteneği ile adeta şov yapan Erenkul, satış temsilcilerini hayrete düşürdü. O video ise sosyal medyada binlerce yorum ve beğeni aldı. , O anları DHA'ya anlatan Erenkul, videonun bu kadar büyük bir ilgi göreceğini tahmin etmediğini söyledi. Erenkul, "Trafikte ve her yerde kadınlara karşı bir ön yargı var. Ben de zaman zaman bunları yaşıyorum., Trafikte bana da çok korna çalıyorlar. Bu kimliğinizle, kim olduğunuzla alakalı değil, sırf cinsiyetinizden dolayı bazı sıkıntılar yaşıyorsunuz. Biz de buraya dikkat çekmek istedik. Ne yazık ki kadınların otomobille ilgisinin olmadığı insanların kafasına tabu gibi yerleşmiş" dedi., Satış temsilcilerinin korku dolu anlar yaşadığını ifade eden Burcu Burkut Erenkul, "Hem elektrikli hem hızlı hem de sportif bir arabaydı. Bir de saçma sorular soran birini canlandırdım orada. Fren disklerine bunlar tabak mı diye sorular sorunca endişelendiler tabii. Daha sonra test sürüşüne çıktık. Ben o anda ani gaz, fren yaptım ve rotadan çıktım. Bir ara yanımdaki satış sorumlusu 'ortadakine basın' diyordu. Yani fren derse anlamayacağımı düşünüyordu. O esnada ben otomobili döndürmeye başladım. Otomobili çarpma endişesiyle biraz akıllarını aldık diyelim. Ben sadece çok korkarlarsa direksiyonuma müdahale ederlerse diye korktum" diye konuştu., 7 yaşından beri bu sporun içinde olan Erkul, profesyonel bir pilot olmasına rağmen sadece kadın olduğu için ön yargılara maruz kaldığını belirtti., Erenkul, "Bu sporun içindeyken bir yarış otomobilinin içindeyken kaskım, tulumum olmasına rağmen insanlar tepki gösterebiliyor. Hatta küçük çocuklar kaskla yarıştan çıktığım anda koşarak gelip, 'abi tekrar yanlar mısın, bir de buradan yanla' dedikten sonra kaskımı çıkardığımda beni görünce şaşırarak 'kadınmış' diyerek hiç konuşmadan arkalarını dönüp geri giderlerdi. Bu beni çok üzüyordu açıkçası. Sosyal medyanın gücüyle o çocuklara da ulaştığımızı düşünüyorum. Bir kadının gerçekten iyi otomobil kullanabileceğini ve kadın isterse her şeyi başarabilir" ifadelerini kullandı., İstanbul'un en fazla tercih edilen yeşil alanlarından Belgrad Ormanı'nda bugün 'kısıtlamasız cumartesi' yoğunluğu vardı. Kimi piknik, kimi yürüyüş yaptı. Araç kuyrukları ise uzadıkça uzadı. İstanbullular, doğanın ve yeşilin tadını Belgrad Ormanı'nda çıkardı. Mücahit Topçu ve Caner Emre Kınacı'nın haberi.</t>
+  </si>
+  <si>
+    <t>Trafikte kadın sürücülere karşı önyargılı bakış açısının günümüzdeki durumunu ve kadın sürücülerin otomobil meraklarını Hakan Çelik'le Hafta Sonu programında değerlendiren sosyal medya fenomenleri Doğan Kabak ve Eren Tekin, önemli değerlendirmelerde bulundu. Kadın sürücülerin trafikte yaşadığı taciz ve zorluklar dile getirilirken, otomotiv sektörüne bakış açıları da yorumlandı., PROGRAMIN TAMAMINI İZLEMEK İÇİN TIKLAYIN</t>
+  </si>
+  <si>
+    <t>https://www.cumhuriyet.com.tr/haber/maske-takmayan-yolcu-kendisini-uyaranlara-saldirdi-1743528</t>
+  </si>
+  <si>
+    <t>İzmit Gündoğdu Boğazova Caddesi’nde meydana gelen halk otobüsüne binen bir kadın, maske takmadı. Sürücü, adı öğrenilemeyen kadını maske takması için uyarak, "Maskesiz yolcu almıyorum" dedi., Küçük çocuğu ile birlikte koltuğa oturan kadın ise, "Kapa çeneni nasıl almıyorsun" yanıtı verdi. Bunun üzerine başka bir kadın yolcu, "Terbiyesiz" diyerek, kadına maske takmaması durumunda şikayetçi olacağını bildirdi.Kadın ise elindeki maskeyi kadına doğru sallayarak, "Bak takmıyorum" dedi. Sürücünün, suçlu olduğunu söylediği kadın, "Kimi çağırırsan çağır" diye konuştu.Kadın daha sonra ayağa kalkarak, ön koltukta oturan kadınlara küfredip, saldırdı., Bu sırada küçük bir çocuk, "Yeter" diye bağırırken, otobüs sürücüsü kadınları ayırmaya çalıştı. Şikayet üzerine gelen polis, kadın ile sürücü ve yolcuların ifadelerini aldı.Maske takmayan kadına, İl Hıfzıssıhha Kurulu kararlarına uymaması nedeniyle ceza kesileceği belirtildi. </t>
+  </si>
+  <si>
+    <t>https://www.denizli20haber.com/haber-fren-yerine-gaza-basan-kadin-surucu-3-yayayi-ezdi-37263.html</t>
+  </si>
+  <si>
+    <t>Denizli’de 'U' dönüşü yapmak isterken fren yerine gaza basan kadın sürücü, kaldırıma çıkıp trafik ışığını devirdikten sonra köpekleriyle birlikte kaldırımda yürüyen yayaları ezdi. 5 yayadan 3'üne çarpan otomobilin bir kişiyi ezip ağır yaralandığı kazada güvenlik kameralarına anbean yansıdı.,  , ,  , Kaza, öğle saatlerinde Merkezefendi ilçesi 29 Ekim Bulvarı'nda meydana geldi. Edinilen bilgilere göre; 20 BK 259 plakalı otomobili ile seyir halinde olan Emine Beler, bulvardan 'U' dönüşü yapmak isterken bir anda fren yerine gaza bastı. Kadın sürücünün kontrolünü kaybettiği otomobil, kaldırıma çıkarak önce trafik ışığını devirdi. Ardından kaldırımda kontrolsüz bir şekilde ilerlemeye devam eden otomobil, köpeklerini gezintiye çıkaran 3 genç ile karşı yönden delen iki kişiye daha çarptı.,  , , Otomobilin çarptığı Meltem Çoğaşlıoğlu (21) ile Furkan Sevinç (18) kaldırma savruldu. Ön kısmı hurdaya dönen aracın altına aldığı Eyüp Batuhan (20) ise ağır yaralandı. Çevredeki vatandaşların yardımı ile otomobilin altından çıkarılan Batuhan, sağlık ekipleri tarafından Denizli Devlet Hastanesine kaldırıldı. Kazada hafif şekilde yaralandıktan sonra ayakta tedavi edilen diğer gençlerin ise sağlık durumlarının iyi olduğu öğrenildi.,  , _x000D_
+ , Güvenlik kameralarına anbean yansıyan korku dolu anlar tüyleri ürpertti. Kontrolden çıkan otomobilin trafik ışığını devirdikten sonra yayalara çarpması, iki gencin yola savrulması ile paniğe kapılan yaya ve köpeğin sağa sola kaçışması görüntülerde yer aldı.,  , Yorumunuz
+                                                    başarıyla alındı, inceleme ardından en kısa sürede yayına
+                                                    alınacaktır.</t>
+  </si>
+  <si>
+    <t>Tavas İlçe Başkanı Erdoğan Şama hayatını..., Denizlipor'da Genel Kurul ertelendi, Lokman Kuzdere hayatını kaybetti, Denizli'de simide zam geldi!, Doğalgaza Haziran ayı zammı, Kaza, Fethiye – Kayaköy yolu üzerinde meydan geldi. Edinilen bilgilere göre Fatma G.'nin kullandığı 48 T 3222 plakalı ticari araç, karşı yönden gelen Derya B. yönetimindeki 48 JR 556 plakalı otomobille kafa kafaya çarpıştı.Kazada sürücüler ile Fatma G.’nin kullandığı ticari takside yolcu olarak bulunan, Emma Louıse B., Devereaux Ellen J., Necla K. ile diğer otomobilde bulunan Remzi T. yaralandı. Kazayı görenlerin 112 Acil Çağrı Merkezi’nden yardım istemesi üzerine olay yerine Jandarma ve çok sayıda sağlık ekipleri sevk edildi. Yaralılar, kaza yerinde 112 Acil Servis ekiplerince yapılan ilk müdahalenin ardından Fethiyedeki Hastanelere kaldırıldı. Yaralıların hayati tehlikesinin bulunmadığı öğrenilirken, kaza ile ilgili soruşturma devam ediyor., Kaynak:İHA, Facebook Paylaş, Twitter Paylaş, Editörün Diğer Yazıları, Mail: email protected, Başka haber bulunmuyor!, , DENİZLİ VATAN MEDYA 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Aydın'ın Kuyucak ilçesinde, bir köpeği iple otomobilin arkasına bağlayarak çektiği iddiasıyla 1033 TL ceza kesilen kadın sürücü A.S., hayvana eziyet edecek hiçbir şey yapmadığını öne sürdü.    , Aydın- Denizli karayolu kırsal Pamukören Mahallesi yakınlarında, geçen pazar günü akşam saatlerinde seyir halinde olan 20 B 1177 plakalı otomobile bir köpeğin, iple bağlanarak çekildiği görüldü. Yoldan geçen bir sürücü tarafından kaydedilen görüntüler, sosyal medyada yer aldı. Plaka üzerinden sürücüyü ve otomobili tespit eden polis, kadın sürücü A.S.'nin adresini belirleyerek kendisine ulaştı. A.S. hakkında 5199 Sayılı Kanunun 14. Maddesi (a) bendi uyarınca, bin 33 TL para cezası kesti. Köpek ise Aydın Büyükşehir Belediyesi Zabıta görevlileri tarafından teslim alınarak barınağa bırakıldı.,  , ,  , 'OTOMOBİLİN BAGAJINA KOYMAK İSTEDİK AMA GİRMEDİ', Köpeğe eziyet etmediğini belirten A.S., yazılı açıklama yaparak, "10 Aralık tarihinde ailecek 10 gün izne çıktık. Eve döndüğümüzde zayıf ve bitkin düşmüş ölmek üzereyken bir köpekle karşılaştık. Bu köpeği kurtarmak için beslemeye başladık. Köpeği besledikçe bize alıştı. Evin önünden gelip geçeni rahatsız etmeye başladı. Komşular da köpeği bağlamamız konusunda uyardı. Köpeği bağladık ama bu defa dışarıdan gelen köpekler, köpeğe zarar vermeye başladı. Bazen de ipini kopararak insanlara saldırmaya başladı. Ona alıştık ve o güne kadar baktık. Çocuklar da ismini 'Kuru' olarak koydu. Saldırganlığı nedeniyle büyükşehir belediye ekiplerini arayarak, barınağa götürmelerini istedik. Götüreceğiz demelerine rağmen 2 hafta bekledik, götürmediler. Bizde hayvanı sahiplendirmek istedik. Ama dişi olduğu için kimse almak istemedi. Saldırganlığı nedeniyle yoldan geçenler, köpeği öldüreceğini söyledi. Çok sevdiğimiz köpeği korumak amaçlı, ilerideki bir mezbahanın oraya götürerek bakmak istedik. Otomobilin bagajına koymak istedik ama girmedi. Biz de çok zayıf bir iple köpeği otomobilin arkasına bağladım. Herhangi bir zorlama olmadı. Zorlasak ip kopacak şekildeydi. Otomobili birinci viteste ağır ağır sürüyordum. Köpeği götüreceğim mesafe ise 350 metre ancak uzaklıktaydı. Oraya bırakarak ekmeğini de verdik. Bizi çekenler ise evden çıktığımız bile gördüler. Aradan bir süre sonra da köpek eve geriye döndü. Eve gelen veterinerlerin kontrolünde herhangi bir eziyete rastlanmadı. Hayvanlara eziyet edecek hiçbir şey yapmadım" dedi.,  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adana’nın Seyhan ilçesi Ziyapaşa Mahallesi Kasım Gülek Bulvarı’nda alkollü olduğu ileri sürülen Mustafa D.’ye (49), yolun karşısına geçerken otomobil çarptı., Çevredeki bir esnafın ihbarı üzerine kaza yerine sevk edilen sağlık ekibinin ilk müdahalesinin ardından Mustafa D., Adana Şehir Eğitim ve Araştırma Hastanesi’ne kaldırıldı., Tedaviye alınan Mustafa D.’nin 3.7 promil alkollü olduğu belirlendi. Mustafa D., doktorların tüm çabasına karşın kurtarılamadı., Polis ekipleri, kaçan sürücünün yakalanması için çalışma başlattı., Ekipler, kaza sırasında aracın aynasının kırıldığını belirledi. Kırık ayna parçasından yola çıkan ekipler, bölgedeki güvenlik kamerası görüntülerini incelemeye aldı., Görüntülerden 01 AFN 937 plakalı otomobilin aynasının olmadığını tespit etti., , Ekipler, aracı merkez Yüreğir ilçesi Atakent Mahallesi’ndeki bir sitenin otoparkında park halindeyken buldu. Aracın sürücüsü Pınar A., polis ekiplerince gözaltına alındı., Emniyete getirilerek sorguya alınan Pınar A.’nın, ifadesinde “Aracımla yasal hız sınırında caddede seyir halindeydim. Aracın sol kısmından ‘pat’ diye bir ses geldi. Sol tarafıma baktığımda bir şey göremedim. Ancak dikiz aynamın yerinde olmadığını fark ettim. Bunun üzerine yol kenarındaki yön levhası ya da tabelaya çarptığımı düşündüm ve durmayıp yola devam ettim. Bir canlıya çarptığımı düşünmedim. Böyle bir şey olsaydı kesinlikle durup, yardım ederdim.” dediği öğrenildi., , Ayrıca Pınar A.’nın, “Bir insana çarptığımı, sabah polis evime geldiğinde öğrendim. Eğer olay anında bunu fark etmiş olsaydım, mutlaka durup yardım ederdim.” dediği bilgisine de ulaşıldı., Emniyetteki işlemlerinin ardından ‘taksirle ölüme sebebiyet vermek’ suçlamasıyla adliyeye sevk edilen Pınar A., çıkarıldığı mahkemece tutuklandı., , Öte yandan, kazaya tanıklık eden ve bölgede bir tekel büfesi işleten 34 yaşındaki Ali Elçin ise “Şahsı tanıyoruz, sürekli alkol alan biri. Refüjde beklerken dengesini kaybedip, yola düştü. Bu sırada da geçen otomobilin dikiz aynası çarptı. Tekrar refüje düştü. Sürücü bir insana çarptığını fark etmeyip yoluna devam etti. Biz de vatandaşa yardım edip, ambulans çağırdık. Hastaneye kaldırıldı ancak ölmüş.” dedi., </t>
+  </si>
+  <si>
+    <t>https://www.ensonhaber.com/ic-haber/gaz-ile-freni-karistiran-kadin-surucu</t>
+  </si>
+  <si>
+    <t>İstanbul Büyükçekmece Çarmıklı Caddesi'nde Ayfer Ü. yönetimindeki otomobil, bir anda kontrolden çıkarak cadde üzerindeki beyaz eşya dükkanına daldı., Kazada ölen ya da yaralanan olmazken, büyük panik yaşandı., Gaz ile freni karıştıran sürücü beyaz eşya dükkanına daldı VİDEO, , Aracından çıkan sürücünün, fren ile gaz pedalını karıştırarak panik yaptığı öğrenildi. Yaşanan bu ilginç kaza, güvenlik kameralarına da saniye saniye yansıdı. Görüntülerde otomobil, bir anda kaldırımı aşarak merdivenlerden iniyor. Araç daha sonra beyaz eşya dükkanına çarparak duruyor.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saat 14.00 sıralarında, Gültepe Mahallesi Raylı Sokak'ta meydana gelen kazada  Safiye Kervan Kıran,  kullandığı 60 TR 710 plakalı otomobille sokağa gireceği sırada, önce aynı yönde ilerleyen Canpolat Işık yönetimindeki bisiklete ardından yaya Tolgahan Daşdelen’e çarptı. Kazada Canpolat ve Daşdelen yaralandı., Çevredekilerin ihbarı üzerine kaza yerine sağlık ve polis ekipleri sevk edildi. Yaralılar, ilk müdahalenin ardından ambulansla Numune Hastanesi'ne kaldırıldı. Tedaviye alınan yaralıların sağlık durumunun iyi olduğu belirtildi., Kazanın şokunu yaşayan otomobil sürücüsü Safiye Kervan Kıran ise bölgeye gelen yakınları tarafından sakinleştirildi.,  , ,      </t>
+  </si>
+  <si>
+    <t>, Can kaybının yaşanmadı maddi hasarlı trafik kazası bugün Adana'da yaşandı., 27 yaşındak Pınar Harman isimli kadının sürücüsü olduğu otomobil yolda ilerken, hızlı girdiği virajda kontrolünü kaybetti. Yolda savrulan araç yol kenarında bulunan ağaca çarpıp kanala girdi., , , , Kanala sarkıtılan halat ile çıkarılan genç kadın şoka girdi. Olay yerinde hazır bulunan 112 sağlık personeli tarafından yapılan ilk müdahaleden sonra talihsiz kadın hastaneye kaldırıldı., Kaza ile ilgili olarak inceleme başlatıldı., 
+_x000D_
+ (adsbygoogle = window.adsbygoogle || ).push({});_x000D_
+, info@gursesgazetesi.com, Bağımsız Sondakika Güncel Haberler!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+_x000D_
+(adsbygoogle = window.adsbygoogle || ).push({});_x000D_
+, HABERDENİZLİ.COM, Acıpayam'da meydana gelen trafik kazasında bir kişi hayatını kaybetti. Kaza Acıpayam'a bağlı Akşar Mahallesinde meydana geldi., Kaza Bugün Sabah Sularında Akşar Mahallesi Çıkışı Kelekçi Gölcük Yolu Üzeri Yaylapınar Yolu Girişinde Meydana Geldi. P.Abay Adlı Bayan Motosiklet Sürücüsü Yaylapınar istikametinden Kelekçi-Gölcük Yoluna Çıktığında Gölcük İstikametinden Gelen R.Eriş İradesindeki Otomobille Çarpıştı. Kazada Motosiklet Sürücüsü P.Abay Ağır Şekilde Yaralandı, Çevredeki Vatandaşların Kazayı Farketmesinin Ardından 112 Acil Yardıma Haber Verdi. Olay Yerine Gelen 112 Ambulans Ekipleri Kazada Ağır Yaralanan P.Abay’ı Acıpayam Devlet Hastanesine Kaldırdı. Hastanede Tüm Müdahaleye Rağmen Kurtarılamayan P.Abay Hayatını Kaybetti., Kaynak: Acıpayamgazetesi, Yorumunuz başarılı bir şekilde gönderilmiştir. Editörlerimizin onayının ardından yayınlanacaktır!</t>
+  </si>
+  <si>
+    <t>https://www.haberler.com/acemi-kadin-surucu-viraji-alamayinca-saglik-13622109-haberi/</t>
+  </si>
+  <si>
+    <t>Acemi kadın sürücü, virajı alamayınca sağlık ocağına girdi, Mersin'de arkadaşıyla birlikte araba sürmeyi öğrenen kadın bir sürücü, virajı dönemeyince sağlık ocağına girdi, , Şans eseri sağlık ocağının aile planlama ve emzirme odasında kimsenin olmaması can kaybını önlerken, araba sürücüsü ile arkadaşı tedbir amacıyla hastaneye kaldırıldı, MERSİN - Mersin'de arkadaşıyla birlikte araba sürmeyi öğrenen kadın bir sürücü, virajı dönemeyince sağlık ocağına girdi. Şans eseri sağlık ocağının aile planlama ve emzirme odasında kimsenin olmaması can kaybını önlerken, hafif yaralanan araba sürücüsü ile arkadaşı tedbir amacıyla hastaneye kaldırıldı. , Edinilen bilgiye göre olay, Mersin'in merkez Toroslar ilçesine bağlı Hüseyin Okan Merzeci Mahallesinde meydana geldi. Zeynep Ç. yönetimindeki 01 BGC 02 plakalı araç, Hüseyin Okan Merzeci Mahallesi Aile Sağlığı Merkezi'nin zemin katına girdi. Olayın ardından çevredekilerin ihbarı üzerine bölgeye çok sayıda ambulans ve polis ekibi sevk edildi. Şans eseri kaza sırasında sağlık ocağının aile planlama ve emzirme odasında kimsenin olmamasından dolayı sağlık çalışanlarına bir şey olmazken, sürücü ile yanındaki arkadaşı hafif şekilde yaralandı. Korku dolu anların yaşandığı olayın ardından araç sağlık ocağının içinden çekici yardımıyla çıkarıldı., Olayda, kadın sürücünün ehliyetinin olmadığı, arkadaşının araba sürmeyi öğrettiği öğrenildi., Öte yandan aynı sağlık ocağına daha öncede birkaç kez araba girdiği ve bundan dolayı camlı bölgeye demir korkuluk yaptırıldığı da öğrenildi., "Kıl payı ölümden kurtulduk", Sağlık çalışanları şans eseri olayda kendilerine birşey olmadığını belirterek, "Kıl payı kurtulduk ölümden" dediler., Kaynak: İhlas Haber Ajansı /  Koray Ünlü, Haberler.com'un size anlık bildirim göndermesine izin veriyor musunuz?</t>
+  </si>
+  <si>
+    <t>https://www.haberler.com/ankara-da-kadin-surucu-ile-kamyon-soforu-tekme-13597720-haberi/</t>
+  </si>
+  <si>
+    <t>Ankara'nın Sincan ilçesinde yol verme tartışması nedeniyle kadın sürücü ile kamyon şoförü tekme tokat kavga etti. Kadın sürücünün ağza alınmayacak küfürler ederek kamyoncu gence saldırdığı anlar cep telefonu kamerasına anbean yansıdı., Olay, Sincan ilçesi Fatih Caddesi üzerinde meydana geldi. İddialara göre, yolda bir kamyoncu ile otomobil sürücüsü kadın arasında yol verme konusu yüzünden kavga çıktı. Trafikte araçlarından inen ikili yaka paça birbirine girdi. Kadın sürücü ağza alınmayacak küfürler ederek kamyoncu gence saldırdı. , , Genç adam yakayı kurtarmaya çalışsa da başarılı olamadı. Kadın ise her defasında adamın üzerine küfür ederek yürüdü ve saldırdı. Çevredeki vatandaşlar ise genç adama kaçması yönünde uyarılarda bulundu. , Otomobil sürücüsü kadın ise şaşkın bakışlar arasında arabasına binip uzaklaştı. Geriye ise ağza alınmayacak küfürlü anlar kaldı. O anlar cep telefonu kamerasına saniye saniye yansıdı., Kaynak: İhlas Haber Ajansı, Haberler.com'un size anlık bildirim göndermesine izin veriyor musunuz?</t>
+  </si>
+  <si>
+    <t>https://www.haberler.com/hurdaya-donen-otomobilden-cikartilan-kadin-surucu-13959821-haberi/</t>
+  </si>
+  <si>
+    <t>, ESKİŞEHİR'de kullandığı otomobilin kontrolünü kaybeden Tuğçe Duysak Özer (30), takla atarak duran araçtan ağır yaralı olarak çıkartıldı. Kaldırıldığı hastanede genç kadının hayatını kaybettiği öğrenildi. , , Kaza, dün Eskişehir-Ankara karayolu Böğürtlen Mahallesi mevkiinde meydana geldi. Tuğçe Duysak Özer, kullandığı 06 BA 7085 plakalı otomobilin kontrolünü kaybetti. Takla atarak duran ve hurdaya dönen araçtan ağır yaralı olarak çıkarılarak Sivrihisar Devlet Hastanesi'ne kaldırıldı. Özer'in, doktorların tüm müdahalesine rağmen hayatını kaybettiği öğrenilirken polis ekipleri kazayla ilgili soruşturma başlattı., Kaynak: Demirören Haber Ajansı, Haberler.com'un size anlık bildirim göndermesine izin veriyor musunuz?</t>
+  </si>
+  <si>
+    <t>https://www.haberler.com/kadina-uzanan-el-bu-kez-karsilik-buldu-13531975-haberi/</t>
+  </si>
+  <si>
+    <t>İstanbul Sarıyer'de trafikte yol verme tartışmasında bir kadına tokat atan adam sert kayaya çarptı. Eski tekvandocu olan kadın, adamı fena şekilde dövdü. Vatandaşların araya girmesiyle kavganın büyümesi önlendi. Olay anı bir vatandaşın cep telefonuna böyle yansıdı., Olay, geçtiğimiz günlerde İstanbul'da meydana geldi. Bir ara sokakta yol tartışması yüzünden bir kadın ve bir erkek sürücü tartışmaya başladı. İddiaya göre, kendine yol vermediğini için sinirlenen erkek sürücü aracından inip, kadın sürücüye sinirlenerek tokat attı. , Eski tekvandocu olan Fatma Z. isimli kadın ise tokat karşısında önce kendini savundu daha sonra ise yaşlı adamın burnundan tutarak etkisiz hale getirdi. Bu sırada el freni çekilmeyen adamın kullandığı araç ise hareket etti. Aracın hareket etmesi ile panikleyen yaşlı adam, yaklaşık 2 metre giden aracına hızla binerek el frenini çekti. Kadın ise yaşlı adamın arkasından yumrukları vurmaya devam etti. Bu sırada ikilinin arasına bir genç girerek ayırdı. Yaşlı adamın aracına binerek olay yerinden uzaklaşmasının ardından kadın da aracına binerek olay yerinden uzaklaştı. , Olay anları ise bir vatandaşın cep telefonuna saniye saniye yansıdı., Kaynak: İhlas Haber Ajansı, Haberler.com'un size anlık bildirim göndermesine izin veriyor musunuz?</t>
+  </si>
+  <si>
+    <t>https://www.haberler.com/son-dakika-haberleri-tir-in-altinda-kalan-kadin-surucu-hayatini-13960016-haberi/</t>
+  </si>
+  <si>
+    <t>Sinem Kuran (45) idaresindeki 35 GB 4539 plakalı otomobil, bugün sabah saatlerinde, Akçay Caddesi 6'ncı Sanayi Kavşağı'nda Ali K. (65) yönetimindeki 34 DAE 978 plakalı TIR'a yandan çarptı. , Maddi hasarlı kaza sonrası otomobilinden inen Kuran, o sırada hareket eden tırın altında kalarak can verdi. Çevredekilerin ihbarı üzerine kaza yerine, polis ve sağlık ekipleri sevk edildi. , , Tırın altından çıkartılan Kuran'ın olay yerinde hayatını kaybettiği belirlenirken tır şoförü Ali K. gözaltına alındı. Kazayla ilgili polis ekipleri soruşturma başlattı., Kaynak: Demirören Haber Ajansı, Haberler.com'un size anlık bildirim göndermesine izin veriyor musunuz?</t>
+  </si>
+  <si>
+    <t>https://www.haberler.com/ukrayna-da-tramvay-yoluna-park-eden-kadin-surucu-12540834-haberi/</t>
+  </si>
+  <si>
+    <t>Ukrayna'da tramvay yoluna park eden kadın sürücü, trafiği 2 saat boyunca felç etti, Ukrayna, (DHA) ? Ukrayna'da aracını tramvay trafiğini engelleyecek şekilde park kadın sürücü, trafiği 2 saat boyunca felç etti. Rayların kenarına park edilen aracı, tramvaydaki yolcular ve çevredekiler ileriye ve geriye iterek tramvayların önünü açtı., , Odessa şehrinde tramvayların 3 şeritten geçtiği işlek bir bulvarın ortasına park edilen araç, tramvayların geçişini engelledi. Gelen ve giden tramvayların geçişini sağlama işi ise çevredeki vatandaşlara ve tramvaydaki yolculara düştü., Güvenlik kamerasınca kaydedilen görüntülerde, kadın sürücünün, aracını tramvayların geçiş güzergahına yakın bir noktaya park ettiği ve aracından inerek uzaklaştığı görüldü. Daha sonra park halindeki aracın bulunduğu raylardan tramvayın geçemediği, çevredekilerin ve tramvay yolcularının park halindeki aracı ileriye ve geriye iterek geçmeye çalışan tramvaylara yol açtığı görüldü. Vatandaşlar ve yolcular, 2 saat boyunca 7 kez aracı ileriye ve geriye itmek zorunda kaldı. 2 saatin sonunda kadın sürücü, çocuğuyla birlikte aracına binerek uzaklaştı., Görüntüler sosyal medyada çok sayıda yorum aldı. Bazı kullanıcılar, kadının sorumsuz olduğunu belirtirken, bazıları ise vatandaş ve yolcuların çabasını tebrik etti., Kaynak: Demirören Haber Ajansı, Haberler.com'un size anlık bildirim göndermesine izin veriyor musunuz?</t>
+  </si>
+  <si>
+    <t>https://www.haberturk.com/antalya-haberleri/69785968-carptigi-motosikletli-olen-kadin-surucu-gozyaslarina-boguldusinir-krizi-geciren-surucu</t>
+  </si>
+  <si>
+    <t>Antalya’nın Gazipaşa ilçesinde otomobiliyle çarptığı motosiklet sürücüsüne kalp masajı yapılırken sinir krizi geçiren kadın, "Benim de çocuğum var. Onun da çocuğu vardır. O da evine ekmek götürüyordur. Ben bir daha çocuğumu göremeyecek miyim” diyerek gözyaşlarına boğuldu. Motosiklet sürücüsü müdahaleye rağmen hayatını kaybetti.  Kaza, Milli Egemenlik Bulvarı Gazipaşa Meteoroloji İstasyonu önünde saat 10.00 sıralarında meydana geldi.Edinilen bilgiye göre, AlanyaGazipaşa istikametinde seyir halinde olan Dilek Kurt (21) yönetimindeki 06 GC 3575 plakalı otomobil, tali yoldan çıkan Durmuş Demiral (57) yönetimindeki 07 UM 805 plakalı motosiklete çarptı. Kazada motosiklet sürücüsü metrelerce sürüklendi. Çarpmanın etkisiyle vücudunun çeşitli yerlerinden ağır yaralanan motosiklet sürücüsü Demiral’a ilk müdahaleyi, bir yakınının haber vermesi üzerine olay yerine giden Gazipaşa Devlet Hastanesi Başhekimi Hasan Sözen yaptı. Demiral yapılan kalp masajına cevap vermedi.  Demiral’a ilk müdahale yapılırken otomobil sürücüsü Dilek Kurt gözyaşlarına sahip olamadı. Sinir krizleri geçiren Kurt, “Benim de çocuğum var. Onun da çocuğu vardır. O da evine ekmek götürüyordur. Ben bir daha çocuğumu göremeyecek miyim” diyerek gözyaşlarına boğuldu.  Olay yerine gelen 112 Acil Servis ambulansı ile Gazipaşa Devlet Hastanesine kaldırılan Demiral tüm müdahalelere rağmen kurtarılamadı. Demiral’ın evli ve iki çocuk babası olduğu öğrenildi.    , İLGİLİ HABERLER, Üretim ve Tasarım.
+                    Bilgi Grubu</t>
+  </si>
+  <si>
+    <t>Kahramanmaraş'ta jandarma trafik ekipleri, "8 Mart Dünya Kadınlar Günü" dolayısıyla kadın sürücü ve yolculara karanfil dağıttı.    Onikişubat İlçe Jandarma Komutanlığına bağlı trafik timleri, 8 Mart Dünya Kadınlar Günü'nde kadınları unutmayarak, sabahın erken saatlerinde TürkoğluKahramanmaraş yolu üzerinde bulunan Hacı Mustafa Mahallesinde uygulama noktası oluşturdu.  Uygulama noktasından geçen kadın sürücü ve yolcuları durduran jandarma, karanfil vererek Kadınlar Günü'nü kutladı. Rutin kontrol yapılacağını düşünen kadınlar, karanfil hediyesini görünce şaşkınlıklarını gizleyemedi ve memnuniyetlerini dile getirdi.    , İLGİLİ HABERLER, Üretim ve Tasarım.
+                    Bilgi Grubu</t>
+  </si>
+  <si>
+    <t>Kaza, gece saatlerinde ilçeye bağlı Halide Edip Adıvar Caddesi ile İnönü Caddesi kesişimin de bulunan Üçyol Kavşağı’nda meydana geldi., İddiaya göre, Gül Ö. (41) idaresindeki 35 KH 3132 plakalı otomobil, Üçyol Kavşağı’nda kırmızı ışık ihlali yaparak dönüş yaptığı esnada, kimliği henüz belirlenemeyen kadın sürücünün idaresindeki 35 GD 3613 plakalı otomobil ile çarpıştı. Kazada otomobil sürücüsü Gül Ö., hafif şekilde yaralanırken, yanında bulunan arkadaşı Eda. S(40),yara almadı. Her iki araçta da maddi hasar meydana geldi., ,  , LEVYEYLE DEHŞET SAÇTI İDDİASI , , , Araçların karıştığı kaza sonrası, kimliği belirlenemeyen 35 GD 3613 plakalı otomobilin sürücüsü aracından inerek, otomobiline levye ile saldırdığı iddiasında bulunan Gül Ö., olay anında çok korktuklarını ifade ederek, sözlerini şu şekilde sürdürdü, “Kavşaktan dönerken saniyelik bir şekilde kırmızıda geçmişim. Karşı taraftan gelen araç, otomobilimin sağ tarafından vurdu. Sonra diğer sürücü levye ile birlikte aracından inerek, bana küfürler savurup aracımın camını patlattı. Camın içinden sarkarak levye ile üzerime saldırdı. Arkadaşım kafamı korumuş olmasaydı şuan beynim patlamış olabilirdi. Hala olayın şokundayım” dedi., Otomobil içerisindeki Eda S. ise yaşanılan olayı şu şekilde aktardı, “Seyir halinde kavşaktan dönerken bir kaza yaşandı. Diğer otomobildeki sürücü aracından levye ile çıkarak üzerimize saldırdı. Şoför tarafındaki cama patlatana kadar levye ile vurdu. Sanırım canımıza kast etmek istedi. Bu durumdan dolayı mağduruz” diye konuştu., KAZA SONRASI BAYGINLIK GEÇİRDİ , Kazanın şokunu atlatamayan ve yaşadığı korku dolu anlar sonucu baygınlık geçiren Gül Ö.’ye ilk müdahale olay yerindeki yakınları ve trafik polislerince yapıldı. İhbar üzerine gelen 112 Acil Sağlık ekiplerince ambulansa alınan Gül Ö.’nün sağlık durumunun iyi olduğu öğrenildi., Kaza sonrası, polis ekiplerince, olay yerinden hızla uzaklaşan otomobil sürücüsünü yakalamak için alışma başlatıldı., , BAKMADAN GEÇME, Üretim ve Tasarım. Bilgi Grubu</t>
+  </si>
+  <si>
+    <t>https://www.haberturk.com/malatya-haberleri/87963520-hafriyat-kamyonunun-carptigi-kadin-oldu-surucu-gozaltinda</t>
+  </si>
+  <si>
+    <t>MALATYA, (DHA)MALATYA'da, yolun karşısına geçmeye çalışan Şengül Uçar (56), hafriyat kamyonunun çarpması sonucu yaşamını yitirdi. Sürücü Bayram G. (47), gözaltına alındı. Kaza, sabah saatlerinde, Cevatpaşa Mahallesi'nde meydana geldi. Bayram G., yönetimindeki 44 BS 187 plakalı hafriyat kamyonuyla yolun karşısına geçmek isteyen Şengül Uçar'a çarptı. Kazayı görenlerin ihbarıyla bölgeye polis ve sağlık ekipleri sevk edildi. Sağlık görevlilerince ilk müdahalesi yapılan ağır yaralı Uçar, ambulansla Malatya Eğitim ve Araştırma Hastanesi'ne kaldırıldı. Tedaviye alınan Şengül Uçar, doktorların tüm çabasına rağmen kurtarılamadı. Sürücü Bayram G. ise gözaltına alındı. Kazayla ilgili soruşturma başlatıldı. DHA-Güvenlik Türkiye-Malatya Taha AYHAN2021-06-10 17:49:11 , İLGİLİ HABERLER, Üretim ve Tasarım.
+                    Bilgi Grubu</t>
+  </si>
+  <si>
+    <t>https://www.haberturk.com/sivas-haberleri/85346632-sivasta-jandarmadan-kadin-surucu-ve-yolculara-cicek</t>
+  </si>
+  <si>
+    <t>SİVAS, (DHA)SİVAS'ın Kangal ilçesinde jandarma ekipleri, 8 Mart Dünya Kadınlar Günü nedeniyle kontrol noktasında durdurulan kadın sürücü ve yolculara çiçek verdi. İl Jandarma Komutanlığı'na bağlı, İlçe Jandarma Komutanlığı Trafik Timleri, 8 Mart Dünya Kadınlar Günü nedeniyle yol kontrol noktasında durdurulan kadın sürücü ve yolculara sürpriz yaptı. Araçları tek tek durduran ekipler, sürücü veya yolcu durumundaki kadınlara çiçek vererek, kolonya ve çikolata ikramında bulundu. Uygulamadan memnun kalan kadınlar, ekiplere duyarlılıkları için teşekkür etti.  DHA-Genel Türkiye-Sivas Hüsnü Ümit AVCI2021-03-08 14:54:12 , İLGİLİ HABERLER, Üretim ve Tasarım.
+                    Bilgi Grubu</t>
+  </si>
+  <si>
+    <t>Konya'nın Selçuk ilçesinden iki yaşındaki kızını yanına alarak evden ayrılan kadın, eşinin ihbarıyla polisi alarma geçirdi. Otomobille Aksaray yönüne giderken, 3 kontrol noktasında durmayan kadın sürücü, polisin kurduğu kapanla durdurulabildi.Aracından inmeyen anne, arka koltuktaki çocuğun yanına geçerken, uzun süren ikna çalışmasının ardından hastaneye kaldırıldı., , Olay,  Konya'nın merkez Selçuklu ilçesinde yaşandı. İHA'nın haberine göre, psikolojik sorunları olan ve bir süredir tedavi gördüğü öğrenilen A.K.Ç. (34),eşinin evde olmadığı sırada 2 yaşındaki kızı F.Ç.'yi de alarak otomobille evden ayrıldı. Kısa bir süre sonra eve geldiğinde eşini ve çocuğunu göremeyen S.Ç. (36),eşinin psikolojik sorunları olması ve tedavi görmesi nedeniyle durumu hemen polise bildirdi., , UYGULAMA YAPAN EKİPLERE BİLGİ VERİLDİ, İhbar üzerine harekete geçen Konya İl Emniyet Müdürlüğü ekipleri, kadının kullandığı otomobili Aksaray-Konya karayolunda Plaka Tanıma Sistemi (PTS) aracılığıyla bularak Aksaray istikametine gittiğini tespit etti. Bunun üzerine Aksaray yönünde yaklaşık 5 kilometre ileride uygulama yapan ekiplere anonsla bilgi verildi. Yolda güvenlik önlemleri alan polis ekipleri kadının kullandığı araca 'dur' ihtarında bulundu. A.K.Ç. polisin dur ihtarına uymayarak aşırı süratli şekilde Aksaray istikametine kaçmaya devam etti., , POLİSTAN SONRA JANDARMADAN DA KAÇTI, Bu sırada Kızören mevkiinde bulunan jandarma ekiplerine bilgi verildi. Bir süre sonra Kızören mevkiinde jandarma ekiplerinin de dur ihtarına uymayarak hızla kaçmayı sürdüren sürücü A.K.Ç., Aksaray istikametine devam etti. Ardından yol güzergahındaki Aksaray'ın Sultanhanı İlçe Polis Merkezine haber verildi. Sultanhanı İlçe Polis Merkezi ekipleri de yolda güvenlik önlemi alırken, A.K.Ç. burada da 'dur' ihtarına uymayarak hızla Aksaray istikametine kaçmayı sürdürdü., AKSARAY GİRİŞİNDE KAPAN KURULDU, , Aksaray girişinde polis ekipleri geniş güvenlik önlemleri aldı. Sürücü A.K.Ç.'nin psikolojik sorunları olması ve otomobilde 2 yaşında bir kız çocuğunun bulunması nedeniyle Aksaray İl Emniyet Müdürlüğü ekipleri büyük bir hassasiyetle operasyonu yönetirken, kadının 3 ayrı noktada 'dur' ihtarına uymadığı ve yine durmayacağı değerlendirilerek uygulama noktasından 500 metre ileriye kapan kuruldu. Aksaray'a giren kadın sürücüyü arkasından bir sivil ekip otosu sürekli olarak takip etti. Uygulama noktasına yaklaşması bilgisi üzerine uygulama noktasında bulunan polis ekipleri yoldan geçen araçlarla kısmen depolama yaptı., Ardından hızla geldiği görülen kırmızı otomobil, depolama yapılmasına rağmen dur ihtarında bulunan polis memurunun üzerine araç sürerek sağında bulunan aracı kıl payı kurtararak süratli bir şekilde uygulama noktasını geçti. Bunun üzerine 500 metre ileride bulunan kapan diğer polis ekipleri tarafından açıldı. A.K.Ç. otomobille kapanın üzerinden geçerken, patlayan lastikler bir süre sonra indi. Karasu Kavşağı'na kadar devam eden kadın sürücü burada lastiklerinin inmesi ve kırmızı ışıkta bekleyen diğer araçlar olması nedeniyle durmak zorunda kaldı. Polis ekipleri her ihtimale karşı yolda ve çevrede geniş güvenlik önlemleri alırken, lastikler polis ekiplerince bıçakla kesilerek tamamen patlatıldı., , KAPILARI KİLİTLEYİNCE CAMLAR KIRILDI, Araç içerisinde kapıları kilitleyen sürücü A.K.Ç. polis ekiplerine zor anlar yaşattı. Camları tamamen kapatarak kapıları kilitleyen kadın, uzun süre polis ekiplerince ikna edilmeye çalışıldı. Uzun uzun uğraşan ve yoğun bir çaba gösteren polis ekipleri kadına kapıyı açtıramadı. Havanın sıcak olmasını, otomobilin camlarının da tamamen kapalı olmasını ve araç içerisinde 2 yaşında bir kız çocuğunun bulunmasını göz önünde bulunduran polis ekipleri bunalma ve boğulma ihtimaline karşı kadın ve kızının sağlığı açısından otomobilin camını kırmak zorunda kaldı. Polis memuru araçtan getirdiği acil çıkış demiri ile otomobilin sağ ön camını kırdı ve içeriye hava girmesini sağladı., KORKAN KADIN TELEFONLA EŞİNİ ARADI, , Eliyle camları temizleyen polis bu sefer de kadının çığlıklarıyla karşı karşıya kaldı. Kadının psikolojik sorunları olması nedeniyle polis ekipleri büyük bir hassasiyetle kadına yaklaşmaya çalıştı. İlk olarak kadının kucağında bulunan ve ağlayan kız çocuğunu almak isteyen polis ekipleri kadının çığlıkları ve ısrarı üzerine çocuğu alamadı. Kadının sakinleşmesi için su vererek ikna etmeye çalışan polis ekipleri olay yerine 112 Acil Sağlık ekibi çağırdı. Sağlık ekipleri de kadını ikna etmek için uzun bir süre çaba sarf ederken, korkan kadın telefonla eşini aradı. Eşinden yardım isteyen kadın zaman zaman, "Benim çocuğum, hayır. Sabri, Sabri, Sabri lütfen gel. Biraz uzaklaşın benden. Çantamı bırak. Sabri etrafımızda bir sürü adam var. Bir dakika sessiz olun. Sabri çabuk yetiş Sabri, Fatma çok korktu. Nevşehir yolundayız. Kapıları açtılar zaten hava alıyoruz" dedi., , 'SABRİ, FATMA'YI KAYBETMEK İSTEMİYORUM', Polis ekipleri korkmaması gerektiğini defalarca söylemesine rağmen korkularını gideremeyen ve sürekli ağlayan A.K.Ç., "Lütfen beni bir rahat bırakın. Kapıları kapatın. Eşimle rahatça konuşayım sonra ne olacaksa olsun. Sabri korkuyorum. Korkumu giderecek bir şey söyler misin bana. Senin sesini duymak istiyorum. Fatma'mı almazlar değil mi? Sabri, Fatma'yı kaybetmek istemiyorum” telefonda eşine ağladı., POLİS KIZ ÇOCUĞUNUN YÜZÜNÜ YIKADI, Uzun uğraşlara rağmen bir türlü ikna olmayan kadın, telefonun bir ucunda da eşi tarafından araçtan inmesi yönünde ikna edilmeye çalışıldı. Annesinin kucağında ne olduğunu anlamayan ve çığlıklarla ağlayan 2 yaşındaki kız çocuğu polis ekiplerince sakinleştirilmeye çalışıldı. Yaklaşık 1 saat süren ikna süresince havasızlıktan ve terden sırılsıklam olan kız çocuğunun yüzünü ve kafasını polis ekipleri araç içerisinde yıkadı. Ardından telefonda eşinin, polisin ve sağlık ekiplerinin büyük çabasıyla ikna olan kadın kucağında çocuğuyla birlikte araçtan inerek ambulansa bindirildi., , AKSARAY'DA TEDAVİ ALTINA ALINDI, 112 Acil Sağlık kepleri, çocuk ve kadına ilk müdahaleyi olay yerinde ambulans içerisinde yaptı. Ambulans içerisinde sedyeye yatırılan kadın, çocuğunu bir an kucağından bırakmadı. İlk müdahalelerinin ardından kadın ve kızı ambulansla Aksaray Üniversitesi Eğitim ve Araştırma Hastanesi Acil Servisi'ne getirildi. Ambulanstan sedyeyle indirilen kadının kız çocuğunu kucağından bırakmaması dikkat çekerken, kadın ve kızı acil serviste tedavi altına alındı. Olayla ilgili soruşturma başlatıldı., , BAKMADAN GEÇME, Üretim ve Tasarım. Bilgi Grubu</t>
+  </si>
+  <si>
+    <t>Zonguldak’ın Ereğli ilçesinde trafik kazası meydana geldi. Bariyerlere çarparak kullanılamaz hale gelen araçta sürücü ağır yaralandı.    Kaza; saat 13.25 sularında, Kdz. Ereğli  Alaplı karayolu Tersaneler bölgesinde meydana geldi. Edinilen bilgilere göre, Kdz. Ereğli'den Alaplı'ya seyir halinde olan Pınar G. (31) idaresindeki 61 ES 378 plakalı Opel marka otomobil, sürücünün kontrolü kaybetmesi sonucu bariyerlere çarptı. Kazada aracın ön camının ve hava yastıklarının patladığı görülürken sürücü Pınar G. ağır yaralandı. Kazayı görenlerin 112 Acil Çağrı Merkezi'ne ihbarda bulunmaları üzerine, olay yerine sağlık ve polis ekipleri sevk edildi. Kazada yaralanan sürücü Pınar G., olay yerinde yapılan ilk müdahalenin ardından ilçede bulunan özel hastaneye kaldırıldı. Olay yerine gelen polis ekipleri bölgede güvenlik önlemi alarak, trafik kontrollü bir şekilde sağlandı. Kazaya karışan otomobil çekici yardımıyla yoldan kaldırılırken, araç kullanılamaz hale geldi. Kaza ile ilgili soruşturma başlatıldı.    , İLGİLİ HABERLER, Üretim ve Tasarım.
+                    Bilgi Grubu</t>
+  </si>
+  <si>
+    <t>https://www.hurriyet.com.tr/dur-ihtarina-uymayan-kadin-surucu-kazada-oldu-40834553</t>
+  </si>
+  <si>
+    <t>, , Yusuf ÇINAR/ÇORUM, (DHA)- ÇORUM'da sürücüsü polisin 'Dur' ihtarına uymayan otomobil, kontrolden çıkarak yol kenarındaki demir bariyerlere çarptı. Kazada ehliyetine alkollü araç kullandığı için el konulan sürücü Candan Al (26) yaşamını yitirirken, arkadaşı Esra Yılmaz (24) ağır yaralandı.  Kaza, Çorum-Samsun karayolu 4'üncü kilometrede meydana geldi. İddiaya göre, Samsun yönünden Çorum istikametine giden Candan Al idaresindeki 19 AL 353  plakalı otomobil, bölge trafik önünde polisin 'Dur' ihtarına uymadı. Hızla uzaklaşan otomobil, bir süre sonra sürücüsünün direksiyon hakimiyetini kaybetmesi sonucu kontrolden çıkarak yol kenarındaki demir bariyerlere çarptı. Kazada otomobil sürücüsü Candan Al ve yanındaki arkadaşı Esra Yılmaz ağır yaralandı. İki yaralı olay yerine sevk edilen ambulanslarla Çorum Erol Olçok Eğitim ve Araştırma Hastanesi'ne kaldırıldı. Otomobil sürücüsü Candan Al, doktorların tüm müdahalesine rağmen kurtarılamadı. Polisin yaptığı incelemede, sürücünün alkollü araç kullandığı gerekçesiyle ehliyetine 2 yıl süre ile el konulduğu belirlendi. Kaza ile ilgili soruşturma sürüyor., FOTOĞRAFLI, Hurriyet.com.tr’nin Çorum haberleri bölümünde, DHA’nın abonelerine gönderdiği Çorum haberleri otomatik olarak derlenmektedir. hurriyet.com.tr editörleri otomatik akış içinde 'Dur' ihtarına uymayan kadın sürücü kazada öldü, arkadaşı yaralı haberine editoryal müdahalede bulunmamıştır. Haber içeriklerinden hukuken ilgili ajanslar sorumludur., Sayfa Başı, © Copyright 2021Hürriyet Gazetecilik ve Matbaacılık A.Ş.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HÜRRİYET'E BAĞLI KAL, E-Gazete ile tüm gelişmeler, bilgisayar, tablet ve telefonunda., Aşağıdaki linke tıklayarak, üyelik işlemlerini gerçekleştirebilirsin., Hürriyet haberlerinden geri kalma, tüm aboneliklerini yönet ve abone ol., Dünyadan en güncel haberler, Türkiye'den sondakika haberleri, ekonomi dünyasından en flaş gelişmeler için Hürriyet'in uygulamalarını kullanabilirsiniz., Kaza, saat 12.00 sıralarında Adnan Kahveci Mahallesi Yavuz Selim Bulvarı'nda meydana geldi.34 JY 3177 plakalı otomobili kullanan sürücü iddiaya göre kavşaktan bir aracın kontrolsüz çıktığını görünce ona çarpmamak için direksiyonu aniden kırdı. Otomobil hızla refüje çıkarak buradaki yön tabelalarını devirerek durdu. Otomobili kullanan kadın sürücü için 112 Ambulansı istenirken polise de haber verildi. Hayati tehlikesi bulunmadığı belirtilen sürücü, ambulans ile hastaneye kaldırıldı. Soruşturma sürdürülüyor.,  , Kripto Para Piyasaları   için Bigpara, Kripto Para Piyasaları   için Bigpara, Türkiye gündeminden son dakika haberleri, bugün yaşanan en son gelişmeler, siyaset gündeminden güncel haberler ve bütün son dakika haberleri için Hürriyet'in internet haber sitesi hurriyet.com.tr; Hurriyet.com.tr haber içerikleri kaynak gösterilmeden alıntı yapılamaz, Kanuna aykırı ve izinsiz olarak kopyalanamaz, başka yerde yayınlanamaz.,  © Copyright 2021 Hürriyet Gazetecilik ve Matbaacılık A.Ş </t>
+  </si>
+  <si>
+    <t xml:space="preserve">HÜRRİYET'E BAĞLI KAL, E-Gazete ile tüm gelişmeler, bilgisayar, tablet ve telefonunda., Aşağıdaki linke tıklayarak, üyelik işlemlerini gerçekleştirebilirsin., Hürriyet haberlerinden geri kalma, tüm aboneliklerini yönet ve abone ol., Dünyadan en güncel haberler, Türkiye'den sondakika haberleri, ekonomi dünyasından en flaş gelişmeler için Hürriyet'in uygulamalarını kullanabilirsiniz., Emniyet Genel Müdürlüğü verilerinden derlenen bilgiye göre, 2006 yılında 2 milyon 872 bin 951 olan kadın sürücü sayısı, 10 yıl içinde 6 milyon 533 bin 500'e yükseldi.   10 yıl önce toplam sürücü sayısı 17 milyon 586 bin 179 iken bu sayının 14 milyon 713 bin 228'ini erkekler, 2 milyon 872 bin 951'ini de kadınlar oluşturuyordu. Bir başka ifadeyle, toplam sürücü sayısının yüzde 83,7'si erkek, yüzde 16,3'ü ise kadındı. Son 10 yıl baz alındığında, kadın sürücülerin sayısı yaklaşık 3 kat artışla 6 milyon 533 bin 500'e yükselirken, erkek sürücü sayısı ise 20 milyon 955 bin 650'ye ulaştı.ERKEKLERE GÖRE 3 KAT FAZLA ARTTI, Buna göre, erkek sürücü sayısı yüzde 42,4 artarken, kadın sürücü sayısı ise yüzde 127,4 artış gösterdi. Böylece 10 yıl önce ehliyet sahibi olanların yüzde 16,3'ünü oluşturan kadın sürücülerin oranı yüzde 23,8'e çıkarken, erkek sürücülerin oranı yüzde 83,7'den yüzde 76,2'ye geriledi. Türkiye'de kayıtlı sürücü sayısı ise 10 yıl öncesine göre yüzde 56,3 artışla 27 milyon 489 bin 150'ye yükseldi. Böylece ehliyetli kadın sürücü sayısı, İstanbul'dan sonra nüfus bazında en kalabalık şehirler olan Ankara ve İzmir'in nüfusunu da aşarak, toplamda 80 ilin nüfusunu geçmiş oldu., Kripto Para Piyasaları   için Bigpara, Kripto Para Piyasaları   için Bigpara, Türkiye gündeminden son dakika haberleri, bugün yaşanan en son gelişmeler, siyaset gündeminden güncel haberler ve bütün son dakika haberleri için Hürriyet'in internet haber sitesi hurriyet.com.tr; Hurriyet.com.tr haber içerikleri kaynak gösterilmeden alıntı yapılamaz, Kanuna aykırı ve izinsiz olarak kopyalanamaz, başka yerde yayınlanamaz.,  © Copyright 2021 Hürriyet Gazetecilik ve Matbaacılık A.Ş </t>
+  </si>
+  <si>
+    <t>https://www.hurriyet.com.tr/gundem/korna-calan-kadin-surucuyu-darp-eden-supheli-yakalandi-41401176</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HÜRRİYET'E BAĞLI KAL, E-Gazete ile tüm gelişmeler, bilgisayar, tablet ve telefonunda., Aşağıdaki linke tıklayarak, üyelik işlemlerini gerçekleştirebilirsin., Hürriyet haberlerinden geri kalma, tüm aboneliklerini yönet ve abone ol., Dünyadan en güncel haberler, Türkiye'den sondakika haberleri, ekonomi dünyasından en flaş gelişmeler için Hürriyet'in uygulamalarını kullanabilirsiniz., Sosyal medya üzerinde bir kadın sürücünün yolda korna çaldığı için tartıştığı bir sürücü tarafından yol ortasında darp edildiği görüntülerin yayınlanması üzerine polis harekete geçmişti. Akşam saatlerinde ani fren yapmasının ardından arkasındaki otomobili kullanan kadın sürücüye saldıran şüpheli, onu iterek ve vurarak yere yıktıktan sonra çevredekilerin müdahalesi üzerine otomobiline binerek uzaklaşmıştı., 108 LİRA CEZA KESİLDİ, Trafik Denetleme Şube Müdürlüğü ekiplerinin görüntüleri incelemesinin ardından kimliği tespit edilen sürücü H.H.B. gözaltına alındı. Sürücü H.H.B.'ye Karayolları Trafik Kanunun 59. maddesinden (Yerleşim yerleri dışındaki karayolunda zorunlu haller dışında duraklamak veya park etmek, zorunlu hallerde gerekli önlemleri almadan duraklamak veya park etmek) 108 TL Trafik İdari Para cezası kesildi., ADLİ İŞLEM YAPILACAK, Ancak darp edilen kadın sürücü Ş.A.'nın şikayeti üzerine sürücü H.H.B. adli işlemlerin yapılması için Eyüpsultan Polis merkezi amirliğine teslim edildi.,  , Kripto Para Piyasaları   için Bigpara, Kripto Para Piyasaları   için Bigpara, Türkiye gündeminden son dakika haberleri, bugün yaşanan en son gelişmeler, siyaset gündeminden güncel haberler ve bütün son dakika haberleri için Hürriyet'in internet haber sitesi hurriyet.com.tr; Hurriyet.com.tr haber içerikleri kaynak gösterilmeden alıntı yapılamaz, Kanuna aykırı ve izinsiz olarak kopyalanamaz, başka yerde yayınlanamaz.,  © Copyright 2021 Hürriyet Gazetecilik ve Matbaacılık A.Ş </t>
+  </si>
+  <si>
+    <t>https://www.hurriyet.com.tr/gundem/maltepede-kazadan-sonra-kadin-surucu-soka-girdi-41468689</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HÜRRİYET'E BAĞLI KAL, E-Gazete ile tüm gelişmeler, bilgisayar, tablet ve telefonunda., Aşağıdaki linke tıklayarak, üyelik işlemlerini gerçekleştirebilirsin., Hürriyet haberlerinden geri kalma, tüm aboneliklerini yönet ve abone ol., Dünyadan en güncel haberler, Türkiye'den sondakika haberleri, ekonomi dünyasından en flaş gelişmeler için Hürriyet'in uygulamalarını kullanabilirsiniz., Kaza, saat 20.30 sıralarında Maltepe Fındıklı Mahallesi Başıbüyükyolu Caddesi üzerinde meydana geldi. Melek Çiftçi’nin kullandığı 59 UZ 319 plakalı otomobil, sürücüsünün direksiyon hakimiyetini kaybetmesiyle kontrolden çıkarak içinde oturan kişilerin bulunduğu cadde üzerinde park halindeki 59 TE 029 plakalı araca çarptı. İhbar üzerine olay yerine sağlık ve polis ekipleri sevk edildi. Polis ekipleri, vatandaşları kaza yerinden uzaklaştırdı. Olayda 3 kişi yaralanırken, kaza yapan otomobilin sürücüsü Melek Çiftçi, uzun süre şoktan kurtulamadı. Sedyeye yatmak istemeyen yaralı sürücü, vatandaşlara kaza yaptığı otomobilini sordu. Yaralılar, olay yerine gelen ambulanslarla hastanelere kaldırıldı. Mahalle sakini kazanın yaşandığı caddeden geçen otomobillerin çok hızlı olduğunu, bu nedenle kazaların çok yaşandığını söyledi., Kazayı gören bir kişi, Tam net göremedim ama orada iki kişi sohbet ediyorlardı. Duran arabaya dengeyi, direksiyon hakimiyetini kaybetti, vurdu. Duran arabada 2 kişi, bir de bir bayan var." dedi., Kripto Para Piyasaları   için Bigpara, Kripto Para Piyasaları   için Bigpara, Türkiye gündeminden son dakika haberleri, bugün yaşanan en son gelişmeler, siyaset gündeminden güncel haberler ve bütün son dakika haberleri için Hürriyet'in internet haber sitesi hurriyet.com.tr; Hurriyet.com.tr haber içerikleri kaynak gösterilmeden alıntı yapılamaz, Kanuna aykırı ve izinsiz olarak kopyalanamaz, başka yerde yayınlanamaz.,  © Copyright 2021 Hürriyet Gazetecilik ve Matbaacılık A.Ş </t>
+  </si>
+  <si>
+    <t>, , Umut KARAKOYUN/İZMİR, (DHA)- EMNİYET mensupları, 10 Nisan Polis Haftası'nı kutlamaya hazırlanırken, İzmir'de trafikte görev yapan kadın polisler, özellikle denetimde kural tanımayan sürücülere göz açtırmıyor. Kadın trafik polisleri, 2018 yılının 3 ayında 25 bin aracı denetledi. Kadın polislere en büyük desteği ise kadın sürücüler veriyor.İzmir Emniyet Müdürlüğü Trafik Denetleme Şube Müdürlüğü'nde çalışan 38 kadın personelden, 20'si, trafik akışını düzenliyor, yol kontrolü yapıyor, sürücülerin kurallara uyması için çalışıyor. Denetleme hizmetlerinde çalışan kadın polis memurları, 2'şer kişilik ekipler halinde, İzmir'in trafiğini kontrol altında tutuyor. 18 yıllık polis memuru Neşe Sağcan, 6 yıldır ekiplerde görevli. Her zaman dışarda olduklarını ve sürücülerden ilginç tepkiler aldıklarını söyleyen Neşe Sağcan, bazı sürücülerin kadın trafik polisleri ile karşılaştıklarında çok şaşırdıklarını söyledi. Bunun yanı sıra çok güzel tepkiler de aldıklarını belirten Sağcan, "Kavşaklarda bize selam gönderip çok güzel olduğumuzu söyleyen çok sayıda kişi var. Sıkıntı yaşadığımız zamanlar da oluyor. Agresif sürücülerimiz çok fazla. Ama bir kadın olarak bunların üstesinden gelebiliyoruz. Bir oğlum var, yaptığım işten dolayı o da çok memnun. Bir kadının aktif şekilde çalışması onu da mutlu ediyor" dedi.'VATANDAŞIN GÜVENLİĞİ İÇİN BURDAYIZ'Aynı şubede görevli 18 yıllık polis memuru Aysun Baybörü de 4 yıl önce ekiplerde göreve başladı. İşini severek yaptığını vurgulayan Baybörü, özellikle kadınlardan cesaret verici sözler duyduklarını ve bunun da kendilerini mutlu ettiğini dile getirdi. Baybörü, şöyle konuştu:"Trafikte olmak güzel ancak bazen kötü anlarımız da olabiliyor. Çünkü çok farklı insanlarla karşılaşabiliyoruz. Buna rağmen çevremizden çok güzel tepkiler alıyoruz. Özellikle kadınlardan çok fazla tebrik alıyoruz. Bizi görünce gurur duyduklarını söylüyorlar. Bu durum bizi mutlu ve motive ediyor. Bu şekilde geri dönüşler almak güzel. Dışarısı yoğun, yorucu ama güzel. Trafikteki denetimleri titizlikle yapmamızdaki tek amaç, daha güvenli bir trafik akışı sağlamak. Bazen kural ihlalinden dolayı ceza yazdığımızda tepki gösterenler oluyor ama herkes şunu bilmeli ki biz vatandaşların güvenliği için buradayız."'SAHA GÖREVİNİ MEMURLAR İSTEDİ'İzmir Emniyeti Trafik Denetleme Şube Müdürü Şamil Özsagulu, kadın polis memurlarının vatandaşların güvenli şekilde seyahat etmeleri amacıyla ekip hizmetlerinde görevlendirildiklerini söyledi. Trafik Denetleme Şube Müdürlüğü'nün yüzde 10'luk bölümünü kadın personelin oluşturduğunu kaydeden Şamil Özsagulu, "Kadın personel ekiplerimiz, yolcuların sağlıklı şekilde seyahat etmeleri ve kent merkezinde trafik kazalarını en aza indirmek için üstün bir çaba sarf ediyorlar. 2018 yılının 3 ayında 25 bin araç sadece kadın personel tarafından denetlendi. Trafik güvenliğinde, kadın personelimizin önemli bir payı olduğunu ortada" ifadelerini kullandı. Kadın trafik memurlarının alanda çalışmasının özel bir tercih olmadığını açıklayan Özsagulu, personelin istekleri doğrultusunda bu şekilde bir çalışma sistemi kurduklarını vurguladı.YOLCULARDAN KADIN POLİSLERE DESTEKTrafik kontrol noktalarında kadın polis memurları ile karşılaşan sürücüler de şaşkınlıklarını gizleyemiyor. Memurlara destek veren sürücülerden Hasip Sabunoğlu, kadın trafik polislerinin bu görevi yürütmesinin çok güzel olduğuna değindi. Taner Sarıhan isimli sürücü ise "Trafikte  kadın memur görmek çok önemli, İzmir'e yakışan bir durum. Kadın daha zarif, daha insancıl" dedi. Bazı sürücüler de trafik polislerinin kadın olmasının çok daha iyi olduğunu çünkü kadınların daha kibar ve  güven verici olduklarını belirtti.FOTOĞRAFLI, Hurriyet.com.tr’nin İzmir haberleri bölümünde, DHA’nın abonelerine gönderdiği İzmir haberleri otomatik olarak derlenmektedir. hurriyet.com.tr editörleri otomatik akış içinde Kadın trafik polislerine, kadın sürücü desteği haberine editoryal müdahalede bulunmamıştır. Haber içeriklerinden hukuken ilgili ajanslar sorumludur., Sayfa Başı, © Copyright 2021Hürriyet Gazetecilik ve Matbaacılık A.Ş.</t>
+  </si>
+  <si>
+    <t>https://www.hurriyet.com.tr/yerel-haberler/gaziantep/islahiye/jandarmadan-kadin-surucu-ve-yolculara-cicek-41757846</t>
+  </si>
+  <si>
+    <t>Jandarmadan, kadın sürücü ve yolculara çiçek, , , Kadir ÇELİK/İSLAHİYE(Gaziantep), (DHA)- Gaziantep’in İslahiye ilçe Jandarma ekiplerince yol kontrol uygulamasında kadın sürücü ve yolculara 8 Mart Dünya Kadınlar Günü nedeniyle çiçek dağıtıldı.İslahiye-Hasa karayolunda bulunan kontrol noktasında İlçe Jandarma Komutanı Binbaşı Ümit Tahta'nında katıldığı uygulamada ekipler, kadın sürücü ve yolculara çiçek hediye ederek,8 Mart Dünya Kadınlar Günü’nü kutladı. Jandarma ekiplerinin sürpriziyle karşılaşan kadınlar, jest karşısında jandarmalara teşekkür etti., FOTOĞRAFLI, Islahiye haberleri Hürriyet yerel haberler sayfasında. Haber ajanslarının Islahiye ilinden Jandarmadan, kadın sürücü ve yolculara çiçek hakkında ilettiği tüm haberler hurriyet.com.tr farkı ile sizlere ulaştırılıyor. Bu haber ilk olarak 08 Mart 2021 tarihinde saat 13 35’de yayınlandı. Son dakika gelişmesi oldukça Jandarmadan, kadın sürücü ve yolculara çiçek haberi güncellenecektir., Sayfa Başı, © Copyright 2021Hürriyet Gazetecilik ve Matbaacılık A.Ş.</t>
+  </si>
+  <si>
+    <t>Olay, Kocaeli İzmit ilçesi Leyla Atakan Caddesi ile Cumhuriyet Caddesi’nin kesiştiği kavşakta meydana geldi. Edinilen bilgilere göre, İrem Ö. (22) idaresindeki 41 BY 126 plakalı Opel marka araç, karşıdan karşıya geçmeye çalışan Merve Pala (16) ile Gizem Sude Adıgüzel’e (16) çarptı. Çarpışmanın etkisi ile yere düşen Merve Pala kanlar içinde kaldı. Gizem Sude Özdemir ise kazayı hafif sıyrıklarla atlattı., Kazayı gören çevredeki vatandaşlar durumu hemen 112 Acil Yardım ekiplerine bildirdi. İhbar üzerine olay yerine sağlık ve polis ekipleri sevk edildi. Yaralı genç kıza ise ilk müdahaleyi, olay yerinde tesadüfen bulunan 112 ambulans şoförü yaptı., , "Merve, Merve..." diye seslendi, Ağzından kan gelen ve kendisinden geçen kızı sürekli uyaran sürücünün, 'Merve, Merve" diye uyarması ve kendisine getirmeye çalışması dikkat çekti., Diğer yaralı Gizem Sude Adıgüzel ise yaralı halde yakınları ile telefonda konuşarak durumunun iyi olduğunu anlatmaya çalıştı. Kısa süre sonra olay yerine gelen sağlık ekipleri tarafından ilk müdahalesi yapılan yaralılar Umuttepe Üniversite Hastanesi’ne kaldırıldı. Polis ekipleri kazayla ilgili inceleme başlattı., , 
+.cls-1,.cls-2{fill:#231f20;}.cls-2,.cls-4{fill-rule:evenodd;}.cls-3,.cls-4{fill:#d71921;}
+, 
+, Bu site deneyimlerinizi kişiselleştirmek amacıyla KVKK ve GDPR uyarınca çerez(cookie) kullanmaktadır. Bu konu hakkında detaylı bilgi almak için tıklayın.  Sitemizi kullanarak, çerezleri kullanmamızı kabul edersiniz.</t>
+  </si>
+  <si>
+    <t>https://www.karamangundem.com/m/asayis/karaman-da-feci-kaza-kadin-surucu-yaralandi-h416952.html</t>
+  </si>
+  <si>
+    <t>, , , , Kaza bugün 18.00 sıralarında Hamidiye Mahallesi İbrahim Öktem Caddesi üzerinde bulunan mumlu kavşakta meydana geldi.
+ , İddiaya göre H.K.(40) yönetimindeki 70 HC 580 plakalı otomobil ile Ü.O. idaresindeki 70 AAE 172 plakalı otomobil kavşakta çarpıştı. Çarpışmanın etkisi ile kadın sürücü H.K. otomobilin açık camından dışarıya fırladı. Otomobiller ise yaklaşık 20 metre ileriye savrularak orta refüje çarptı.
+Olayı gören çevredeki vatandaşların ihbarı üzerine olay yerine sağlık ve polis ekipleri sevk edildi. Olay yerine gelen ambulansla Karaman Eğitim ve Araştırma Hastanesi’ne kaldırılan kadın sürücü H.K tedavi altına alındı., Olayla ilgili soruşturma başlatılırken yaralanan sürücünün durumunun iyi olduğu öğrenildi.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eskişehir'de meydana gelen trafik kazasında bir kişi hayatını kaybetti., Ayşe Yörükoğlu idaresindeki 81 AAN 360 plakalı otomobil, Eskişehir-Alpu kara yolu Ağapınar Mahallesi yakınlarında sürücüsünün direksiyon hakimiyetini kaybetmesi sonucu yol kenarında bulunan tarlaya devrildi., Tepebaşı İlçe Sağlık Müdürlüğünde işçi olarak çalıştığı öğrenilen Ayşe Yörükoğlu, hayatını kaybetti., Yörükoğlu'nun cenazesi, olay yeri incelemesinin ardından otopsi işlemleri için Osmangazi Üniversitesi Tıp Fakültesi morguna kaldırıldı., , 
+Kaynak:Eskişehir Haberleri </t>
+  </si>
+  <si>
+    <t>https://www.kocaelidenge.com/haber/7269807/izmit-trafiginde-siradan-bir-gun-kadin-surucu-trafigi-boyle-tikadi-isyan-edip-arabadan-inenler-var</t>
+  </si>
+  <si>
+    <t>Kocaeli İzmit’in trafiği artık saç baş yolduruyor. Bir taraftan İzmit Yürüyüş Yolu’ndaki çalışmalar, öteki taraftan giderek artan kent trafiği, her şeyi içinden çıkılmaz bir hale sokuyor. Bütün bunlar devam ederken, İnönü Caddesi’ndeki bir manzara isyan ettirdi ve saç baş yoldurdu. Detaylar, Kocaeli Denge’nin özel haberinde.
+, ,  Kocaeli İzmit trafiğinde her şey kötü gidiyor! Trafikte her şey kötüye giderken, bir de buna sürücü hataları eklenince “yok artık” diyoruz. Son dönemde yaşadığımız üzücü olayların etkisiyle araç sayısında artış yaşanıyor. Artık herkesin özel arabası var. Bazı evlerde birden fazla araba bulunuyor. Böyle olunca  trafik sıkışıyor. İzmit Yürüyüş Yolu’nda uzun bir süredir devam eden yenileme çalışmaları da şüphesiz trafiğin artmasına neden olan bir başka etken. Hal böyle olunca, trafik sıkıştıkça sıkışıyor. Ya sürücü hataları? Evet, bir de onlar var…, İzmit İnönü Caddesi, 8 Haziran Salı günü, üstelik trafiğin en yoğun olduğu saatlerde lüks jipiyle seyir halinde olan kadın sürücü, yan yola dönmek istediğinde önünde park halinde bir araç gördü. Normalde, bu aracın solundan rahatlıkla dönebilirdi ama inat etti ve geçmedi. Hiç istifini bozmadan “Önümden çekilsin” dedi. Önündeki aracın sürücüsü o sırada araç içinde değildi. Kadın sürücü, sol taraftan geçmemekte direnince arkada kuyruklar uzadı, arabasından inenler oldu!, İzmit İnönü Caddesi’nde kadın sürücünün yolda durmasının ardından arkada uzun kuyruklar oluştu, bir taraftan kornaya basanlar, bir taraftan bağıranlar derken şehir karıştı. İnönü Caddesi esnafı müdahale etmek istedi, kadını ikna etmek için herkes elinden geleni yapmaya çalıştı. Ama nafile! Kadın sürücü, “nuh dedi, peygamber demedi”! “Kimse benim yoluma aracını park edemez” diyen Balıkesir plakalı kadın sürücüyü kimse durduramadı. Öndeki aracın sürücünün gelmesinden sonra herkes derin bir nefes aldı ve trafik normale döndü. İzmit trafiğinde bugün bir olay daha yaşandı…, 
+08 Haz 2021 - 12:24
+-
+Asayiş
+Yazdır
+, Yorumunuz yarım kaldı, devam etmek için üstteki yoruma, silmek için buraya tıklayın, Kırmızı alanlar eksik veya hatalı girildi. Lütfen bu alanları düzeltip tekrar gönderelim, Yorumunuz için teşekkürler, en kısa sürede gözden geçirilip yayınlanacaktır, Yorum yazarak Kocaeli Denge Topluluk Kuralları’nı kabul etmiş bulunuyor ve yorumunuzla ilgili doğrudan veya dolaylı tüm sorumluluğu tek başınıza üstleniyorsunuz. Yazılan yorumlardan Kocaeli Denge hiçbir şekilde sorumlu tutulamaz., Anadolu Ajansı (AA), İhlas Haber Ajansı (İHA), Demirören Haber Ajansı (DHA) tarafından servis edilen tüm haberler Kocaeli Denge editörlerinin hiçbir editöryel müdahalesi olmadan, ajans kanallarından geldiği şekliyle yayınlanmaktadır. Sitemize ajanslar üzerinden aktarılan haberlerin hukuki muhatabı Kocaeli Denge değil haberi geçen ajanstır., Şimdi oturum açın, her yorumda isim ve e.posta yazma zahmetinden kurtulun. Oturum açmak için bir hesabınız yoksa, oluşturmak için buraya tıklayın.
+, Yorum yazarak  Kocaeli Denge Topluluk Kuralları’nı kabul etmiş bulunuyor ve yorumunuzla ilgili doğrudan veya dolaylı tüm sorumluluğu tek başınıza üstleniyorsunuz. Yazılan yorumlardan Kocaeli Denge hiçbir şekilde sorumlu tutulamaz., Anadolu Ajansı (AA), İhlas Haber Ajansı (İHA), Demirören Haber Ajansı (DHA) tarafından servis edilen tüm haberler Kocaeli Denge editörlerinin hiçbir editöryel müdahalesi olmadan, ajans kanallarından geldiği şekliyle yayınlanmaktadır. Sitemize ajanslar üzerinden aktarılan haberlerin hukuki muhatabı Kocaeli Denge değil haberi geçen ajanstır., 42 - Kadın doğrusunu yapmış, trafik polisi ve cekiciler sokaklarda araba avlayana kadar cadde ortasına parkeden araçları temizlesin, Kadın - Eril diliniz, kadınları suçlayan başlığınız nedeniyle yakında açıklama yapmak zorunda kalacaksınız. , Yazılan yorumlardan Kocaeli Denge hiçbir şekilde sorumlu tutulamaz. Sitemizin Topluluk Kurallarına uymayan yorumlar yayınlanmaz. Yorumunuzla ilgili doğrudan veya dolaylı tüm sorumluluğu tek başınıza üstleniyorsunuz. , Anadolu Ajansı (AA), İhlas Haber Ajansı (İHA), Demirören Haber Ajansı (DHA) tarafından servis edilen tüm haberler Kocaeli Denge editörlerinin hiçbir editöryel müdahalesi olmadan, ajans kanallarından geldiği şekliyle yayınlanmaktadır. Sitemize ajanslar üzerinden aktarılan haberlerin hukuki muhatabı Kocaeli Denge değil haberi geçen ajanstır., 
+Kartepe Uzunçiftlik muhitinde, Hürsoy İnsaat Firmasının yapmış olduğu, Hürsoy City 3.Etapta, 3 katlının 3.katı , 2+1, 117 m2, doğalgaz kombili, ekst..., 
+Seri İlan sayfası için buraya tıklayın.
+Günlük 5 TL den başlayan fiyatlarla ilanınızı şimdi oluşturun
+, Kocaeli Denge, Kocaeli ile özdeşleşen markaları ağırlıyor., +90 (262) 321 34 14  Reklam bilgi, Sitemizde  online, Reklam seçeneklerimizi inceleyin, 
+©Copyright 2021 Kocaeli Denge Tüm Hakları Saklıdır
+-
+Veri PolitikasıKullanım Şartları
++90 (262) 321 34 14
+,  Veri politikasındaki amaçlarla sınırlı ve mevzuata uygun şekilde çerez konumlandırmaktayız. Detaylar için veri politikamızı inceleyebilirsiniz.</t>
+  </si>
+  <si>
+    <t>https://www.medyagazete.com/haber/kisitlama-gununde-baska-bir-aracin-sikistirdigi-kadin-surucu-bariyerlere-carpti-172458</t>
+  </si>
+  <si>
+    <t>Basın Ekspres yolunda kısıtlama gününde başka bir aracın sıkıştırması sonucu, aracın direksiyon hakimiyetini kaybeden sürücü bariyerlere çarptı. Kazada yaralanan sürücü ambulans ile hastaneye kaldırıldı., Kaza Basın Ekspres yolu Yenibosna ayrımında meydana geldi. İddiaya göre 34 YDB 34 plakalı aracın sürücüsü, başka bir aracın sıkıştırması sonucu direksiyon hakimiyetini kaybederek yol ayrımında bulunan bariyerlere çarptı. Çarpmanın sonucunda bariyerler aracın motor kısmına saplandı. Kazayı gören vatandaşlar durumu hemen sağlık, itfaiye ve polis ekiplerine bildirdi. Olay yerine gelen sağlık ekipleri kazada yaralanan kadın sürücüyü ilk müdahalesini olay yerinde yaptıktan sonra ambulans ile hastaneye kaldırdı. Kaza sonrasında bariyerlere saplanan aracı itfaiye ekipleri bariyerlere kurtardı. Kaza sonrasında olay yerine gelen polis ekipleri de yolda bulunan kamera görüntülerini inceleyerek kazaya sebep olduğu iddia edilen aracı yakalamak için çalışma başlattı., Facebook Paylaş, Twitter Paylaş,  Bakan Ersoy: Güvenli Turizm Sertifika Pr... ,  Fırtına afetinin ardından Ayvalıkta enka... , Başka haber bulunmuyor!, , Copyright © 2021 Medya Gazete. Her hakkı saklıdır.</t>
+  </si>
+  <si>
+    <t>Olay, dün saat 15.30 sıralarında Çağlayan Mahallesi 2094 sokakta meydana geldi. Edinilen bilgiye göre, annesini ziyaret etmek için 07 ALL 879 plakalı otomobiliyle yola çıkan sağlık personeli Esra Uludağ (34), tam aracını park edeceği sırada bir ses duydu. İlk başta başka bir araca çarptığını sanan Uludağ, otomobilinin ön camındaki delik ve çatlakları fark edince neye uğradığını şaşırdı. Sürücü Uludağ’ın haber vermesi üzerine olay yerine polis ekipleri sevk edildi. İlk belirlemelere göre deliğin kurşun yüzünden olduğu değerlendirildi. Olay yeri inceleme ekipleri aracın dış ön konsolunda uzun süre boş kovan aradı., , Genç kadının yaşadığı korku yüzünden okunurken, ekipler cam ve çevresinde boş kovana rastlayamadı. Ön konsolda olduğu düşünülen boş kovanın bulunması için araç sanayiye götürüldü., , Olayla ilgili polisin araştırması sürüyor.,  ,  , Türkiye'den ve Dünya’dan son dakika haberler, köşe yazıları, magazinden siyasete, spordan seyahate bütün konuların tek adresi milliyet.com.tr; Milliyet.com.tr haber içerikleri kaynak gösterilmeden alıntı yapılamaz, kanuna aykırı ve izinsiz olarak kopyalanamaz, başka yerde yayınlanamaz., Türkiye’nin haber yaşam platformu Milliyet Dijital yenilendi!, Uygulama ile devam et, gündemi kaçırma!</t>
+  </si>
+  <si>
+    <t>https://www.milliyet.com.tr/gundem/kadin-surucu-ankarayi-birbirine-katti-1870977</t>
+  </si>
+  <si>
+    <t>Olay, sabah saatlerinde gerçekleşti. Polis merkezine düşen, ‘Aracında köpek bulunan alkollü bir kadın, cadde üzerinde yolu trafiğe kapatmış’ ihbarı üzerine ekipler harekete geçti. Polis, Beşevler Mahallesi Alparslan Türkeş Bulvarı üzerindeki aracın yanına geldi. Kadın sürücü, emniyet aracını görünce kaçmaya başladı. Polis ekipleri de sürücünün arkasından devam etti. Kadının gittiği güzergâh telsizle merkeze aktarıldı. Kadın sürücünün ilerlediği kavşaklar ekipler tarafından kesildi. Hızla Konya Yolu istikametine giden sürücü, Kepekli kavşakta trafik kapatılarak durduruldu., , POLİSİN ÜZERİNE SÜRDÜ, Aracından inmeyen kadın yoluna devam etti. Yanında köpeğiyle hızla ilerleyen sürücü, bir sitenin içine girdi. Bir süre sonra buradan ayrılan sürücü ile polis arasındaki kovalamaca ara sokaklarda devam etti. Turan Güneş Bulvarı’na çıkan bayan sürücü, ışıklı kavşakta polis tarafından durduruldu. Polisin ‘in ihtarına’ uymayan sürücü, polisin üzerine aracını sürerek, yoluna devam etti. Kadın sürücü daha sonra ekip araçlarıyla, Yıldız kavşağında kıstırıldı. Aracın içerisinde sigara yakan sürücü, polisin bütün ikazlarına rağmen aşağı inmedi. Bunun üzerine polis, aracın önüne kapan açtı., 4 LASTİĞİ PATLATILDI, Kapanın üzerinden geçen ve 4 lastiği patlayan sürücü, önündeki aracı iterek, kaçmaya devam etti. Bir süre bu civarda polis tarafından kovalan sürücü, soluğu eşinin işyerinin önünde aldı. Sürücü aracından inmekte direnince, polis otomobilin ön camını kırmak zorunda kaldı. Gözaltına alınan sürücü, güçlükle polis otosuna bindirildi., Yanında bulunan köpeği ise bahçenin korkuluk demirliklerine bağlandı. Sahibi gözaltına alınırken havlayan köpek, kadının eşi tarafından binaya alındı., Gözaltına alınan ve isminin Nur A. olduğu öğrenilen sürücü karakola götürüldü., Öte yandan, kovalamaca sırasında bazı araçlarda maddi hasar oluşurken, bir polis aracıda orta refüje çıktı., Türkiye'den ve Dünya’dan son dakika haberler, köşe yazıları, magazinden siyasete, spordan seyahate bütün konuların tek adresi milliyet.com.tr; Milliyet.com.tr haber içerikleri kaynak gösterilmeden alıntı yapılamaz, kanuna aykırı ve izinsiz olarak kopyalanamaz, başka yerde yayınlanamaz., Türkiye’nin haber yaşam platformu Milliyet Dijital yenilendi!, Uygulama ile devam et, gündemi kaçırma!</t>
+  </si>
+  <si>
+    <t>https://www.milliyet.com.tr/gundem/otomobilin-carptigi-7-yasindaki-omer-oldu-surucu-kadin-sinir-krizi-gecirdi-6309593</t>
+  </si>
+  <si>
+    <t>Kaza, saat 11.30 sıralarında Döşemealtı ilçesi Habibler Caddesi’nde meydana geldi. Cadde üzerindeki evlerinden cuma namazına gitmek için çıkan Ömer Sevban Ergin'e Dilek A. yönetimindeki 07 DBD 23 plakalı otomobil çarptı., Otomobilin sürüklediği Ömer, çağrılan sağlık ekibinin müdahalesi sonrası kaldırıldığı hastanede yaşamını yitirdi. Kaza sonrası sinir krizi geçiren otomobil sürücüsü Dilek A.'ya ise sağlık ekipleri müdahale etti. Dilek A., ambulansta yapılan müdahalenin ardından polis merkezine götürüldü., , Kaza sonrası küçük Ömer'in ayakkabısının yolun ortasında kaldığı görüntüler, yürekleri dağladı., KAZA SONRASI ORTAYA ÇIKAN DRAMAntalya'nın Döşemealtı ilçesinde cuma namazına gitmek için evden çıkan 7 yaşındaki Ömer Sevban Ergin'e otomobiliyle çarparak ölümüne neden olan Dilek A.'nın, yıllar önce benzer bir acı yaşadığı belirlendi., Kaza sonrası sinir krizi geçiren Dilek A.'nın, 2 yaşındaki çocuğunu trafik kazasında kaybettiği ortaya çıktı.,  ,  , Türkiye'den ve Dünya’dan son dakika haberler, köşe yazıları, magazinden siyasete, spordan seyahate bütün konuların tek adresi milliyet.com.tr; Milliyet.com.tr haber içerikleri kaynak gösterilmeden alıntı yapılamaz, kanuna aykırı ve izinsiz olarak kopyalanamaz, başka yerde yayınlanamaz., Türkiye’nin haber yaşam platformu Milliyet Dijital yenilendi!, Uygulama ile devam et, gündemi kaçırma!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+_x000D_
+İHA        
+ 30.03.2021 - 06:49
+, _x000D_
+    Yıldırım İlçesi Beyazıt mahallesinde meydana gelen olayda, kısıtlamanın son saatlerinde sokak arasında devriye atan bekçi ekipleri şüphelendikleri 16 P 7772 plakalı otomobile dur ihtarında bulundu. Dur ihtarına uymayan 16 P 7772 plakalı kadın sürücü Kıbrıs sokak üzerinde Yusuf K., isimli bekçiye çarparak olay yerinden hızlıca uzaklaştı. Olay yerine ihbar üzerine çok sayıda polis ekibi ve sağlık ekibi sevk edildi. Olay yerine gelen sağlık ekiplerinin ilk müdahalesinin ardından yaralı bekçi Yüksek İhtisas Eğitim ve Araştırma Hastanesine kaldırıldı. Bekçinin durumunun iyi olduğu öğrenildi. Polis ekipleri ise kaçan kadın sürücüyü bulmak için çalışma başlattı._x000D_
+, 
+_x000D_
+                        Markette dünürlerini taradı: Market sahibi öldü_x000D_
+, 
+_x000D_
+                        TÜBİTAK'ın İzmir Depremi araştırması_x000D_
+, 
+_x000D_
+                        SON DAKİKA HABERİ... MSB: 5 terörist etkisiz hale getirildi_x000D_
+, 
+_x000D_
+                        Aktarlarda şifalı 'kardeş kanı' diye satılan bitki öldürüyor_x000D_
+, 
+_x000D_
+                        ABD başkanlarına yazılan kayıp ‘sultan mektupları’_x000D_
+, 
+_x000D_
+                        Meteoroloji'den son dakika hava durumu uyarısı! Ankara, İstanbul ve İzmir'de hava nasıl olacak? İşte detaylar..._x000D_
+, Sayfa Yükleniyor..., _x000D_
+                            Web sitemizdeki çerezleri (cookie) kullanıcı deneyimini artıran teknik özellikleri desteklemek için kullanıyoruz._x000D_
+                            Aynı zamanda analitik çerezler de kullanıyoruz. Çerezleri reddetmek istiyorsanız detaylı bilgi için tıklayınız.
+</t>
+  </si>
+  <si>
+    <t>https://www.ntv.com.tr/turkiye/makas-atarak-carptigi-kadin-hafizasini-yitirdi-asli-kusurlu-surucu-serbest,fnY467PnrE2bRSxe1LbJ8g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+_x000D_
+DHA        
+ 04.01.2021 - 18:33
+, 
+, İstanbul Bakırköy'de sürücüsünün makas atarak çarptığı kadın hafızasını yitirdi. Asli kusurlu sürücünün serbest bırakılmasına yakınlarından tepki geldi. , Kaza, geçen 16 Ağustos'ta İncirli Caddesi'ndeki yaya geçidinde meydana geldi. İsmiye Aral, yolun karşı tarafına geçmek isterken, hızla gelen bir başka otomobili makas atarak sollayan sürücünün yönetimindeki otomobilin çarpması ile neye uğradığını şaşırdı., Ağır yaralanan kadın hastaneye kaldırıldı. 3 ay süreyle yoğun bakımda kalan kadın sağlık durumunun düzelmeye başlaması üzerine normal odaya alındı, ancak hafızasının yerinde olmadığı görüldü., 
+''İNSAN HAYATI BU KADAR UCUZ OLMAMALI''Annesinin yanından aylardan bu yana ayrılmayan çocuklarından Şanser Aral, bilirkişi raporunda sürücü Bilal Hıdır A'nın asli kusurlu görünmesine ve ortada kamera görüntüleri bulunmasına rağmen sürücü Bilal Hıdır A'nın kazadan hemen sonra serbest bırakılmasını kabul edemediklerini söyledi. Aral, "İnsan hayatı bu kadar ucuz olmamalı" dedi._x000D_
+, 
+_x000D_
+                        Markette dünürlerini taradı: Market sahibi öldü_x000D_
+, 
+_x000D_
+                        TÜBİTAK'ın İzmir Depremi araştırması_x000D_
+, 
+_x000D_
+                        SON DAKİKA HABERİ... MSB: 5 terörist etkisiz hale getirildi_x000D_
+, 
+_x000D_
+                        Aktarlarda şifalı 'kardeş kanı' diye satılan bitki öldürüyor_x000D_
+, 
+_x000D_
+                        ABD başkanlarına yazılan kayıp ‘sultan mektupları’_x000D_
+, 
+_x000D_
+                        Meteoroloji'den son dakika hava durumu uyarısı! Ankara, İstanbul ve İzmir'de hava nasıl olacak? İşte detaylar..._x000D_
+, Sayfa Yükleniyor..., _x000D_
+                            Web sitemizdeki çerezleri (cookie) kullanıcı deneyimini artıran teknik özellikleri desteklemek için kullanıyoruz._x000D_
+                            Aynı zamanda analitik çerezler de kullanıyoruz. Çerezleri reddetmek istiyorsanız detaylı bilgi için tıklayınız.
+</t>
+  </si>
+  <si>
+    <t>https://www.ntv.com.tr/video/turkiye/kadin-ve-erkek-surucu-birbirine-girdi,yrvEk8rumEe3etu0SkXq-g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+_x000D_
+_x000D_
+NTV                                
+ 15.09.2020 - 10:41
+| Son Güncelleme : 15.09.2020 - 12:11
+, 
+Tarihi Yarımada altında gizemli keşif
+, 
+Çay servisine giden patronu 20 günlük işçisi soydu
+, 
+İstanbul'da sağanak ve dolu
+, 
+4 ayrı suçtan aranıyordu foseptik çukurunda yakalandı
+, 
+Otomobil ile patpat böyle çarpıştı
+, 
+Pitbull saldırısında ağır yaralandı
+, 
+Marmara Denizi'ndeki müsilaj uçakla havadan görüntülendi
+, 
+Kendisini ağlatabilene 100 TL veriyor
+, 
+Gölde bulduğu yavru yunusu denizle buluşturdu
+, 
+Günün öne çıkan haberlerini 60 saniyede izleyin (11 Haziran 2021)
+, 
+NTV'ye Gazeteciler Cemiyeti ödülü
+, 
+İstanbul'da hamile eşini sokak ortasında dövdü
+, 
+Günün öne çıkan haberlerini 60 saniyede izleyin (10 Haziran 2021)
+, 
+Otel yangınında can pazarı
+, 
+Marmara'da müsilaj adası oluştu
+, _x000D_
+                            Web sitemizdeki çerezleri (cookie) kullanıcı deneyimini artıran teknik özellikleri desteklemek için kullanıyoruz._x000D_
+                            Aynı zamanda analitik çerezler de kullanıyoruz. Çerezleri reddetmek istiyorsanız detaylı bilgi için tıklayınız.
+</t>
+  </si>
+  <si>
+    <t>https://www.posta.com.tr/kadin-surucu-aracini-tekmeleyen-saldirgani-kaputun-uzerinde-polis-merkezine-goturdu-2278203</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bursa'nın Orhangazi ilçesinde bir kadın sürücü, otomobiline saldırıp ön camını tekmeleyen genci kaputun üzerinde emniyete götürdü. Gencin ön kaput üzerindeki tehlikeli yolculuğu MOBESE kameraları tarafından anbean görüntülendi., , , , İlginç olay Orhangazi İznik karayolunda yaşandı. İddiaya göre, 2 çocuk annesi olan Yasemin Erdem kendisine ait 16 AGY 414 plakalı otomobili ile Orhangazi’ye bağlı Üreğil köyünden Orhangazi şehir merkezine gelmek için yola çıktı. Güzergah üzerinde önüne aniden çıkan bir köpeğe çarpmamak için yavaşlayan Yasemin Erdem köpeğin geçmesinden sonra yoluna devam etti. Yasemin Erdem’in son anda çarpmaktan kurtulduğu köpeğe karşı yönden gelen ve Osman T.(20) idaresindeki bir başka otomobil çarptı. Olaydan Yasemin Erdem'i sorumlu tutan Osman T. içerisinde 3 erkek ve 1 kadının bulunduğu otomobili ile Yasemin Erdem'in peşine düştü. Erdem'in kullandığı otomobili uzun süre takip eden Osman T., Orhangazi-İznik yolu otoban köprüsü altındaki trafik ışıklarında önünü kesti., , Camları ve arabayı tekmeleyip yumruklayan Osman T. aracın kaputuna çıktı. Can havli ile aracı hareket ettiren Yasemin Erdem, 20 yaşındaki genç adamı kaputun üzerinde 2 kilometre ilerideki Emniyet Müdürlüğü önüne kadar götürdü. Polisin müdahale ettiği olay sonrasında hakarete de uğrayan Yasemin Erdem şahıslardan şikayetçi oldu. Polis, Osman T., Mustafa T ve Mahmut T.’yi emniyet müdürlüğü binası içine aldı. Burada ifadeleri alınan şahıslar serbest kalırken, Yasemin Erdem şikayetçi oldu., , Osman T.'nin kaput üzerinde yaptığı 2 kilometrelik yolculuk ilçenin MOBESE kameraları tarafından saniye saniye görüntülendi. Kaput üzerinde arabanın camını tekmeleyen Osman T.'nin bir taraftan da düşmemek için gösterdiği çaba paniğe kapılan Yasemin Erdem'in bir an önce emniyete gitmek için aracını ters yönden sürmesi anbean kaydedildi., Olayın şokunu uzun süre üzerinden atamayan Yasemin Erdem yaşadıklarını anlattı. Olay gecesi kendisi, küçük kızı, kendi kız kardeşi ve onun oğlu ile Üreğil Mahallesinden Orhangazi’ye doğru gelirken, önüne bir köpek çıktığını, köpeğe çarpmamak için yavaşladığını belirterek, "Bir süre aracımla ilerledikten sonra önüme aniden bir araç çıktı ve yolumu kesti. Araçtan 3 erkek şahıs indi. Aracımı tekmelemeye ve yumruklamaya başladılar. Büyük korku yaşadık. O esnada daha sonra isminin Osman olduğunu öğrendiğim şahıs arabamın kaputuna çıktı. Aynı anda aracımın önü de açılınca ben hareket ettim. Olay yerinden yaklaşık 2 kilometre ileride şehir merkezi girişinde trafik lambalarına kadar geldik. Yolda hareket ederken olabildiğince yavaş gittim ki kaputtaki genç düşsün istemedim. Trafik lambalarında kırmızı ışıktayken daha önce önümü kesen otomobil gelip kavşakta bana çarparak tekrar önümü kesti dedi. Yeşil ışığın yanması ile yeniden hareket ettiğini belirten Yasemin Erdem o şekilde şehir içinden kornaya basarak Emniyet Müdürlüğü önüne kadar gittim. Polisler de büyük şaşkınlık yaşadı. Şahsı alıp emniyet binasına soktular. Daha sonra kendilerinden şikayetçi oldum dedi. Yasemin Erdem yaşadığı olayın şokunu bir türlü üzerinden atamadığını da belirterek, çocuklarım hala o akşamki felaketi yaşıyorlar. Şu anda davamız devam ediyor. Hepsinden davacıyım" dedi., , </t>
+  </si>
+  <si>
+    <t>_x000D_
+                                    Adana'da, Songül Dalmızrak (23), lüks cipiyle seyir halindeyken elektrikli bisikletiyle yolun karşısına geçmeye çalışan Songül Yiğit?e çarptı. Çarpmanın etkisiyle yola savrulan Yiğit, ambulansla hastaneye kaldırıldı. Dalmızrak ise kazanın şokunu uzun süre atlatamadı._x000D_
+                                , Kaza, dün saat 12.00 sıralarında merkez Seyhan ilçesine bağlı Tellidere Mahallesi'nde meydana geldi. İddiaya göre, Songül Dalmızrak (23) yönetimindeki 01 DLP 67 plakalı lüks cip, cadde üzerinde ilerlerken, yolun karşısına geçmek isteyen Songül Yiğit (39) idaresindeki elektrikli bisiklete çarptı. Çarpmanın etkisiyle Yiğit yola savruldu. Kaza anları, bölgede bulunan bir güvenlik kamerasına yansıdı. Kazanın ardından aracını durduran Dalmızrak, yaralanan kadının yanına koşarak yardım etti. Dalmızrak'ın bildirmesi üzerine olay yerine polis ve sağlık ekipleri sevk edildi. Bölgeye gelen sağlık görevlileri, ilk müdahalesinin ardından Yiğit'i ambulansla hastaneye götürdü. Dalmızrak ise cipini ara sokağa çekip yeniden olay yerine gelirken, kazanın şokunu uzun süre atlatamadı. Kaza yerine gelen yakınlarına sarılıp gözyaşlarına boğulan genç kadın ise uzun süre sakinleştirilemedi.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_x000D_
+                                    Bursa'da hatalı park nedeniyle otomobili otoparka çekilen kadın sürücü, polislere hakaret edip, otomobiline binerek kaçmaya çalıştı. O anlar cep telefonu kamerasına yansırken, polis ekipleri kadından şikayetçi oldu._x000D_
+                                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">_x000D_
+                                    İstanbul Bahçeşehir’de otomobilini park etmek isteyen bir kadın sürücü, iddiaya göre fren ile gazın yerini karıştırınca dükkanın içine girdi. O esnada dükkanın boş olması olası bir faciayı önledi._x000D_
+                                </t>
+  </si>
+  <si>
+    <t>https://www.sabah.com.tr/video/yasam/uskudarda-yokus-asagi-inen-kadin-surucu-otomobiliyle-takla-atti-video</t>
+  </si>
+  <si>
+    <t>_x000D_
+                                    Üsküdar’da otomobilinin direksiyon hakimiyetini kaybeden kadın sürücü bir evin bahçe duvarına çarptıktan sonra takla attı. Kaza anında sokak üzerinde kimsenin olmaması olası bir faciayı önlerken, kazada yaralanan kadın sürücü hastaneye kaldırıldı._x000D_
+                                , Kaza, Üsküdar Altunizade Mahallesi Gonca Sokak'ta saat 12.30 sıralarında meydana geldi. Edinilen bilgiye göre, sokak üzerinde yokuş aşağı seyir halinde olan 34 DL 7552 plakalı araç sürücüsü F.K. isimli kadın şahıs, hız nedeniyle direksiyon hakimiyetini kaybetti. Aracının kontrolünü sağlayamayan F.K. yol kenarında bulunan bir eve ait bahçenin duvarına çarptıktan sonra aracıyla takla attı., Olayı gören çevredeki vatandaşlar durumu polis ve sağlık ekiplerine bildirdi. Adrese gelen sağlık ekipleri yaralı kadını çevredeki en yakın hastaneye kaldırırken, polis ekipleri ise olay yerinde incelemelerde bulundu., Kaza esnasında olay yerinde olan vatandaş Mehmet Bayındır, "Olay sabah saatlerinde oldu. Kazanın sesini duyduk. Duvarı çarpmasıyla araç aniden ters döndü. Ekipler, kadın sürücüyü araçtan çıkardıktan sonra tedbir amaçlı hastaneye götürdüler. Kadının sağlık durumunun iyi olduğu söylendi" diye konuştu.</t>
+  </si>
+  <si>
+    <t>https://www.sabah.com.tr/yasam/2019/06/03/ehliyetsiz-kadin-surucu-kaldirimdaki-2-yasli-kadini-boyle-ezdi</t>
+  </si>
+  <si>
+    <t>Edinilen bilgiye göre, kaza, merkez Yüreğir ilçesi, Selahattin Eyyubi Mahallesinde meydana geldi. İddiaya göre S.K. isimli kadın direksiyon eğitimi için erkek arkadaşının hafif ticari aracını kullanmak istedi. S.K. bir süre aracı arkadaşı yanındayken sürmeye devam etti. Ancak S.K. heyecanlanıp fren yerine gaza basınca direksiyon hakimiyetini kaybedip kaldırımda oturan akraba olan Münevver Can (74) ve Raziye Can'a (74) çarpıp park halindeki araca sıkıştırdı. Kaza sonrası çevredeki vatandaşlar hemen yardıma koştu. Kadın sürücü şok olmuş halde araçtan inerken bir kişi ise arabaya binip aracı geri alarak kadınları sıkıştığı yerden kurtardı. Kadın sürücü ise çarptığı kadınlara bakıp fenalık geçirdi. Bu anlar ise güvenlik kamerası tarafından saniye saniye görüntülendi., Ehliyetsiz kadın sürücü, kaldırımdaki 2 yaşlı kadını böyle ezdi, Bu arada vatandaşlar polise ve sağlık ekiplerine haber verdi. Olay yerine gelen ambulanslarla iki kadın hastaneye kaldırıldı ancak tüm müdahalelere rağmen kurtarılamadı. Olay yerine gelen polis de kadın ve erkek arkadaşını polis merkezine götürdü. Burada kadının ehliyetsiz olduğu ortaya çıkarken, erkek şahıs aracı kendisinin kullandığını söyledi ancak güvenlik kamera kayıtlarından aracı kadının kullandığı tespit edildi. Kadın sürücü iki kişiyi öldürmekten sevk edildiği adliyede nöbetçi sulh ceza hakimliği tarafından tutuklandı. İki kadın ise yakınları tarafından toprağa verildi._x000D_
+Münevver Can'ın eşi İbrahim Can eşinin ve bir akrabasının kaldırımda otururken bir hiç yüzünden hayatını kaybettiğini, aracının sahibinin kapı komşuları olduğunu ancak şikayetçi olduğunu söyledi.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kaza, merkez Seyhan ilçesine bağlı Pınar Mahallesi Mavi Bulvar'da meydana geldi. Pınar Harman (27) yönetimindeki 01 DHJ 27 plakalı otomobil, virajda kontrolde çıkarak yol kenarındaki ağaca çarpıp sulama kanalına uçtu., , İçerisinde su bulunmayan kanala düşen otomobili görenler, polis, itfaiye ve sağlık ekiplerine haber verdi. Bölgeye sevk edilen itfaiye ekipleri, araçta sıkışan Pınar Harman'ı kurtardı. İlk müdahalesi kaza yerinde yapılan Pınar Harman, kanala sarkıtılan halat merdivenle çıkarıldı. Harman'ın bu sırada şoka girdiği ve ellerinin titrediği görüldü. Harman, ambulansla hastaneye götürülerek tedaviye alındı., 
+_x000D_
+Kazayı görünce yardıma koşan sürücü Şehmus Çelik (45), "Önce bir ses duyduk. Ardından kanala bir otomobilin düştüğünü gördük. Hemen aracımı sağa çekip, yanına gittim. Kadın sıkışmıştı. İtfaiye ekipleriyle birlikte çıkardık. Yüzünü falan yıkadık ama baygındı" dedi., </t>
+  </si>
+  <si>
+    <t>Susurluk'ta Kürse kavşağında 10 DP 185 plakalı otomobiliyle seyir halinde olan Melis B. (29) otomobilin direksiyon hakimiyetini kaybetti. Kontrolden çıkarak şarampole devrilen otomobil hurdaya döndü. Kazayı gören diğer sürücülerin ihbarı üzerine olay yerine Jandarma ve Sağlık ekipleri sevk edildi. Sağlık ekipleri, hurda yığınına dönen araç içerisindeki Melis B. Ye müdahale etti ancak talihsiz kadının hayatını kaybettiğini belirledi. Melis B.'nin cansız bedeni, Susurluk Devlet Hastanesi morguna gönderildi.</t>
+  </si>
+  <si>
+    <t>https://www.sabah.com.tr/yasam/2021/06/12/yok-boyle-aci-kadin-surucu-minik-duruyu-ezdi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antalya'da halası Rukiye Akça ile birlikte yaya geçidinden yolun karşısına geçmeye çalışan Duru Akça'ya otomobilin çarpması sonucu feci şekilde can veri. Korkunç kazanın ardından Duru'ya çarpan kadın sürücü gözaltına alındı. Feci kaza Muratpaşa ilçesi Rauf Denktaş Bulvarı'nda meydana geldi. Ermenek Mahallesi Kuleli Sokak'ta oturan Akça ailesinin minik kızları Duru, halası Rukiye Akça ile birlikte Kuran dersinde aldığı karne hediyesi markete dondurma ve oyuncak almaya gitti., , YAYA GEÇİNDE ÇARPTI, Rauf Denktaş Bulvarı'nda hala yeğen birlikte yaya geçidinden karşıya yürümeye başladı. Bu sırada 2 araç durdu. Arkadan gelen bayan sürücünün kullandığı otomobil durmayarak Duru Akça'ya feci şekilde çarptı. Hala Rukiye Akça kanlar içinde kalan yeğenini görünce çığlık atmaya başladı. Olay yerine gelen sağlık ekipleri tarafından hastaneye kaldırılan Duru Akça yapılan tüm müdahalelere rağmen kurtarılamadı., , GÖZYAŞLARINA BOĞULDU, Korkunç kazanın ardından kızlarını öldüğünü öğrenen baba Ali, anne Teslime Akça gözyaşlarına boğuldu. Cenaze otopsi için Adli Tıp Kurumu morguna kaldırıldı. Akça ailesi kızlarının ölümüne sebep olan kadın sürücüden şikayetçi ve davacı oldu. Sürücünü kızlarına yaya geçidinde çarptığını belirten Akça ailesi, "İki araç duruyor. Bizim kızımıza çarpan lüks araç ise süratle gelip çarpıyor. Bu kaza değil resmen cinayet" diyerek tepkilerini dile getirdiler., , KURAN KARNESİ ALMIŞTI, Hala Rukiye Akça, iki kardeş Deniz ve Duru camideki yaz Kur'an Kursu'na gidiyorlardı. Dün ikisi de Takdir alıp geldiler. Bizde ödül olarak makete oyuncak ve dondurma almaya gidiyorduk. Kadın sürücü gelip çarptı. Akı alır gibi değil. İki araç durdu. O durmadı" diyerek tepkilerini dile getirdi. Duru'dan geriye kazadan 35 dakika önce çekilmiş resmi kaldı., , ABLASI DENİZ, 'DURU MELEK OLUP GELECEK', Korkunç kaza Duru ile kendisinden bir yaş küçük olan Deniz'i ayırdı. Kardeşini kaza geçirdiğini öğrenen Deniz'in, "Duru melek oldu. Ölen amcamı görüp geri gelecek" demesi herkesi ağlattı., , EVLADA SON BAKIŞ, Duru Akça'nın cenazesi Adli Tıp Kurumu morgundan alınışı sırasında anne teslime ve hala Rukiye Akça'nın çığlıkları yürükleri parçaladı. Gözyaşlarına boğulan anne ve hala, "Duru bizleri bırakıp ta nerelere gidiyorsun meleğim" sözleri herkesi ağlattı. Duru'nun cansız bedeni Ermenek Mezarlığı'nda gözyaşları içinde toprağa verildi., , KADIN SÜRÜCÜ ADLİYEYE SEVK EDİLDİ, Öte yandan Duru Akça'nnı ölümüne neden olan kadın sürücü Berna Y.B. karakoldaki ifadesinin ardından adliyeye sevk edildi. Kadın sürücünün kullandığı aracın plakasının polis tarafından sır gibi saklaması dikkat çekti.,  </t>
+  </si>
+  <si>
+    <t>Aydın'ın Sultanhisar ilçesine bağlı Atça Mahallesinde Perşembe günü meydana gelen trafik kazasında karşı şeride geçerek karşıdan gelen kamyonete çarpan otomobil sürücüsü hayatını kaybetti.
+, Kaza, Sultanhisar ilçesine bağlı Atça Mahallesi Marla Restoran yakınlarında Perşembe günü 19.30 sıralarında meydana geldi. Alınan bilgilere göre,  Aydın'dan  Nazilli istikametine doğru seyir halinde olan 35 AKP 874 plakalı otomobil sürücüsü 38 yaşındaki Sergül Kaya, yağmurun başladığı saatlerde bilinmeyen bir nedenden dolayı aracının direksiyon hakimiyetini kaybetti. Orta refüjü aşarak karşı şeride geçen otomobil, Nazilli istikametinden gelen Mutlu D. (42) idaresindeki 09 ADJ 14 plakalı kamyonetle çarpıştı. Çarpışma sonunda talihsiz kullandığı otomobilde büyük hasar oluştu. Diğer sürücülerin ihbarı üzerine olay yerine çok sayıda 112 acil sağlık, polis ve 110 AKS ekibi sevk edildi. Kazada otomobili kullanan sürücü Sergül Kaya olay yerinde hayatını kaybettiği belirlenirken, kamyonet sürücü Mutlu D. İse ilk müdahalesinin ardından Nazilli Devlet Hastanesi’ne kaldırıldı., 112 acil sağlık ekiplerinin kazada yerinde yaptığı ilk müdahalede kazada hayatını kaybeden talihsiz kadının hamile olduğunu söylemesi üzerine tutanaklara geçilen bilginin basına yansıması üzerine ağabey İbrahim Kaya, çıkan haberlerin gerçek olmadığı söyledi. Kardeşinin hamile olmadığının ön otopside meydana çıktığını ifade eden acılı ağabey Kaya, “Akşam saatlerinde acı haberi öğrendik, çok üzüldük. İzmir’de bir fabrikada çalışıyordu. Anne babamız Nazilli’de yaşıyor, onun yanlarına geliyordu. 112 Acil Sağlık Ekibi kaza yerine gelince hamile diye geçmiş. Kardeşimin hamile olması mümkün değil. Çünkü 2 sene önce eşinden ayrıldı. 18 yaşında bir kızı ve 11 yaşında bir oğlu var. Zaten öldüğüne üzüldük, birde bu haberi de göründe annem babam ve çocukları çok üzüldü. Ön otopside hamile olmadığı ortaya çıktı. 112 Ekibi sadece gözlem yaparak hamile demişler ve basındaki arkadaşlarda bu ifadeyle haberi böyle yazmışlar. Haberin düzeltilmesini ve kamuoyunun yanlış algıya düşmemesi için bu şekilde bilgilendirilmesini istiyoruz” ifadelerini kullandı., 
+30 Nis 2020 - 19:58
+Aydin-
+Asayiş
+Yazdır
+, Muhabir Metin Can, Yorumunuz yarım kaldı, devam etmek için üstteki yoruma, silmek için buraya tıklayın, Kırmızı alanlar eksik veya hatalı girildi. Lütfen bu alanları düzeltip tekrar gönderelim, Yorumunuz için teşekkürler, en kısa sürede gözden geçirilip yayınlanacaktır, Yorum yazarak Aydın Ses Gazetesi Topluluk Kuralları’nı kabul etmiş bulunuyor ve yorumunuzla ilgili doğrudan veya dolaylı tüm sorumluluğu tek başınıza üstleniyorsunuz. Yazılan yorumlardan Aydın Ses Gazetesi hiçbir şekilde sorumlu tutulamaz., Anadolu Ajansı (AA), İhlas Haber Ajansı (İHA), Demirören Haber Ajansı (DHA) tarafından servis edilen tüm haberler Aydın Ses Gazetesi editörlerinin hiçbir editöryel müdahalesi olmadan, ajans kanallarından geldiği şekliyle yayınlanmaktadır. Sitemize ajanslar üzerinden aktarılan haberlerin hukuki muhatabı Aydın Ses Gazetesi değil haberi geçen ajanstır., Şimdi oturum açın, her yorumda isim ve e.posta yazma zahmetinden kurtulun. Oturum açmak için bir hesabınız yoksa, oluşturmak için buraya tıklayın.
+, Yorum yazarak  Aydın Ses Gazetesi Topluluk Kuralları’nı kabul etmiş bulunuyor ve yorumunuzla ilgili doğrudan veya dolaylı tüm sorumluluğu tek başınıza üstleniyorsunuz. Yazılan yorumlardan Aydın Ses Gazetesi hiçbir şekilde sorumlu tutulamaz., Anadolu Ajansı (AA), İhlas Haber Ajansı (İHA), Demirören Haber Ajansı (DHA) tarafından servis edilen tüm haberler Aydın Ses Gazetesi editörlerinin hiçbir editöryel müdahalesi olmadan, ajans kanallarından geldiği şekliyle yayınlanmaktadır. Sitemize ajanslar üzerinden aktarılan haberlerin hukuki muhatabı Aydın Ses Gazetesi değil haberi geçen ajanstır., Aydın Ses Gazetesi, Aydin ile özdeşleşen markaları ağırlıyor., +90 (256) 213 16 50  Reklam bilgi, 
+©Copyright 2021 Aydın Ses Gazetesi Tüm Hakları Saklıdır
+-
+Veri PolitikasıKullanım Şartları
++90 (256) 213 16 50
+,  Veri politikasındaki amaçlarla sınırlı ve mevzuata uygun şekilde çerez konumlandırmaktayız. Detaylar için veri politikamızı inceleyebilirsiniz.</t>
+  </si>
+  <si>
+    <t>https://www.sesgazetesi.com.tr/haber/5168802/aydinda-feci-kaza-kadin-surucu-hayatini-kaybetti</t>
+  </si>
+  <si>
+    <t>Aydın’ın Efeler ilçesinde kanala uçarak suya gömülen araçla birlikte sudan çıkartılan Ayşegül Aydın, kaldırıldığı hastanede hayatını kaybetti.
+, Olay, Hayvan Pazarı yakınlarında meydana geldi. Ayşegül  Aydın, kullandığı 09 LZ 900 plakalı hafif ticari aracının direksiyon hakimiyetini kaybetti. Kontrolden çıkan araç, demir telleri yıkarak kanala uçtu. Aracın kanala uçtuğunu gören çevredeki vatandaşlar durumu jandarma ve itfaiye ekiplerine bildirdi. Olay yerine gelen itfaiye ekipleri kurtarma çalışmalarına başladı. Suya gömülen araç, vinç yardımıyla sudan çıkartılırken aracın içerisinde bulunan kadın sürücü, ambulansla Aydın Devlet Hastanesi’ne kaldırıldı. Aydın, burada yapılan tüm müdahaleye rağmen kurtarılamadı. Kazayla ilgili soruşturma başlatıldı., 
+01 Eyl 2020 - 16:40
+Aydin-
+Asayiş
+Yazdır
+, Muhabir Kazım Yörükce, Yorumunuz yarım kaldı, devam etmek için üstteki yoruma, silmek için buraya tıklayın, Kırmızı alanlar eksik veya hatalı girildi. Lütfen bu alanları düzeltip tekrar gönderelim, Yorumunuz için teşekkürler, en kısa sürede gözden geçirilip yayınlanacaktır, Yorum yazarak Aydın Ses Gazetesi Topluluk Kuralları’nı kabul etmiş bulunuyor ve yorumunuzla ilgili doğrudan veya dolaylı tüm sorumluluğu tek başınıza üstleniyorsunuz. Yazılan yorumlardan Aydın Ses Gazetesi hiçbir şekilde sorumlu tutulamaz., Anadolu Ajansı (AA), İhlas Haber Ajansı (İHA), Demirören Haber Ajansı (DHA) tarafından servis edilen tüm haberler Aydın Ses Gazetesi editörlerinin hiçbir editöryel müdahalesi olmadan, ajans kanallarından geldiği şekliyle yayınlanmaktadır. Sitemize ajanslar üzerinden aktarılan haberlerin hukuki muhatabı Aydın Ses Gazetesi değil haberi geçen ajanstır., Şimdi oturum açın, her yorumda isim ve e.posta yazma zahmetinden kurtulun. Oturum açmak için bir hesabınız yoksa, oluşturmak için buraya tıklayın.
+, Yorum yazarak  Aydın Ses Gazetesi Topluluk Kuralları’nı kabul etmiş bulunuyor ve yorumunuzla ilgili doğrudan veya dolaylı tüm sorumluluğu tek başınıza üstleniyorsunuz. Yazılan yorumlardan Aydın Ses Gazetesi hiçbir şekilde sorumlu tutulamaz., Anadolu Ajansı (AA), İhlas Haber Ajansı (İHA), Demirören Haber Ajansı (DHA) tarafından servis edilen tüm haberler Aydın Ses Gazetesi editörlerinin hiçbir editöryel müdahalesi olmadan, ajans kanallarından geldiği şekliyle yayınlanmaktadır. Sitemize ajanslar üzerinden aktarılan haberlerin hukuki muhatabı Aydın Ses Gazetesi değil haberi geçen ajanstır., Aydın Ses Gazetesi, Aydin ile özdeşleşen markaları ağırlıyor., +90 (256) 213 16 50  Reklam bilgi, 
+©Copyright 2021 Aydın Ses Gazetesi Tüm Hakları Saklıdır
+-
+Veri PolitikasıKullanım Şartları
++90 (256) 213 16 50
+,  Veri politikasındaki amaçlarla sınırlı ve mevzuata uygun şekilde çerez konumlandırmaktayız. Detaylar için veri politikamızı inceleyebilirsiniz.</t>
+  </si>
+  <si>
+    <t>https://www.sondakika.com/haber/haber-antalya-da-2-kadin-surucu-trafikte-sac-saca-kavga-14197493/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Antalya'da 2 kadın sürücü, araçlarını durdurup yol ortasında saç saça kavga etti., Öfkeli kadınları erkek sürücüler ayırırken, o anlar cep telefonu kamerasına saniye saniye yansıdı., Antalya'nın Muratpaşa ilçesi 12'nci cadde üzerinde ve yoğun trafikte 2 kadın sürücü kavgaya tutuştu. Aracından inen kadın, diğer kadını önce otomobilinden inmesine fırsat vermemek için kapıyla sıkıştırmaya çalıştı. Kendini kapı engelinden kurtaran kadın, diğer kadın sürücünün üzerine atladı. İki kadın saç saça kavga edip yerde yuvarlandı., , Kadın sürücülerin kavgasını, araçlarını durdurup kavgaya koşan erkek sürücüler ayırdı. Kadın sürücüleri ayırmak oldukça zor olurken, o anlar bir sürücünün cep telefonu kamerasına saniye saniye yansıdı.,  Muratpaşa, Antalya, kavga, Güncel, Son Dakika ,  Kaynak: DHA ,  Son Dakika › Güncel › ANTALYA'DA 2 KADIN SÜRÜCÜ TRAFİKTE SAÇ SAÇA KAVGA ETTİ - Son Dakika , Sondakika.com'un size anlık bildirim göndermesine izin veriyor musunuz?</t>
+  </si>
+  <si>
+    <t>https://www.sondakika.com/haber/haber-diyarbakir-da-kadin-surucu-baska-arac-tarafindan-13387124/</t>
+  </si>
+  <si>
+    <t>Diyarbakır- Şanlıurfa karayolunda kadın sürücünün kullandığı aracın arkadan gelen bir başka araç tarafından sıkıştırılması sonrası yaşanan trafik kazası güvenlik kamerasına an be an yansıdı. Kazada kadın sürücü ağır olmak üzere yanındaki çocuk da yaralandı., Kaza, Diyarbakır-Şanlıurfa karayolu 3. kilometrede meydana geldi. İddiaya göre, plakası belli olmayan bir otomobil kadın sürücünün kullandığı 07 N 8014 plakalı otomobili yolda sıkıştırdı. İsmi öğrenilemeyen kadın sürücü direksiyon hakimiyetini kaybederek refüjdeki direğe çarparak yola savruldu. Bu sırada yolda seyir halinde olan 21 DF 454 otomobil de kaza yapan otomobile arkadan çarptı. Kazada kadın sürücü ağır yaralanırken yanındaki çocuk ise hafif yaralandı. Yoldan geçen sürücülerin durumu bildirmesi üzerine olay yerine çok sayıda ambulans ve polis ekipleri sevk edildi. Sağlık ekipleri yaralılara yaptığı ilk müdahalenin ardından çevredeki özel hastaneye kaldırdı. Çevrede inceleme yapan polisler gidiş ve geliş olarak bölünen karayolunun tek şeridini bir süreliğine kapatarak kontrollü olarak araç geçişini sağladı. Polis, kazaya karışan otomobilleri bölgeye çağırdıkları çekicilerle kaldırdı. Kaza yerinin temizlenmesinin ardından yol trafiğe tekrardan açıldı., , Kazada yaralanan kadın sürücünün durumu ciddiyetini korurken yaşanan kaza anı ise an be an güvenlik kamerasına yansıdı. Polis kaza ile ilgili inceleme başlattı. - DİYARBAKIR,  Diyarbakır, Şanlıurfa, 3. Sayfa, Son Dakika ,  Kaynak: İHA ,  Son Dakika › 3. Sayfa › Diyarbakır'da kadın sürücü başka araç tarafından sıkıştırıldı: 2 yaralı - Son Dakika , Sondakika.com'un size anlık bildirim göndermesine izin veriyor musunuz?</t>
+  </si>
+  <si>
+    <t>Beylikdüzü ve Esenyurt mevkilerinde E-5 yanında usta bir şoförle araç kullanan 68 yaşındaki kadın sürücü Şakire Asaroğlu, aracının arkasına “Acemi bayan şoför, lütfen korna basmayınız” yazılı pankart astı., Yolda giden diğer sürücüler durum karşısında şaşkınlıklarını gizleyemezken, Asaroğlu'nun bu yaptığının ise işe yaradığı gözlendi., Kendinin 1995 yılından bu yana ehliyet sahibi olduğunu ifade eden Şakire Asaroğlu, “ Bana dikkat etsinler yaşım var çocuğum yaşıma hürmet etsinler. Şu anda 1 ay oldu. 1 aydır böyle araba kullanıyorum. Ehliyetim 1995 yılından bu yana var ihtiyaç oldu yürüyemiyorum. Yaşlanınca daha çok ihtiyacım oldu araca. Şimdi hastaneden geliyorum” dedi. İHA</t>
+  </si>
+  <si>
+    <t>Kaza, 09 Haziran pazar günü sabah saat 05.30 sıralarında Merkez Mezitli İlçesi Menderes Mahallesi GMK Bulvarı üzerindeki yer alan yaya geçidinde meydana geldi., Aynı mahallede annesi Gülsen Kahramanoğlu ile yaşayan 48 yaşındaki Arzu Kahramanoğlu, her zaman olduğu gibi sabah erken saatte kalkarak spor yapmak üzere deniz sahiline gitmek istedi., Genç kadına, GMK Bulvarı üzerinde yer alan yaya geçidinden karşıya geçtiği sırada, aşırı süratli ve alkollü olduğu belirlenen Zeynep Kocadağ'ın kullandığı 33 AAB 882 plakalı araç çarptı. Kazada ağır yaralanarak olay yerine gelen ambulansla Mersin Üniversitesi Tıp Fakültesi Hastanesi'ne kaldırılan Arzu Kahramanoğlu, tedavi alındıktan yaklaşık iki saat sonra yaşamını yitirdi., Kazadan hemen sonra olay yerine ulaşan trafik ekipleri sürücü Zeynep Kocadağ'ı gözaltına altı. Yapılan kontrolde yüzde 60 promil alkollü çıkan Zeynep Kocadağ, aynı gün çıkarıldığı nöbetçi mahkemece ‘Taksirle ölüme neden olma, alkollü ve tehlikeli araç kullanma' suçundan tutuklandı. Kazadan yara almadan kurtulan Kocadağ'ın verdiği ilk ifadesinde, yaya geçidinden geçmeye çalışan bayanı fark ettiğini, geçeceğini düşündüğü için yola devam etmek istediğini, kazanın nasıl olduğunu bilmediği yönünde ifade verdiği belirlendi., Yıllarca görev yaptığı Posta İşletme Müdürlüğü'nde ve çevresinde son derece sevilen ve yardım severliği ile tanınan Arzu Kahramanoğlu'nun yaşamını yitirmesi ailesini, yakınlarını ve mesai arkadaşlarını yasa boğdu. Genç kadın, doğum günü olan 10 Haziran'da Mezitli Mezarlığı'nda gözyaşları arasında sonsuzluğa uğurlandı., Meydana gelen trafik kazasında alkollü sürücün kurbanı olan kızı Arzu Kahramanoğlu'nun yaşamını yitirmesiyle yıkılan anne Gülsen Kahramanoğlu, ancak iğnelerle sakinleştiriliyor. Acılı annenin yaklaşık 15 yıl önce de 18 yaşındaki oğlu Tümer'i, Antalya'da yolun karşısına geçerken bir trafik kazasında kaybettiği belirlendi.</t>
+  </si>
+  <si>
+    <t>Kadıköy D-100 Karayolu Kozyatağı mevkiinde aracıyla ilerleyen bir kadın sürücü, içi yolcu dolu olan otobüsün kendisini yolda sıkıştırdığını iddia ederek otobüsü takip etmeye başladı. Otobüsü kilometrelerce takip eden sürücü, bir kaç kez otomobiliyle otobüsün önünü kesip yolu kapattı., Aracından inen kadın otobüs şoförüyle tartışmaya başladı. Otobüs şoförünün, üzerine otobüsü sürdüğünü iddia eden kadın polis ekiplerini de aradı. Otobüsteki yolcular ise kadına tepki gösterirken, otobüs şoförüne destek oldu., İETT otobüsünün canına kast ettiğini ifade eden kadın sürücü kilometrelerce takip edip defalarca otobüsün önünü kesti. Foto: DHA, Otobüs şoförü ise aracıda kamera kayıtları bulunduğunu ve yolcuların yaşananlara şahit olduklarını belirtti. Hastane randevusuna geç kaldığını ifade eden bir kadın yolcu ise, “Ben şoförün yerinde olsam seni döverdim. Şoför beyefendi biriymiş” dedi. (DHA)</t>
+  </si>
+  <si>
+    <t>Olay, dün saat 18.00 sıralarında Çekmeköy ilçesi Mimar Sinan Mahallesi Mimar Sinan Caddesi üzerinde yaşandı. Bankada işlemini yapmak için aracını banka önüne park eden Arzu E., kısa süre içerisinde işlemini tamamlayıp aracına bindiğinde arkasında bir başka aracın olduğunu görünce sürücüden aracını çekmesini istedi. Arzu E.’nin iddiasına göre deliye dönen kadın sürücü, hakaretler ederek yanına gittiği Arzu E.’nin kapısına vurmaya başladı. İddiaya göre konuşmak için camı  açan Arzu E.’ye saldıran kadın çevredeki vatandaşlar tarafından uzaklaştırıldı., ÇEVREDEKİLERİN YARDIMIYLA UZAKLAŞTIRILDI, Olayın ardından darp raporu alan Arzu E., en yakın polis karakoluna giderek şikayetçi oldu.Arzu E., “Bugün hayatımda ilk kez televizyonda izlediğim gibi bir olayla karşı karşıya geldim. Bir kadın trafik magandasıyla maalesef çok kötü bir  olay yaşadım. Yaşadığım ilçede her zaman gittiğim bankanın ATM'sinden para çekmek üzere arabamı park ettim., “SAÇIMI ÇEKEREK BENİ DIŞARI ÇIKARMAK İSTEDİ”, Parayı çektikten sonra da park yerinden çıkmam ve yoluma devam etmem gerekiyor. Çıkabilmem için de yoldaki mevcut araçların bana yol vermesi gerekiyor. Burada böyle bir sistem var fakat ben bunu bugün sağlayamadım. Orada birkaç çocuğun yardımıyla arkadaki aracın bana yol vermesi için ‘Söyler misiniz, iletir misiniz, ben arabamı çıkartayım’ dedim. Hiçbir şey duyulmamış, rica edilmemiş gibi arkadaki aracın sahibi sonradan öğrendim ki bir kadın, arabasını durdurmadığı  gibi üzerime doğru sürdü ve benim arabamı park yerinden çıkmaması için zorlayıcı bir harekette bulundu. Bu zorlayıcı hareketin üzerine ‘Bana yol vermeniz gerekmiyor mu? Biraz geri alır mısınız, çıkmam gerekiyor., ‘Çünkü o bölgede bana yol verilecek ki arkadaki araçlar da trafiğe kalmadan ışıktan geçebilsin, böyle bir durum. Fakat kendisi bana yol vermediği gibi arabasını yolun ortasında durdurdu, arabasından çıktı ve benim arabamı tekmelemeye başladı. Sanki kendisi haklı ben haksızmışım gibi arabamın camı da onunla diyalog kurmak istediğim için açıktı, bundan faydalanıp benim kolumu, saçlarımı çekerek beni arabamın dışarısına almaya çalıştı. Burada bir kadın beni feci şekilde darp etti, sadece bana değil aracıma da zarar verdi” dedi., ‘ERKEKLERE BU KADAR İFTİRA ATILMASINI ARTIK HOŞ GÖRMÜYORUM’, Yaşadığı olayı anlatırken gözleri dolan Arzu E., “Ben erkeklere bu kadar iftira atılmasını artık hoş görmüyorum. Çünkü bir kadının da ne kadar çirkinleşebileceğini trafikte yaşadım. 44 yaşındayım ve hayatımda hiç böyle bir şeye maruz kalmamıştım, yıllardır şoförüm. Şikayetçi oldum, karakola gittim. Şu anda sinirlerim o kadar bozuk ki hakikaten hiç yaşamadığım bir şey için hastanelerde darp raporu aldım, karakola gittim ifademi verdim. Umarım bu süreç hızlanır. Hukuk sistemine güveniyorum. Bu kadının gerçekten ceza almasını istiyorum. Böyle bir hareketi bir daha kimsenin yapmasını istemiyorum” ifadelerini kullandı. İHA</t>
+  </si>
+  <si>
+    <t>Rusya'nın başkenti Moskova'ya bağlı Podolsk kentinde, trafik lambalarının bulunmadığı bir kavşakta bir midilli atıyla otomobil çarpıştı. Kavşakta dönerek başka yola giren otomobil ilerlerken midilli atına bağlı at arabasındaki kadın sürücü at arabasının hızını arttırdı., Bu sırada duramayan at ile otomobil çarpıştı. Çarpışma sırasında at arabasındaki kadın sürücü uçarak yola fırladı., Olay yerine ambulans ve polis ekipleri yönlendirilirken, at arabasının kadın sürücüsünün kazada hafif bir şekilde yaralandığı ve tedavi altına alındığı belirtilirken, midilli atının ise kazadan yara almadan kurtulduğu kaydedildi., At çarpan araçta, ezikler meydana gelirken kazayla ilgili at arabasının kadın sürücüsüne ceza kesildiği öğrenildi. Başka bir araçtan çekilen görüntüler sosyal medyada yayınlanınca ilk kez görünen at ile araç çarpışması büyük ilgi çekti. (İHA)</t>
+  </si>
+  <si>
+    <t>Olay dün akşam saatlerinde İstanbul’un Merter ilçesinde yaşandı. D-100 Karayolu Bakırköy istikametinde ilerleyen bir kadın sürücü metrobüs bariyerlerine yakın bir noktada bir kedi gördü., EN SOL ŞERİTTE DURDU, Metrobüs yolu ile karayolunu birbirinden ayıran bariyerlerde mahsur kalan kediyi kurtarmak için harekete geçen kadın otomobilini en sol şeritte durdurdu. Aracından inerek kediyi kurtarmak isteyen kadına metrobüs durağında bulunan bir yolcu da yardımcı oldu. Kediyi araçların altında ezilmekten kurtaran kadın kediyi aracına aldı. Bir süre duran trafik daha sonra normal akışına döndü. (DHA)</t>
+  </si>
+  <si>
+    <t>Reyhan Ü. ve yanında yolcu konumunda bulunan arkadaşı Ahmet T. (37), 35 KD 5928 plakalı otomobil ile Boğaziçi Caddesi’nde seyir halinde olduğu sırada, uygulama yapan polis ekipleri otomobili durdurdu. Trafik polisinin kimlik ve ehliyet talep ettiği sırada, Reyhan Ü. otomobilin polisin üzerine sürerek olay yerinden kaçtı. Otomobilden uzaklaşan trafik polisi, konuyu diğer polis ekiplerine bildirdi. Reyhan Ü.’nün hareket ettiği güzergah üzerinde uygulama yapan polis ekipleri de Reyhan Ü.’yü durdumaya çalıştı ancak ihtarlara uymayan Reyhan Ü. kaçmaya devam etti., VİRAJI ALAMADI, Polis ekipleri Reyhan Ü.’yü durdurmak için otomobilin lastiklerine ateş etti. Buna rağmen kaçmaya devam eden Reyhan Ü., Yenişehir Mahallesi 1202 Sokak’ta virajı alamaması sonucu otomobilin direksiyonunu kaybederek kaldırıma çarptıktan sonra durdu. Durumun bildirilmesi üzerine bölgeye çok sayıda polis ve sağlık ekibi sevk edildi. Sağlık ekiplerinin yaptığı kontrolde, Reyhan Ü. ve Ahmet T.’nin kaza sonucu herhangi bir yara almadığı öğrenildi. Öte yandan, bölgeye gelen trafik polisi ekipleri Reyhan Ü.’ye alkolmetre ile ölçüm yapmak istedi., Bir süre alkolmetre ile ölçüm yapılmaması için direnen Reyhan Ü., daha sonra yapılan kontrolde 2.09 promil alkollü çıktı. Polis ekipleri,  Reyhan Ü.’ye alkol ölçümü yaparken, yanında bulunan arkadaşı Ahmet T. gazetecileri engellemeye çalıştı. Reyhan Ü.’nün görüntülenmemesi için bir süre direnen ve alkollü olduğu ileri sürülen Ahmet T., gazetecilere tepki gösterdi., OTOMOBİLDE İÇKİ ŞİŞESİ , Reyhan Ü.’nün alkollü çıkmasının ardından olay yeri inceleme ekiplerinin yaptığı kontrolde, kaza sonrası otomobilde içki şişesi ve bardaklar olduğu görüldü. Reyhan Ü. ve arkadaşı Ahmet T., polis ekipleri tarafından gözaltına alınarak polis merkezine götürüldü. Alkollü araç kullanmak, ‘Dur’ ihtarına uymamak, sokağa çıkma kısıtlamasını ihlal etmekten ceza kesilen sürücünün ehliyetine el konuldu ve otomobili trafikten men edildi. Olayla ilgili soruşturmanın sürdüğü öğrenildi. (DHA)</t>
+  </si>
+  <si>
+    <t>https://www.sozcu.com.tr/2021/gundem/kavsakta-can-pazari-10-yarali-6484077/</t>
+  </si>
+  <si>
+    <t>Kaza, saat 01.00 sıralarında merkez Aziziye ilçesinin Dadaşkent semtindeki belediye hizmet binası önünde E 80 karayolunda meydana geldi. Sürücüleri belirlenemeyen kazada Erzincan’dan Erzurum istikametine gide otomobil, iddiaya göre Dadaşkent istikametinden gelen ve kavşaktan kontrolsüz şekilde ana yola çıkan hafif ticari araçla çarpıştı., Kazanın şiddetiyle sürücüsünün direksiyon hakimiyetini kaybettiği otomobil yol kenarındaki bir iş yerinin duvarına çarparak durdu, içindeki 3 kişi hafif şekilde yaralandı., Hurdaya dönen hafif ticari araçta ise sürücü ile birlikte 7 kişi yaralandı. Yaralılardan bazılarının kaza sırasında çarpışmanın şiddetiyle araçtan karayoluna savruldukları öğrenildi. Araçta annesinin kucağında bulunan bebek ise şans eseri kazayı yara almadan atlattı., KAZAZEDE BEBEĞE YOLDAN GEÇEN KADIN SAHİP ÇIKTI, İhbar üzerine bölgeye itfaiye, sağlık ve polis ekipleri sevk edildi. Can pazarını yaşandığı kazada sıkışan bir kişi ise olay yerine gelen itfaiye ekipleri tarafından vatandaşların da yardımıyla çıkarıldı. Annesi ve yakınları yaralı olmasına rağmen kazayı burnu bile kanamadan atlatan bebek Feyza Bilire ise yoldan geçen bir kadın sahip çıktı. Bebeği kucağına alarak uzun süre ilgilendi., Hafif ticari araçta yaralanan Ramazan Bilir, Şahin Bilir, Şükran Bilir, Hatice Bilir, Arif Çerez, Dilek Çerez ve Mehmet Akif Çereze ilk müdahale olay yerinde sağlık ekipleri tarafından yapıldı. Ardından yaralılar, bebekle birlikte Atatürk Üniversitesi Araştırma Hastanesine kaldırıldı. Otomobilde bulunan 3 kişinin ise hafif şekilde yaralandıkları belirlendi., Karayolunda kontrollü olarak sağlanan trafik akışı ise kaza yapan araçların çekilip, yolun temizlenmesinin ardından normale döndü. (DHA)</t>
+  </si>
+  <si>
+    <t>Kaza, saat 22.30 sıralarında Alanya’nın Emişbeleni Mahallesi'nde meydana geldi. İlçe merkezine seyir halinde olan Ayşe Yakut (33) idaresindeki 07 AEV 961 plakalı otomobil, sürücüsünün direksiyon hakimiyetini kaybetmesi sonucu virajı alamayarak 20 metrelik uçuruma yuvalandı., Kazayı görenlerin 112 Acil Çağrı Merkezi'ne haber vermesi üzerine olay yerine sağlık ve jandarma ekipleri sevk edildi. Taklalar atarak ters duran araçtaki ağır yaralı sürücü Yakut'u ekipler bulunduğu yerden çıkardı. Sağlık ekipleri tarafından yapılan ilk müdahalenin ardından Yakut, ambulansla Alanya Alaaddin Keykubat Üniversitesi Eğitim ve Araştırma Hastanesine götürüldü. Yoğun bakıma ünitesine alınan talihsiz kadın, doktorların tüm müdahalesine rağmen yaşamını yitirdi.Gülen’in cenazesi savcılık tarafından yapılan incelemenin ardından ailesine teslim edildi. (İHA)</t>
+  </si>
+  <si>
+    <t>Bir Avrupa Birliği (AB) projesi olarak Türkiye Odalar ve Borsalar Birliği (TOBB) ile iş birliği içinde yürütülen “Mahir Eller” projesine İzmir Metro A.Ş., bünyesindeki 3 meslek grubu da dahil edildi. Proje kapsamında, “Kent içi Raylı Sistemler Katener Bakım Elemanı” ve “Kent İçi Raylı Sistemler Trafik Kontrolörü” meslek gruplarında personeli belgelendirilen ilk kurum olmayı başaran İzmir Metro A.Ş. proje kapsamında en fazla kadın sürücü personeli barındıran kurum olma unvanını da elde eti., Projeye dahil edilen İzmir Metro A.Ş.nin 16 personeli “Kent içi Raylı Sistemler Katener Bakım Elemanı”, 33 personeli “Kent İçi Raylı Sistemler Trafik Kontrolörü”, 20 personeli ise “Kent İçi Raylı Sistemler Tren Sürücüsü” kategorilerinde yeterlilik belgesi almaya hak kazandı. “Katener Bakım Personeli” ve “Trafik Kontrolörü” meslek gruplarında proje kapsamında belgelendirilen ilk kurum İzmir Metro A.Ş. oldu. “Kent İçi Raylı Sistemler Tren Sürücülüğü” programına katılan İzmir Metrosu ve İzmir Tramvayı’nda görevli 20 tren sürücüsünün 14’ünün kadın olması da dikkat çeken bir diğer unsurdu., İzmir’in kadın metro ve tramvay sürücüleri, projede kadınların en yoğun olarak temsil edildiği meslek grubunu oluşturdu. Programa katılanlar, yeterlilik belgesine hak kazanmak için önce teorik sınava tabi tutuldu, başarı olanlar ise sahada sınava alındı. Değerlendirme, ulusal meslek standartlarına ve yeterliliklerine göre yapıldı. Böylece projeye dahil edilen İzmir Metro A.Ş. personelinin tamamı, yeterliliğinin ulusal meslek standartlarında olduğunu kanıtladı., AB finansmanı ile yürütülen proje, TOBB iş birliği ile 12 ilde mesleki yeterliliği tescillenen personel yetiştirmeyi amaçlıyor. Projenin İzmir ayağını Ege Bölgesi Sanayi Odası (EBSO) yürütüyor., İHA</t>
+  </si>
+  <si>
+    <t>https://www.trthaber.com/haber/dunya/suudi-arabistanin-ilk-kadin-surucusu-ehliyetini-aldi-368603.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+, _x000D_
+	Kadınların araba sürmesinin yasak olduğu Suudi Arabistan’da ilk defa bir kadın sürücü belgesi aldı., _x000D_
+	2030 vizyonu kapsamında ülkede bugünden itibaren isteyen kadınlar sürücü belgesi alabilecek., _x000D_
+	Belgelerini alan kadınlar, belge aldıktan 3 hafta sonra trafiğe çıkabilecek. , _x000D_
+	Geçtiğimiz Eylül ayında Kral Selman bin Abdulaziz’in imzalı kararnamesi ile "kadınların araç sürmesi önündeki yasal engelin kaldırıldığı" duyurulmuştu., _x000D_
+	Kaynak: İHA_x000D_
+	 </t>
+  </si>
+  <si>
+    <t>https://www.trthaber.com/haber/dunya/suudi-arabistanli-kadin-surucu-f1-araci-kullandi-371660.html</t>
+  </si>
+  <si>
+    <t>_x000D_
+	Suudi Arabistan Motor Sporları Federasyonu'nun ilk kadın yönetim kurulu üyesi Aseel el-Hamad, araç kullanmalarına serbesti getirilen ülkesindeki hemcinsleri adına bir ilke imza attı., 
+, , _x000D_
+	Renault Formula 1 Takımı'ndan yapılan açıklamaya göre, el-Hamad, sezonun 8. yarışı Fransa Grand Prix'si öncesi gerçekleşen geçit töreninde F1 otomobilinin direksiyonuna geçti., 
+, , _x000D_
+	El-Hamad, 10 yıl sonra Formula 1 takvimine dönen Fransa Grand Prix'sine ev sahipliği yapan Paul Ricard Pisti'nde, Renault'nun 2012 sezonundaki aracı E20'yi sürdü., _x000D_
+	Kaynak: AA, Reuters</t>
+  </si>
+  <si>
+    <t>https://www.trthaber.com/haber/turkiye/kadin-surucu-alkollu-olmasaydi-aybuke-hayatta-olacakti-520017.html</t>
+  </si>
+  <si>
+    <t>_x000D_
+	Kaza, 4 Eylül sabahı, Selçuklu ilçesi Yeni İstanbul Yolu üzerindeki Cumhuriyet Polis Merkezi önündeki kavşakta yaşandı., _x000D_
+	Samet Kurt, 42 CRL 81 plakalı otomobiliyle kırmızı ışıkta durdu. Ancak arkadan gelen 50 yaşındaki Emel Gümüş'ün kullandığı 34 AAN 361 plakalı otomobil, Kurt'un aracına çarptı. 4 aracın karıştığı zincirleme kazada 31 yaşındaki Samet Kurt, 28 yaşındaki eşi Teslime Kurt ve bebek koltuğundaki 2 yaşındaki Aybüke Kurt yaralandı., 
+, , _x000D_
+	Yoldan geçen bir doktorun ilk müdahalesini yaptığı Aybüke ve diğer yaralılar, ambulanslarla Selçuk Üniversitesi Tıp Fakültesi Hastanesi'ne kaldırıldı., 
+Küçük Aybüke hayatını kaybetti, 
+, , _x000D_
+	Samet-Teslime Kurt çifti yapılan tedavilerinin ardından taburcu edilirken, beyin kanaması geçiren Aybüke, yoğun bakım ünitesinde alındı., _x000D_
+	Küçük Aybüke, 15 Eylül akşamı hayatını kaybetti., 
+Alkollü ve ehliyetsiz, _x000D_
+	Kazanın ardından gözaltına alınan ve bir mühendislik firmasının ortağı olan sürücü Emel Gümüş'ün ehliyetsiz ve 120 promil alkollü olduğu halde araç kullandığı ortaya çıktı., _x000D_
+	Emel Gümüş'ün kazadan bir hafta önce alkollüyken hasarlı kazaya karıştığı, ehliyetine 6 ay süreyle el koyulduğu, son kazadaki aracın ise kiralık olduğu tespit edildi., _x000D_
+	Polisteki ifadesinde, ''Alkollü ve ehliyetsiz araç kullanmanın suç olduğunu biliyorum ancak işlerimi takip edebilmek için araç mecburen kullanıyorum" diyen Gümüş, sevk edildiği adliyede, adli kontrolle serbest bırakıldı., 
+Yeniden gözaltına alınıp tutuklandı, _x000D_
+	Cumhuriyet Başsavcılığının itirazı üzerine yeniden gözaltına alınan Gümüş, Konya 5. Sulh Ceza Hakimliğince 'Bilinçli taksirle birden fazla kişinin yaralanmasına neden olma' suçundan tutuklandı., 
+Bilirkişi raporu: Emel Gümüş asli kusurlu, 
+, , _x000D_
+	Soruştırma kapsamında bilirkişi tarafından hazılanan raporda, kazada Emel Gümüş'ün asli kusurlu olduğu bildirildi. Raporda kaza yerinde 9,5 metre fren izi olduğu anlatılarak, şu ifadelere yer verildi:, _x000D_
+	"Emel Gümüş'ün 120 promil alkollü vaziyette araç kullandığı, görüşün açık olduğu gündüz vakti, tek yönlü Yeni İstanbul Caddesi'ni takiben seyrinde, alkolün de vermiş olduğu etki ile yola gereken dikkati vermemiş, dikkatsiz ve kontrolsüz bir şekilde önündeki aracı yakın takip etmiş, süratli bir şekilde önündeki zorunluluk nedeni ile duran otomobilin arka kısmından çarparak kazaya sebebiyet vermiştir. Sürücü Emel Gümüş yola dikkat ve özen yükümlülüklerini yerine getirmemiş, yol ve trafik durumunun gerektirdiği şartlara göre seyretmemiş, önünde aynı yönde seyreden araç ile arasında emniyetli mesafe bırakmamış, tehlikeli ve süratli araç kullanmış, trafik güvenliğini tehlikeye düşürmüş, önündeki araçları yakın mesafeden takip etmiş, bu aracın yavaşlayacağını yada duracağını hiç düşünmemiştir. Sürücünün yol ve araç trafiğinin durumunu dikkate alması gerekirken almadığından, bu kusurlu davranışı, 'Önlerinde seyreden araçları güvenli ve yeterli bir mesafeden izlememek', 'Arkadan çarpma' ve 'Sürücüler hızlarını kullandıkları aracın yük ve teknik özelliğine görüş, yol, hava ve trafik durumunun getirdiği şartlara uydurmak zorundadırlar' hükümlerini ihlali niteliğindedir. Ayrıca Emel Gümüş'ün 120 promil alkollü olduğu anlaşılmış, bu kusurlu davranışında 'Alkollü araç kullanmak' hükmünün ihlali niteliğindedir.", 
+"Alkollü olmasaydı kaza gerçekleşmezdi", _x000D_
+	Raporda alkolün kazaya etkisine de dikkat çekilerek, "Emel Gümüş, şayet alkol almadan idaresindeki otomobilin hızını, şartlarına ve aracının teknik şartlarına göre kullansaydı ve önündeki aracı yeterli ve güvenli mesafeden takip etseydi bu kaza meydana gelmezdi. Sürücü aracını önüne herhangi bir tehlike çıkacakmış gibi, önündeki seyreden aracın her an durabileceğini düşünerek önündeki araç arasındaki mesafeyi koruması lazımdı. Bu nedenle sürücü Emel Gümüş asli kusurlu, Samer Kurt ve diğer iki araç sürücüsü ise kusursuzdur" denildi. </t>
+  </si>
+  <si>
+    <t>https://www.trthaber.com/haber/turkiye/tartistigi-surucunun-arabasinin-camini-tekmeledi-508788.html</t>
+  </si>
+  <si>
+    <t>_x000D_
+	Eyüpsultan-Güzeltepe Mahallesi Mareşal Fevzi Çakmak Caddesi'nde, dün akşam saat 20.20 sıralarında, trafikte tartıştığı sürücü Sena K'ye saldıran, aracın ön camını kıran ve hakaretlerde bulunan Emre E'nin bu görüntülerinin sosyal medyada yer alması ve mağdurun şikayeti üzerine, İstanbul Cumhuriyet Başsavcılığı soruşturma başlattı., _x000D_
+	Soruşturma kapsamında gözaltına alınan şüpheli Emre E., emniyetteki işlemlerinin ardından Çağlayan'daki İstanbul Adalet Sarayı'na sevk edildi., _x000D_
+	Adliye girişinde gazetecilerin, "Neden arabaya saldırdınız?" sorusuna şüpheli, "Dosyada hepsi var" yanıtını verdi., _x000D_
+	Soruşturma savcılığınca ifadesi alınan şüpheli Emre E., "kasten yaralama" ve "mala zarar verme" suçlarından tutuklanması talebiyle hakimliğe sevk edildi., 
+Vali'den genç kadına destek paylaşımı, _x000D_
+	İstanbul Valisi Ali Yerlikaya da olaya ilişkin Twitter'dan yaptığı paylaşımda, "Trafikte yol verme tartışması nedeniyle Sena kardeşimize saldıran şahıs gözaltına alınmıştır. Beni derinden üzen bu olayı kınıyorum. Hep birlikte takipçisi olacağız." ifadelerini kullanmıştı.</t>
+  </si>
+  <si>
+    <t>_x000D_
+	AA muhabirinin Emniyet Genel Müdürlüğü verilerinden derlediği bilgiye göre, erkek sürücülerin çoğunlukta bulunduğu trafikte kadın sürücülerin sayısı artmaya başladı.
+_x000D_
+	Buna göre, 2005-2014 arasındaki dönemde ehliyet sahibi kişilerin cinsiyet oranındaki erkek üstünlüğü, her geçen yıl azalıyor.
+_x000D_
+	Ehliyeti bulunan erkek sayısının toplam sürücü sayısına oranı, 2005 yılında yüzde 84 olarak gerçekleşti. 2014'te ise bu oran yüzde 77,2'ye geriledi.
+_x000D_
+	Aynı dönemde kadınların oranı her geçen yıl artış gösterdi. Buna göre, 2004'te ehliyetlilerin yüzde 16'sını kadınlar oluştururken, bu oran 2014'te yüzde 22,8'e yükseldi.
+Kadın sürücü sayısı katlandı
+_x000D_
+	Ülke genelinde kadın sürücü sayısında da büyük artışlar sağlanıyor.Ehliyet sahibi olan kadınların sayısı 2005 yılında 2 milyon 719 bin 817'e, 2006'da 2 milyon 872 bin 951'e, 2007'de 3 milyon 67 bin 496'ya, 2008'de 3 milyon 303 bin 959'a, 2009'da 3 milyon 589 bin 639'a, 2010'da 4 milyon 90 bin 895'e, 2011'de 4 milyon 527 bin 998'e, 2012'de 4 milyon 912 bin 65'e, 2013'te ise 5 milyon 412 bin 759'a ulaştı.
+_x000D_
+	Trafikte araç kullanan kadınların sayısı, 2014'te zirve yaptı. Bu dönemde kadın sürücü sayısı 5 milyon 917 bin 309 olarak gerçekleşti. Buna göre, 2005-2014 yılları arasında kadın sürücü sayısında yaklaşık iki kat artış sağlandı._x000D_
+	 , _x000D_
+	(AA)</t>
+  </si>
+  <si>
+    <t>https://www.urfanatik.com/haber/5838700/urfada-kadin-surucu-bariyerlere-carpti-yaralilar-var</t>
+  </si>
+  <si>
+    <t>Şanlıurfa’da sürücüsünün direksiyon hakimiyetini kaybettiği otomobil bariyerlere çarptı. Meydana gelen kazada 2 kişi yaralandı.
+,  Kaza Şanlıurfa-Mardin karayolu üzeri Osmanbey kampüsü civarında meydana geldi. Edinilen bilgiye göre Harran Üniversitesi Osmanbey kampüsü civarında meydana gelen kazada sürücüsü Dilek Tunç sürücüsünün direksiyon hâkimiyetini kaybettiği 34 ANJ 313 plakalı otomobil bariyerlere çarptı., , Meydana gelen kazada sürücü Dilek Tunç ve yanında bulunan arkadaşı Rabia Akengin yaralandı. Haber verilmesi üzerine olay yerine 112, itfaiye ve polis ekipleri sevk edildi. Kısa sürede olay yerine gelen İtfaiye ekipleri yaralıları sıkıştığı yerden çıkartarak sağlık ekiplerine teslim etti. 112 ekiplerinin olay yerindeki ilk müdahalesinin ardından yaralılar hastaneye kaldırılırken, itfaiye ekipleri ve polis ekipleri de kazanın meydana geldiği yol üzerinde güvenlik önlemler aldı., Kazayla ilgili soruşturma başlattı., , 
+01 Ara 2020 - 19:36
+-
+Asayiş
+Yazdır
+, Muhabir İbrahim Çakmak, urfanatik.com son bir ayda 989.869 kez ziyaret edildi., Yorumunuz yarım kaldı, devam etmek için üstteki yoruma, silmek için buraya tıklayın, Kırmızı alanlar eksik veya hatalı girildi. Lütfen bu alanları düzeltip tekrar gönderelim, Yorumunuz için teşekkürler, en kısa sürede gözden geçirilip yayınlanacaktır, Yorum yazarak Urfanatik Gazetesi Topluluk Kuralları’nı kabul etmiş bulunuyor ve yorumunuzla ilgili doğrudan veya dolaylı tüm sorumluluğu tek başınıza üstleniyorsunuz. Yazılan yorumlardan Urfanatik Gazetesi hiçbir şekilde sorumlu tutulamaz., Anadolu Ajansı (AA), İhlas Haber Ajansı (İHA), Demirören Haber Ajansı (DHA) tarafından servis edilen tüm haberler Urfanatik Gazetesi editörlerinin hiçbir editöryel müdahalesi olmadan, ajans kanallarından geldiği şekliyle yayınlanmaktadır. Sitemize ajanslar üzerinden aktarılan haberlerin hukuki muhatabı Urfanatik Gazetesi değil haberi geçen ajanstır., Şimdi oturum açın, her yorumda isim ve e.posta yazma zahmetinden kurtulun. Oturum açmak için bir hesabınız yoksa, oluşturmak için buraya tıklayın.
+, Yorum yazarak  Urfanatik Gazetesi Topluluk Kuralları’nı kabul etmiş bulunuyor ve yorumunuzla ilgili doğrudan veya dolaylı tüm sorumluluğu tek başınıza üstleniyorsunuz. Yazılan yorumlardan Urfanatik Gazetesi hiçbir şekilde sorumlu tutulamaz., Anadolu Ajansı (AA), İhlas Haber Ajansı (İHA), Demirören Haber Ajansı (DHA) tarafından servis edilen tüm haberler Urfanatik Gazetesi editörlerinin hiçbir editöryel müdahalesi olmadan, ajans kanallarından geldiği şekliyle yayınlanmaktadır. Sitemize ajanslar üzerinden aktarılan haberlerin hukuki muhatabı Urfanatik Gazetesi değil haberi geçen ajanstır., Sitemizde  online, Reklam seçeneklerimizi inceleyin, 
+©Copyright 2021 Urfanatik Gazetesi Tüm Hakları Saklıdır
+-
+Veri PolitikasıKullanım Şartları
++90 (532) 175 0403
+,  Veri politikasındaki amaçlarla sınırlı ve mevzuata uygun şekilde çerez konumlandırmaktayız. Detaylar için veri politikamızı inceleyebilirsiniz.</t>
+  </si>
+  <si>
+    <t>https://www.yeniakit.com.tr/haber/trafik-polisleri-kadin-surucu-ve-yolculara-karanfil-dagitti-1110093.html</t>
+  </si>
+  <si>
+    <t>13.06.2021 Günün Âyet ve Hadisi, Hamas Sözcüsü'nden, BAE Dışişleri Bakanı'nın Hamas'ı terör örgütü DEAŞ'a benzetmesine tepki: Araplık değerleriyle bağdaşmaz, HÜDA PAR Genel Başkanı Yapıcıoğlu: Aileyi yıkmak için özel çaba sarf edenler, zehrin içerisine bal katıyorlar!, G7'den Çin'in dev projesine misilleme çıktı, Marmara Denizi Eylem Planı Koordinasyon Kurulu kuruldu, FLAŞ! Doç. Dr. Cihat Yaycı’dan Erdoğan-Biden görüşmesine yönelik bomba açıklamalar: Türkiye işte bunları yapmalıdır!, Fransa'da muhtıracı generaller hesap verecek, Bakan Koca açıkladı: Bir adım daha yaklaştık, Çin'den o ülkeye çağrı: Sömürgecilik rüyasından vazgeç, Yazar Kaçar, siyonistlerin mezalimlerini hatırlattı, Konya İl Emniyet Müdürlüğü Trafik Denetleme Şube Müdürlüğü ekipleri, kadın sürücü ve yolcuların bulunduğu araçları durdurup karanfil vererek 8 Mart Dünya Kadınlar Günü’nü kutladı., Konya İl Emniyet Müdürlüğü Trafik Denetleme Şube Müdürlüğü ekipleri, kadın sürücü ve yolcuların bulunduğu araçları durdurup karanfil vererek 8 Mart Dünya Kadınlar Günü’nü kutladı., Trafik Denetleme Şube Müdürlüğü ekipleri, Ferit Paşa Caddesi üzerinde 8 Mart Dünya Kadınlar Günü dolayısıyla trafik uygulaması yaptı. Uygulama sırasında durdurulan araçlarda bulunan kadın sürücüler ve yolculara trafik polisleri tarafından karanfil hediye edildi. Trafik polisleri, Kadınlar Günü dolayısıyla sürücülerin yanı sıra yoldan geçen kadınlara da karanfil vererek günlerini kutladı. Kadın sürücü ve yolcular ise uygulamadan duydukları memnuniyeti dile getirdi. , TRT'de Pazartesi günlerine damga vuran Uyanış Büyük Selçuklu'nun yapımcısı Emre Konuk'tan bomba bir paylaşım geldi., Türkiye'ye savunma sanayiinde ambargo uygulayan ülkeler, şimdi de siber güvenlikte aynı kararı aldı. Cep telefonlarını inceleyen yazılımlard.., Gazeteci yazar Mahmut Övür, İP Genel Başkanı Meral Akşener'in yakın çevresine, zaman zaman "Ekrem benim oğlum gibidir" dediğini ve cumhurbaş.., WhatsApp İhbar Hattı, +90 (553) 313 94 23, Bip İhbar Hattı, +90 (553) 313 94 23, Yaay İhbar Hattı, +90 (553) 313 94 23, Akit haber güncel son dakika gündem haberleri ve haber arşivi., Biz her vakit, hakikati haykırdık ve gerçeğin izinde olduk. Her devrin gazetesi olmadık, milletin gazetesi olduk., www.yeniakit.com.tr internet sitesinde yayınlanan yazı, haber, röportaj, fotoğraf, resim, sesli veya görüntülü sair içeriklerle ilgili telif hakları Uğurlu Gazetecilik Basın Yayın Matbaacılık Reklamcılık Limited Şirketi’ne aittir. Bu içeriklerin iktibas hakkı saklıdır. İzinsiz ve kaynak gösterilmeksizin iktibas olunamaz; hiçbir surette kopyalanamaz, yeniden yayıma konulamaz., Yüklenme süresi 0.0111 sn.</t>
+  </si>
+  <si>
+    <t>Korkunç kaza TEM yolu Bolu Dağı Tüneli geçişinde meydana geldi. Ankara yönüne giden Aslı Dalkıran yönetimindeki 34 ND 445 plakalı cip, tünele 3 kilometre kala sürücüsünün direksiyon kontrolünü yitirmesi sonucu önündeki Şenel Kaymaz'ın kullandığı 67 ABA 150 plakalı TIR'a çarptı. , Çarpmanın şiddetiyle savrulan cip bariyere çarptı. Dalkıran kullanılmaz hale gelen cipin içinde sıkışırken, çevredekilerin ihbarı üzerine kaza yerine sağlık, jandarma ve itfaiye ekibi sevk edildi. , İtfaiye ekiplerince başlatılan çalışma sonucu yaklaşık 45 dakikada Aslı Dalkıran araçtan çıkarıldı. Yaralı Aslı Dalkıran, sağlık görevlilerince yapılan ilk müdahalesinin ardından hastaneye kaldırılarak tedaviye alındı. Kaza nedeniyle yolda uzun araç kuyrukları oluştu. Aracın yoldan kaldırılmasının ardından trafik normale döndü., ,  ,  ,  ,  ,  ,  ,  ,  ,  </t>
+  </si>
+  <si>
+    <t>Kaza, saat 22.00 sıralarında İzmir Çevreyolu Bornova Işıkkent Kavşağı yakınında meydana geldi. Buca'dan Bornova istikametine giden Melek Aslan yönetimindeki 35 AIE 031 plakalı otomobil, iddiaya göre ani manevra yaparak sağ şeride geçince F.Ç. (42) yönetimindeki  20 P 1828 plakalı TIR'ın 20 P 1829 plakalı dorsesine arkadan çarptı. Çarpmanın etkisiyle Melek Aslan'ın otomobili demir yığınına dönerken, kazayı gören sürücüler durumu sağlık, itfaiye ve polis ekiplerine bildirdi. İhbar üzerine gelen polis ekipleri güvenlik tedbiri alarak, otoyoldaki trafik akışını tek şeritten sağladı.,   Olay yerine gelen sağlık ekiplerinin yaptığı kontrolde, sürücü Melek Aslan'ın olay yerinde hayatını kaybettiği belirlendi. Çarpmanın etkisiyle demir yığını haline dönüşen otomobilde yolcu konumunda bulunan Samet Hafızoğlu ise sıkıştığı yerden itfaiye ekiplerinin yaptığı müdahale sonucu çıkarıldı. Sağlık ekiplerine teslim edilen Hafızoğlu, ambulans ile Ege Üniversitesi Tıp Fakültesi Hastanesi'ne sevk edildi. Burada tedaviye alınan Hafızoğlu'nun hayati tehlikesinin bulunduğu öğrenildi.  ÇEVREYOLUNDA ULAŞIM 3 SAAT TEK ŞERİTTEN SAĞLANDI  Kaza sonrası başlatılan soruşturmada Melek Aslan'ın cesedi savcının incelemesinin ardından itfiaye ekiplerince otomobilden çıkartılarak İzmir Adli Tıp Kurumu morguna gönderildi. TIR sürücüsü F.Ç. ise ifadesi alınmak üzere polis merkezine götürüldü. Kaza nedeniyle otoyolda ulaşım yaklaşık 3 saat tek şeritten sağlandı. İzmir Çevreyolu, kazaya karışan araçların çekici yardımıyla kaldırılması ile normale döndü.  CEP TELEFONUNDA NAVİGASYON AÇIK KALMIŞ  Bu arada polisin kaza ile ilgili başlattığı soruşturmada ilginç ayrıntı ortaya çıktı. Otomobilde yapılan kontrolde Melek Aslan'a ait olduğu belirlenen cep telefonu ile Işıkkent'teki bir adrese gitmek için navigasyonun açık olduğu görüldü., Aslan'ın navigasyona baktığı sırada Işıkkent Kavşağı'nı kaçırdığı için sol şeritten sağ şeride ani manevra yapması sonucu kazanın meydana geldiği tahmin edilirken, polisin de bu yönde rapor tuttuğu öğrenildi. Kaza yerinden 20 metre geride kavşak olduğu görüldü. Kazayla ilgili soruşturma sürdürülüyor.  , , ,  , ,  ,  ,  ,  ,  ,  ,  ,  </t>
+  </si>
+  <si>
+    <t>Osmaniye'de Döndü Bahargülü, takip ettiği dizi olan “Akasya Durağı” adlı dizide taksi şoförlüğü yapan “Melahat” isimli karakterden etkilenerek, 10 yıl önce başlayan taksicilik yapma hayalini gerçeğe dönüştürdü. Bir süre önce banka kredisiyle otomobil alan Döndü Bahargülü, otomobili ticari taksi yaptı. Önceleri oğlunun çalıştırdığı ticari taksiyi, oğlu askerlik hizmetini yapmaya gidince kendisi devralan Bahargülü şöyle konuştu:, , 
+EKONOMİ
+2 bin 249 taksi plakasının sahibi kadın
+, MÜŞTERİLER MEMNUN, Kadın taksici Döndü Bahargülü ile yolculuk yapan Emre Karadal isimli müşterisi ise, “Direksiyonu, trafik kurallarına uyması gayet başarılı. Kadınların hayatın her alanında çalışması gerektiğine inanıyorum. Döndü hanım da işini gayet başarılı yapıyor. Hayırlı olsun diyorum” şeklinde konuştu., 
+GÜNDEM
+Vicdansız taksici: Doğum yapan kadını araçtan attı
+, Yeni Şafak olarak yayın hayatına başladığımız ilk günden itibaren ülkemizde demokrasinin tüm kurumları ile yerleşmesi, milli irade ve değerlerimizin hakim olması için tüm gücümüzle çalıştık. Bu ülkenin geleceğinin derin sularda boğulup gitmemesi için çaba sarf ettik., Fırtınalı günlerde sığınılacak bir liman olduk. Bugüne kadar ülkemize yapmış olduğumuz katkıyı bundan sonra da okurlarımızın desteği ile sürdürmeye devam edeceğiz. Her gün Yeni Şafak’la yeni bir umut olacak., 6698 sayılı Kişisel Verilerin Korunması Kanunundaki amaçlar ile sınırlı ve mevzuata uygun şekilde çerezler kullanılmaktadır. Detaylı bilgi için çerez politikamızı inceleyebilirsiniz.</t>
+  </si>
+  <si>
+    <t>https://www.yenisafak.com/video-galeri/gundem/antalyada-kadin-surucu-carptigi-genc-kizin-basindan-ayrilmadi-2210279</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yeni Şafak olarak yayın hayatına başladığımız ilk günden itibaren ülkemizde demokrasinin tüm kurumları ile yerleşmesi, milli irade ve değerlerimizin hakim olması için tüm gücümüzle çalıştık. Bu ülkenin geleceğinin derin sularda boğulup gitmemesi için çaba sarf ettik. , Fırtınalı günlerde sığınılacak bir liman olduk. Bugüne kadar ülkemize yapmış olduğumuz katkıyı bundan sonra da okurlarımızın desteği ile sürdürmeye devam edeceğiz. Her gün Yeni Şafak’la yeni bir umut olacak. , 6698 sayılı Kişisel Verilerin Korunması Kanunundaki amaçlar ile sınırlı ve mevzuata uygun şekilde çerezler kullanılmaktadır. Detaylı bilgi için çerez politikamızı inceleyebilirsiniz. </t>
+  </si>
+  <si>
+    <t>Polis lastiklere ateş etti! Kadın sürücü ezmeye kalktı - Vatan</t>
+  </si>
+  <si>
+    <t>Vicdanları sızlatan olay! Kadın sürücü köpeğe çarpıp kaçtı - Vatan</t>
+  </si>
+  <si>
+    <t>AMBULANSTA KADIN SÜRÜCÜ GÖREN ŞOFÖRLER - Kayseri Haber</t>
+  </si>
+  <si>
+    <t>Eşine kızan kadın sürücü, kocasının ayağını ezdi - Kdz Ereğli Haberler - PUSULA</t>
+  </si>
+  <si>
+    <t>Kadın sürücü kanala uçtu - Yıldırım Gazetesi</t>
+  </si>
+  <si>
+    <t>Antalya'da motosiklet kullanan kadın sürücü epilepsi nöbeti geçirdi - ABCGazetesi</t>
+  </si>
+  <si>
+    <t>Kadın sürücü fren yerine gaza basınca olanlar oldu. - Doğru Haber</t>
+  </si>
+  <si>
+    <t>Motosikletli kadın sürücü yaralandı - Aydın Hedef Gazetesi</t>
+  </si>
+  <si>
+    <t>Nazilli’de 2 kadın sürücü kafa kafaya çarpıştı - Aydın Hedef Gazetesi</t>
+  </si>
+  <si>
+    <t>Denizli'de otomobil takla attı! Kadın sürücü yaralı - Ayna Haber</t>
+  </si>
+  <si>
+    <t>Yaşlı adama bu şekilde çarptı - Bursa.com - Bursa Haberleri</t>
+  </si>
+  <si>
+    <t>Maske takmayan yolcu kendisini uyaranlara saldırdı - Cumhuriyet</t>
+  </si>
+  <si>
+    <t>Fren yerine gaza basan kadın sürücü 3 yayayı ezdi - denizli 20 haber</t>
+  </si>
+  <si>
+    <t>Gaz ile freni karıştıran kadın sürücü - Ensonhaber</t>
+  </si>
+  <si>
+    <t>Acemi kadın sürücü, virajı alamayınca sağlık ocağına girdi - Haberler.com</t>
+  </si>
+  <si>
+    <t>Yol verme tartışması nedeniyle kadın sürücü ile kamyon şoförü tekme tokat kavga etti - Haberler.com</t>
+  </si>
+  <si>
+    <t>Hurdaya dönen otomobilden çıkartılan kadın sürücü kurtarılamadı - Haberler.com</t>
+  </si>
+  <si>
+    <t>Tokat attığı kadın sürücü tekvandocu çıktı! Adamın dayak yediği anlar kameraya yansıdı - Haberler.com</t>
+  </si>
+  <si>
+    <t>Maddi hasarlı kaza sonrası araçtan inen kadın sürücü feci şekilde can verdi - Haberler.com</t>
+  </si>
+  <si>
+    <t>Ukrayna'da tramvay yoluna park eden kadın sürücü, trafiği 2 saat boyunca felç etti - Haberler.com</t>
+  </si>
+  <si>
+    <t>Çarptığı motosikletli ölen kadın sürücü gözyaşlarına boğuldu Sinir krizi geçiren sürücü: "Benim de... - Habertürk</t>
+  </si>
+  <si>
+    <t>Hafriyat kamyonunun çarptığı kadın öldü; sürücü gözaltında - Habertürk</t>
+  </si>
+  <si>
+    <t>Sivas'ta, jandarmadan kadın sürücü ve yolculara çiçek - Habertürk</t>
+  </si>
+  <si>
+    <t>Dur' ihtarına uymayan kadın sürücü kazada öldü, arkadaşı yaralı - Hürriyet</t>
+  </si>
+  <si>
+    <t>Korna çalan kadın sürücüyü darp eden şüpheli yakalandı - Hürriyet</t>
+  </si>
+  <si>
+    <t>Maltepe’de kazadan sonra kadın sürücü şoka girdi - Hürriyet</t>
+  </si>
+  <si>
+    <t>Jandarmadan, kadın sürücü ve yolculara çiçek - Hürriyet</t>
+  </si>
+  <si>
+    <t>Kocaeli'de kadın sürücü karşıdan karşıya geçen 2 genç kıza çarptı - Internet Haber</t>
+  </si>
+  <si>
+    <t>Karaman'da Feci Kaza! Kadın Sürücü Yaralandı! - Karaman Gündem</t>
+  </si>
+  <si>
+    <t>İzmit Trafiğinde Sıradan Bir Gün! Kadın Sürücü, Trafiği Böyle Tıkadı! İsyan Edip Arabadan İnenler Var… - Kocaeli Denge</t>
+  </si>
+  <si>
+    <t>Kısıtlama gününde başka bir aracın sıkıştırdığı kadın sürücü, bariyerlere çarptı - Medya Gazete</t>
+  </si>
+  <si>
+    <t>Kadın sürücü, kurşunun deldiği yeri görünce büyük korku yaşadı - Milliyet</t>
+  </si>
+  <si>
+    <t>Kadın sürücü Ankara'yı birbirine kattı - Milliyet</t>
+  </si>
+  <si>
+    <t>Otomobilin çarptığı 7 yaşındaki Ömer öldü! Sürücü kadın sinir krizi geçirdi - Milliyet</t>
+  </si>
+  <si>
+    <t>Makas atarak çarptığı kadın hafızasını yitirdi: Asli kusurlu sürücü serbest - NTV</t>
+  </si>
+  <si>
+    <t>Kadın ve erkek sürücü birbirine girdi - NTV</t>
+  </si>
+  <si>
+    <t>Kadın sürücü, aracını tekmeleyen saldırganı kaputun üzerinde polis merkezine götürdü - Posta</t>
+  </si>
+  <si>
+    <t>Üsküdar’da yokuş aşağı inen kadın sürücü otomobiliyle takla attı | Video - Sabah</t>
+  </si>
+  <si>
+    <t>Ehliyetsiz kadın sürücü, kaldırımdaki 2 yaşlı kadını böyle ezdi - Sabah</t>
+  </si>
+  <si>
+    <t>Yok böyle acı! Minik Duru kaza kurbanı oldu… - Sabah</t>
+  </si>
+  <si>
+    <t>Aydın’da feci kaza, kadın sürücü hayatını kaybetti - Aydın Ses Gazetesi</t>
+  </si>
+  <si>
+    <t>ANTALYA'DA 2 KADIN SÜRÜCÜ TRAFİKTE SAÇ SAÇA KAVGA ETTİ - SonDakika.com</t>
+  </si>
+  <si>
+    <t>Diyarbakır'da kadın sürücü başka araç tarafından sıkıştırıldı: 2 yaralı - SonDakika.com</t>
+  </si>
+  <si>
+    <t>Alkollü kadın polislerin canına kast etti - Sözcü</t>
+  </si>
+  <si>
+    <t>Kavşakta can pazarı: 10 yaralı - Sözcü</t>
+  </si>
+  <si>
+    <t>Suudi Arabistan’ın ilk kadın sürücüsü ehliyetini aldı - TRT Haber</t>
+  </si>
+  <si>
+    <t>Suudi Arabistanlı kadın sürücü F1 aracı kullandı - TRT Haber</t>
+  </si>
+  <si>
+    <t>Kadın sürücü alkollü olmasaydı Aybüke hayatta olacaktı' - TRT Haber</t>
+  </si>
+  <si>
+    <t>Kadın sürücünün aracına saldıran şüpheli gözaltında - TRT Haber</t>
+  </si>
+  <si>
+    <t>Urfa’da Kadın sürücü bariyerlere çarptı: Yaralılar var - URFANATİK</t>
+  </si>
+  <si>
+    <t>Trafik polisleri kadın sürücü ve yolculara karanfil dağıttı - Yeni Akit Gazetesi</t>
+  </si>
+  <si>
+    <t>Akasya Durağı'ndan etkilenen kadın sürücü taksici oldu​ - Yeni Şafak</t>
+  </si>
+  <si>
+    <t>Antalya'da kadın sürücü çarptığı genç kızın başından ayrılmadı - Yeni Şafak</t>
+  </si>
+  <si>
+    <t>Dur ikazına uymayan sürücü kısa sürede yakalandı - Kdz - Ereğli Demokrat Medya</t>
+  </si>
+  <si>
+    <t>https://www.trthaber.com/haber/guncel/denizlide-polisin-dur-ihtarina-uymayan-surucu-kaza-yapinca-yakalandi-586901.html</t>
+  </si>
+  <si>
+    <t>[_x000D_
+	Yeni tip koronavirüs (COVID-19) tedbirlerine yönelik Hacıkaplanlar Mahallesi'nde denetim yapan polis ekipleri, 35 ACC 212 plakalı otomobile "dur" ihtarında bulundu., _x000D_
+	Polisten kaçan sürücü, yaklaşık 5 kilometre sonra Zümrüt Mahallesi'nde bir apartmanın bahçe duvarına çarptı., _x000D_
+	Araçtan inen ve yaya olarak kaçmaya çalışan kadın sürücü Ş.N.Ç, yakalandı. Ehliyetinin olmadığı ve sokağa çıkma kısıtlamasından muaf olmadığı belirlenen kadına 8 bin 750 lira para cezası uygulandı., _x000D_
+	Kaza anı, bir iş yerinin güvenlik kamerasına yansıdı.]</t>
+  </si>
+  <si>
+    <t>Kazada ağır yaralanan sürücü hayata tutunamadı https://t.co/CMZ9hWDypG</t>
+  </si>
+  <si>
+    <t>https://www.elbistankaynarca.com/haber/7264261/kazada-agir-yaralanan-surucu-hayata-tutunamadi</t>
+  </si>
+  <si>
+    <t>Elbistan’da otomobille cipin çarpışması sonucu yaşanan trafik kazasında ağır yaralanan 37 yaşındaki kadın sürücü, kaldırıldığı hastanede kurtarılamayarak hayatını kaybetti., Orhangazi Mahallesi Eldelek Caddesi’nde meydana gelen kazada; Termik Caddesi yönünde seyir halinde olan Serhat K. İdaresindeki 38 FN 757 plakalı otomobil, sürücüsünün direksiyon hakimiyetini kaybetmesi sonucu, karşı istikametten gelen 37 yaşındaki Hatice Öztürk’ün kullandığı 06 ACN 781 plakalı ciple kafa kafaya çarpışmıştı. Ortalığı savaş alanına çeviren kazada sürücülerle birlikte otomobilin yolcu koltuğundaki Enes A. yaralanmıştı. Durumu ağır olan cip sürücüsü Öztürk ile otomobilde sıkışan yaralılar, itfaiye ekiplerince demir kesme makinesi yardımıyla çıkarılarak hazır bekletilen 112 Acil Servis görevlileri tarafından Elbistan Devlet Hastanesi’ne kaldırılmıştı. Sürücü Öztürk, burada doktorların tüm müdahalesine rağmen kurtarılamayarak yaşamını yitirdi. 3 çocuk annesi olduğu öğrenilen Öztürk’ün cansız bedeni, savcılık incelemesi ve ön otopsi için morga konuldu. Diğer yaralılardan Enes A., Kahramanmaraş’a sevk edilirken otomobil sürücüsünün de tedavisine burada devam edildiği bildirildi.Kazayla ilgili tahkikat başlatıldı., 
+06 Haz 2021 - 21:00
+-
+Güncel
+Yazdır
+, Yorumunuz yarım kaldı, devam etmek için üstteki yoruma, silmek için buraya tıklayın, Kırmızı alanlar eksik veya hatalı girildi. Lütfen bu alanları düzeltip tekrar gönderelim, Yorumunuz için teşekkürler, en kısa sürede gözden geçirilip yayınlanacaktır, Yorum yazarak Elbistan Kaynarca Topluluk Kuralları’nı kabul etmiş bulunuyor ve yorumunuzla ilgili doğrudan veya dolaylı tüm sorumluluğu tek başınıza üstleniyorsunuz. Yazılan yorumlardan Elbistan Kaynarca hiçbir şekilde sorumlu tutulamaz., Anadolu Ajansı , İhlas Haber Ajansı , Demirören Haber Ajansı  tarafından servis edilen tüm haberler Elbistan Kaynarca editörlerinin hiçbir editöryel müdahalesi olmadan, ajans kanallarından geldiği şekliyle yayınlanmaktadır. Sitemize ajanslar üzerinden aktarılan haberlerin hukuki muhatabı Elbistan Kaynarca değil haberi geçen ajanstır., Şimdi oturum açın, her yorumda isim ve e.posta yazma zahmetinden kurtulun. Oturum açmak için bir hesabınız yoksa, oluşturmak için buraya tıklayın.
+, Yorum yazarak  Elbistan Kaynarca Topluluk Kuralları’nı kabul etmiş bulunuyor ve yorumunuzla ilgili doğrudan veya dolaylı tüm sorumluluğu tek başınıza üstleniyorsunuz. Yazılan yorumlardan Elbistan Kaynarca hiçbir şekilde sorumlu tutulamaz., Anadolu Ajansı , İhlas Haber Ajansı , Demirören Haber Ajansı  tarafından servis edilen tüm haberler Elbistan Kaynarca editörlerinin hiçbir editöryel müdahalesi olmadan, ajans kanallarından geldiği şekliyle yayınlanmaktadır. Sitemize ajanslar üzerinden aktarılan haberlerin hukuki muhatabı Elbistan Kaynarca değil haberi geçen ajanstır., 
+©Copyright 2021 Elbistan Kaynarca Tüm Hakları Saklıdır
+-
+Veri PolitikasıKullanım Şartları
++90  415 04 15
+,  Veri politikasındaki amaçlarla sınırlı ve mevzuata uygun şekilde çerez konumlandırmaktayız. Detaylar için veri politikamızı inceleyebilirsiniz.</t>
+  </si>
+  <si>
+    <t>Motosiklete çarpan sürücü şoka girip gözyaşlarına boğuldu https://t.co/GpMixMBm5m #Gerçek Alanya Gazetesi @gercek_alanya aracılığıyla</t>
+  </si>
+  <si>
+    <t>https://www.gercekalanya.com/asayis/motosiklete-carpan-surucu-soka-girip-gozyaslarina-boguldu-h54786.html</t>
+  </si>
+  <si>
+    <t>Kırmızı ışık ihlali yaptıktan sonra çarpıştığı motosiklet sürücüsünün yaralandığını gören kadın sürücü, şoka girdi. Uzun süre gözyaşı döken kadın güçlükle sakinleştirildi.,  03 Haziran 2021 Perşembe 14:11, Kaza, Manavgat ilçesi Demokrasi Bulvarı girişinde meydana geldi. Edinilen bilgiye göre, Yapaş Şelale istikametinden gelip Demokrasi Bulvarı istikametine gitmekte olan Ümmühan Öz’ün kullandığı 07 LOK 28 plakalı araç, Antalya Caddesi’nde Adliye istikametinden şehir merkezi istikametine seyir halindeki Tuğrul Çuhadar’ın kullandığı 07 APV 872 plakalı motosiklete çarptı.07 LOK 28 plakalı aracın kırmızı ışık ihlali yapması nedeniyle meydana geldiği belirlenen kazada yaralanan motosiklet sürücüsü sağlık ekibinin olay yerindeki müdahalesinin ardından ambulansla hastaneye kaldırıldı., Gözyaşlarına boğuldu, Motosiklet sürücüsünün düşerek yaralandığını gören araç sürücüsü Ümmühan Öz şoka girerken, kaldırıma oturdu ve gözyaşlarına boğuldu. Öz, sağlık ekipleri, vatandaşlar ve trafik ekipleri tarafından güçlükle teskin edildi., Yılanlar fındık bahçelerinde, Türkiye’de en çok manda bulunuyor, Minare ve direkleri leylekler mesken tuttu, Yaylalara göçlerin renkli yolculuğu, Çiçek karakteri farklı yeni bir soğan türü tespit edildi, 
+_x000D_
+ .push;_x000D_
+, 
+_x000D_
+ .push;_x000D_
+, 
+_x000D_
+ .push;_x000D_
+, 
+_x000D_
+ .push;_x000D_
+, 
+_x000D_
+ .push;_x000D_
+, 
+_x000D_
+ .push;_x000D_
+, 
+_x000D_
+ .push;_x000D_
+, 
+_x000D_
+ .push;_x000D_
+, Şekerhane Mahallesi Eczacılar Sokak Burak Apartmanı 18/3 _x000D_
+ALANYA-ANTALYA,  0 242 513 6 513, Yazılım: TE Bilişim</t>
+  </si>
+  <si>
+    <t>Kırmızı ışık ihlali yapıp motosiklete çarpan sürücü şoka girip gözyaşlarına boğuldu #antalya #kaza #asayiş #haberler https://t.co/0cd0LO1I2O</t>
+  </si>
+  <si>
+    <t>https://www.batiakdeniztv.com/asayis/kirmizi-isik-ihlali-yapip-motosiklete-carpan-surucu-soka-girip-h31275.html</t>
+  </si>
+  <si>
+    <t>Antalya’da kırmızı ışık ihlali yaptıktan sonra çarpıştığı motosiklet sürücüsünün yaralandığını gören kadın sürücü, şoka girdi. Uzun süre gözyaşı döken kadın güçlükle sakinleştirildi., Kaza, Manavgat ilçesi Demokrasi Bulvarı girişinde meydana geldi. Edinilen bilgiye göre, Yapaş Şelale istikametinden gelip Demokrasi Bulvarı istikametine gitmekte olan Ümmühan Öz’ün kullandığı 07 LOK 28 plakalı araç, Antalya Caddesi’nde Adliye istikametinden şehir merkezi istikametine seyir halindeki Tuğrul Çuhadar’ın kullandığı 07 APV 872 plakalı motosiklete çarptı.07 LOK 28 plakalı aracın kırmızı ışık ihlali yapması nedeniyle meydana geldiği belirlenen kazada yaralanan motosiklet sürücüsü sağlık ekibinin olay yerindeki müdahalesinin ardından ambulansla hastaneye kaldırıldı., Gözyaşlarına boğuldu, Motosiklet sürücüsünün düşerek yaralandığını gören araç sürücüsü Ümmühan Öz şoka girerken, kaldırıma oturdu ve gözyaşlarına boğuldu. Öz, sağlık ekipleri, vatandaşlar ve trafik ekipleri tarafından güçlükle teskin edildi., Yorumunuz başarılı bir şekilde gönderilmiştir. Editörlerimizin onayının ardından yayınlanacaktır!</t>
+  </si>
+  <si>
+    <t>Motosiklete çarpan kadın sürücü şoka girip gözyaşlarına boğuldu @guncelalanya https://t.co/1USlwU0CMt</t>
+  </si>
+  <si>
+    <t>https://guncelalanya.com/motosiklete-carpan-kadin-surucu-soka-girip-gozyaslarina-boguldu/</t>
+  </si>
+  <si>
+    <t>Bizi sosyal medyada takip edin, SON DAKİKA, 
+Alanya Haber - Güncel Alanya Haber
+,  _x000D_
+			Ak Parti SMA savaşçısı Ahmet bebek için kermes düzenledi		
+,  _x000D_
+			Normalleşmede yeni hedef 21 haziran		
+,  _x000D_
+			Boş sulama kanalına düşen köpek itfaiye tarafından kurtarıldı		
+,  _x000D_
+			Nemanja Milunovic Aytemiz Alanyaspor’da		
+,  _x000D_
+			Boş sulama kanalına düşen köpek itfaiye tarafından kurtarıldı		
+,  _x000D_
+			‘Pandemi bitmiş’ dedirten asker eğlencesi		
+,  _x000D_
+			Yaşlı adam rüzgarın devirdiği cankurtaran kulesinin altında kaldı		
+,  _x000D_
+			Dev karpuzlarla idman yapıp dünya şampiyonasına hazırlanıyor		
+,  _x000D_
+			Emekliye çifte bayram müjdesi! Memura zam geliyor		
+,  _x000D_
+			Bu işletmeler nefes kredisine başvurabilecek		
+,  _x000D_
+			Altın fiyatları zirveye koşuyor		
+,  _x000D_
+			Hibe destekleri ne zaman yatacak?		
+,  _x000D_
+			Nemanja Milunovic Aytemiz Alanyaspor’da		
+,  _x000D_
+			Alanyaspor’da 8 oyuncunun sözleşmesi sona erdi		
+,  _x000D_
+			Pgaec yamaç paraşütü hedef kupası yarışları Alanya’ da		
+,  _x000D_
+			Candeias, Aytemiz Alanyaspor’da		
+,  _x000D_
+			Alanya belediyesi personeline temel ilk yardım eğitimi		
+,  _x000D_
+			ALKÜ’lü akademisyen erken doğumu araştıracak		
+,  _x000D_
+			ALKÜ Tıp fakültesine mükemmeliyet belgesi		
+,  _x000D_
+			Kafe ve restoranlarda günler sonra masaya hizmet		
+,  _x000D_
+			Ak Parti SMA savaşçısı Ahmet bebek için kermes düzenledi		
+,  _x000D_
+			Normalleşmede yeni hedef 21 haziran		
+,  _x000D_
+			Kısıtlamasız ilk cumartesi gününde Alanya sahilleri doldu		
+,  _x000D_
+			Alanya’nın yeni prestij caddesinde sona gelindi		
+,  _x000D_
+			Türkiye 1.si Alanya’dan		
+,  _x000D_
+			Gülden-Metin ikilisi Tosmur’da start alıyor		
+,  _x000D_
+			Gençler doğa ile buluştu, dev maske açtı		
+,  _x000D_
+			Alanyaspor’a maç öncesi meşaleli moral		
+,  _x000D_
+			Alanyalı Topal’dan ikinci albüm		
+,  _x000D_
+			Sahilde sürpriz doğum günü		
+,  _x000D_
+			İstanbul’da yaşayan İranlı ünlü uzmanlar Alanya’da		
+,  _x000D_
+			Şehidimizin adını taşıyan yeğeni ilk yaşını kutladı		
+,  
+,  
+,  
+,  _x000D_
+			Kadın köle veya seks objesi değildir		
+, Kırmızı ışık ihlali yaptıktan sonra çarpıştığı motosiklet sürücüsünün yaralandığını gören kadın sürücü, şoka girdi. Uzun süre gözyaşı döken kadın güçlükle sakinleştirildi.
+Kaza, Manavgat ilçesi Demokrasi Bulvarı girişinde meydana geldi. Edinilen bilgiye göre, Yapaş Şelale istikametinden gelip Demokrasi Bulvarı istikametine gitmekte olan Ümmühan Öz’ün kullandığı 07 LOK 28 plakalı araç, Antalya Caddesi’nde Adliye istikametinden şehir merkezi istikametine seyir halindeki Tuğrul Çuhadar’ın kullandığı 07 APV 872 plakalı motosiklete çarptı.07 LOK 28 plakalı aracın kırmızı ışık ihlali yapması nedeniyle meydana geldiği belirlenen kazada yaralanan motosiklet sürücüsü sağlık ekibinin olay yerindeki müdahalesinin ardından ambulansla hastaneye kaldırıldı., Gözyaşlarına boğuldu
+Motosiklet sürücüsünün düşerek yaralandığını gören araç sürücüsü Ümmühan Öz şoka girerken, kaldırıma oturdu ve gözyaşlarına boğuldu. Öz, sağlık ekipleri, vatandaşlar ve trafik ekipleri tarafından güçlükle teskin edildi.,  Önceki				, Alanya’da polisten uyuşturucu baskını: 4 gözaltı, Sonraki , Kontrol için gittiği serada cansız bedeni bulundu, , , , , ,  
+_x000D_
+				Ak Parti SMA savaşçısı Ahmet bebek için kermes düzenledi			
+, Haberdar olmak için bültenimize abone olun., Paylaşan: 
+, Hoş geldiniz, Hesabınıza giriş yapın., Şifreni Kurtar., Şifre e-postayla gönderilecektir.]</t>
+  </si>
+  <si>
+    <t>Polisten kaçan sürücü bekçilere çarptı: 1'i ağır 2 yaralı - TRT Haber</t>
+  </si>
+  <si>
+    <t>https://www.elbistaninsesi.com/guncel/kazada-agir-yaralanan-surucu-hayata-tutunamadi-h70247.html</t>
+  </si>
+  <si>
+    <t>[06 Haziran 2021 Pazar 20:52, Elbistan’da otomobille cipin çarpışması sonucu yaşanan trafik kazasında ağır yaralanan 37 yaşındaki kadın sürücü, kaldırıldığı hastanede kurtarılamayarak hayatını kaybetti., Orhangazi Mahallesi Eldelek Caddesi’nde meydana gelen kazada; Termik Caddesi yönünde seyir halinde olan Serhat K. İdaresindeki 38 FN 757 plakalı otomobil, sürücüsünün direksiyon hakimiyetini kaybetmesi sonucu, karşı istikametten gelen 37 yaşındaki Hatice Öztürk’ün kullandığı 06 ACN 781 plakalı ciple kafa kafaya çarpışmıştı. Ortalığı savaş alanına çeviren kazada sürücülerle birlikte otomobilin yolcu koltuğundaki Enes A. yaralanmıştı. Durumu ağır olan cip sürücüsü Öztürk ile otomobilde sıkışan yaralılar, itfaiye ekiplerince demir kesme makinesi yardımıyla çıkarılarak hazır bekletilen 112 Acil Servis görevlileri tarafından Elbistan Devlet Hastanesi’ne kaldırılmıştı. Sürücü Öztürk, burada doktorların tüm müdahalesine rağmen kurtarılamayarak yaşamını yitirdi. 3 çocuk annesi olduğu öğrenilen Öztürk’ün cansız bedeni, savcılık incelemesi ve ön otopsi için morga konuldu. Diğer yaralılardan Enes A., Kahramanmaraş’a sevk edilirken otomobil sürücüsünün de tedavisine burada devam edildiği bildirildi., Kazayla ilgili tahkikat başlatıldı. , , , , , 
+_x000D_
+ (adsbygoogle = window.adsbygoogle || []).push({});_x000D_
+, &amp;lt;center&amp;gt;_x000D_
+_x000D_
+0 (344) 415 04 15 &amp;lt;br&amp;gt;_x000D_
+[email protected]_x000D_
+&amp;lt;br&amp;gt;Kızılcaoba Mah. Kışla Cad. 19/1&amp;lt;/center&amp;gt;_x000D_
+_x000D_
+    ,  0 (344) 415 04 15, Bu sitede yayınlanan tüm materyalin her hakkı mahfuzdur. Kaynak gösterilse bile gazetemizin izni olmadan yayınlanamaz., Yazılım: TE Bilişim]</t>
+  </si>
+  <si>
+    <t>Denizli'de polisin "dur" ihtarına uymayan sürücü kaza yapınca yakalandı - TRT Haber</t>
+  </si>
+  <si>
+    <t>[ Antalya'da 2 kadın sürücü, araçlarını durdurup yol ortasında saç saça kavga etti., Öfkeli kadınları erkek sürücüler ayırırken, o anlar cep telefonu kamerasına saniye saniye yansıdı., Antalya'nın Muratpaşa ilçesi 12'nci cadde üzerinde ve yoğun trafikte 2 kadın sürücü kavgaya tutuştu. Aracından inen kadın, diğer kadını önce otomobilinden inmesine fırsat vermemek için kapıyla sıkıştırmaya çalıştı. Kendini kapı engelinden kurtaran kadın, diğer kadın sürücünün üzerine atladı. İki kadın saç saça kavga edip yerde yuvarlandı., , Kadın sürücülerin kavgasını, araçlarını durdurup kavgaya koşan erkek sürücüler ayırdı. Kadın sürücüleri ayırmak oldukça zor olurken, o anlar bir sürücünün cep telefonu kamerasına saniye saniye yansıdı.,  Muratpaşa, Antalya, kavga, Güncel, Son Dakika ,  Kaynak: DHA ,  Son Dakika › Güncel › ANTALYA'DA 2 KADIN SÜRÜCÜ TRAFİKTE SAÇ SAÇA KAVGA ETTİ - Son Dakika , Sondakika.com'un size anlık bildirim göndermesine izin veriyor musunuz?]</t>
+  </si>
+  <si>
+    <t>Kırmızı ışık ihlali yapıp motosiklete çarpan sürücü şoka girip gözyaşlarına boğuldu https://t.co/aMOjEo5E56</t>
+  </si>
+  <si>
+    <t>https://www.afyonpost.com/kirmizi-isik-ihlali-yapip-motosiklete-carpan-surucu-soka-girip-gozyaslarina-boguldu-2/</t>
+  </si>
+  <si>
+    <t>Antalya’da kırmızı ışık ihlali yaptıktan sonra çarpıştığı motosiklet sürücüsünün yaralandığını gören kadın sürücü, şoka girdi. Uzun süre gözyaşı döken kadın güçlükle sakinleştirildi., Kaza, Manavgat ilçesi Demokrasi Bulvarı girişinde meydana geldi. Edinilen bilgiye göre, Yapaş Şelale istikametinden gelip Demokrasi Bulvarı istikametine gitmekte olan Ümmühan Öz’ün kullandığı 07 LOK 28 plakalı araç, Antalya Caddesi’nde Adliye istikametinden şehir merkezi istikametine seyir halindeki Tuğrul Çuhadar’ın kullandığı 07 APV 872 plakalı motosiklete çarptı.07 LOK 28 plakalı aracın kırmızı ışık ihlali yapması nedeniyle meydana geldiği belirlenen kazada yaralanan motosiklet sürücüsü sağlık ekibinin olay yerindeki müdahalesinin ardından ambulansla hastaneye kaldırıldı., Gözyaşlarına boğuldu, Motosiklet sürücüsünün düşerek yaralandığını gören araç sürücüsü Ümmühan Öz şoka girerken, kaldırıma oturdu ve gözyaşlarına boğuldu. Öz, sağlık ekipleri, vatandaşlar ve trafik ekipleri tarafından güçlükle teskin edildi.</t>
   </si>
 </sst>
 </file>
@@ -3279,13 +4331,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E232"/>
+  <dimension ref="A1:E338"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A231" zoomScale="75" workbookViewId="0">
-      <selection activeCell="G232" sqref="G232"/>
+    <sheetView tabSelected="1" topLeftCell="A287" zoomScale="75" workbookViewId="0">
+      <selection activeCell="A339" sqref="A339"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="123" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -3486,7 +4541,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -3556,7 +4611,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -3570,7 +4625,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -3612,7 +4667,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
@@ -3808,7 +4863,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>37</v>
       </c>
@@ -3836,7 +4891,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>39</v>
       </c>
@@ -3850,7 +4905,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>40</v>
       </c>
@@ -3864,7 +4919,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>41</v>
       </c>
@@ -3878,7 +4933,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>42</v>
       </c>
@@ -3892,7 +4947,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>43</v>
       </c>
@@ -3906,7 +4961,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>44</v>
       </c>
@@ -3920,7 +4975,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>45</v>
       </c>
@@ -4004,7 +5059,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>51</v>
       </c>
@@ -4018,7 +5073,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>52</v>
       </c>
@@ -4032,7 +5087,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>53</v>
       </c>
@@ -4060,7 +5115,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>55</v>
       </c>
@@ -4074,7 +5129,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>56</v>
       </c>
@@ -4088,7 +5143,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>57</v>
       </c>
@@ -4116,7 +5171,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>59</v>
       </c>
@@ -4130,7 +5185,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>60</v>
       </c>
@@ -4144,7 +5199,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>61</v>
       </c>
@@ -4158,7 +5213,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>62</v>
       </c>
@@ -4172,7 +5227,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>63</v>
       </c>
@@ -4186,7 +5241,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>64</v>
       </c>
@@ -4214,7 +5269,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>66</v>
       </c>
@@ -4452,7 +5507,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>83</v>
       </c>
@@ -4466,7 +5521,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>84</v>
       </c>
@@ -4480,7 +5535,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>85</v>
       </c>
@@ -6510,7 +7565,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="232" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:4" ht="408" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A232">
         <v>230</v>
       </c>
@@ -6522,6 +7577,1478 @@
       </c>
       <c r="D232" s="3" t="s">
         <v>592</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A233">
+        <v>231</v>
+      </c>
+      <c r="B233" t="s">
+        <v>813</v>
+      </c>
+      <c r="C233" s="2" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A234">
+        <v>232</v>
+      </c>
+      <c r="B234" t="s">
+        <v>814</v>
+      </c>
+      <c r="C234" s="2" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A235">
+        <v>233</v>
+      </c>
+      <c r="B235" t="s">
+        <v>815</v>
+      </c>
+      <c r="C235" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="D235" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A236">
+        <v>234</v>
+      </c>
+      <c r="B236" t="s">
+        <v>816</v>
+      </c>
+      <c r="C236" s="2" t="s">
+        <v>675</v>
+      </c>
+      <c r="D236" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A237">
+        <v>235</v>
+      </c>
+      <c r="B237" t="s">
+        <v>817</v>
+      </c>
+      <c r="C237" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="D237" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A238">
+        <v>236</v>
+      </c>
+      <c r="B238" t="s">
+        <v>818</v>
+      </c>
+      <c r="C238" s="2" t="s">
+        <v>679</v>
+      </c>
+      <c r="D238" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A239">
+        <v>237</v>
+      </c>
+      <c r="B239" t="s">
+        <v>9</v>
+      </c>
+      <c r="C239" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D239" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A240">
+        <v>238</v>
+      </c>
+      <c r="B240" t="s">
+        <v>10</v>
+      </c>
+      <c r="C240" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A241">
+        <v>239</v>
+      </c>
+      <c r="B241" t="s">
+        <v>819</v>
+      </c>
+      <c r="C241" s="2" t="s">
+        <v>682</v>
+      </c>
+      <c r="D241" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A242">
+        <v>240</v>
+      </c>
+      <c r="B242" t="s">
+        <v>12</v>
+      </c>
+      <c r="C242" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="D242" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A243">
+        <v>241</v>
+      </c>
+      <c r="B243" t="s">
+        <v>13</v>
+      </c>
+      <c r="C243" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D243" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A244">
+        <v>242</v>
+      </c>
+      <c r="B244" t="s">
+        <v>14</v>
+      </c>
+      <c r="C244" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="D244" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A245">
+        <v>243</v>
+      </c>
+      <c r="B245" t="s">
+        <v>16</v>
+      </c>
+      <c r="C245" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D245" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A246">
+        <v>244</v>
+      </c>
+      <c r="B246" t="s">
+        <v>820</v>
+      </c>
+      <c r="C246" s="2" t="s">
+        <v>688</v>
+      </c>
+      <c r="D246" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A247">
+        <v>245</v>
+      </c>
+      <c r="B247" t="s">
+        <v>821</v>
+      </c>
+      <c r="C247" s="2" t="s">
+        <v>690</v>
+      </c>
+      <c r="D247" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A248">
+        <v>246</v>
+      </c>
+      <c r="B248" t="s">
+        <v>822</v>
+      </c>
+      <c r="C248" s="2" t="s">
+        <v>692</v>
+      </c>
+      <c r="D248" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A249">
+        <v>247</v>
+      </c>
+      <c r="B249" t="s">
+        <v>21</v>
+      </c>
+      <c r="C249" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="D249" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A250">
+        <v>248</v>
+      </c>
+      <c r="B250" t="s">
+        <v>823</v>
+      </c>
+      <c r="C250" s="2" t="s">
+        <v>695</v>
+      </c>
+      <c r="D250" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A251">
+        <v>249</v>
+      </c>
+      <c r="B251" t="s">
+        <v>23</v>
+      </c>
+      <c r="C251" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D251" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A252">
+        <v>250</v>
+      </c>
+      <c r="B252" t="s">
+        <v>24</v>
+      </c>
+      <c r="C252" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D252" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A253">
+        <v>251</v>
+      </c>
+      <c r="B253" t="s">
+        <v>26</v>
+      </c>
+      <c r="C253" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D253" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A254">
+        <v>252</v>
+      </c>
+      <c r="B254" t="s">
+        <v>27</v>
+      </c>
+      <c r="C254" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="D254" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A255">
+        <v>253</v>
+      </c>
+      <c r="B255" t="s">
+        <v>28</v>
+      </c>
+      <c r="C255" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="D255" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A256">
+        <v>254</v>
+      </c>
+      <c r="B256" t="s">
+        <v>824</v>
+      </c>
+      <c r="C256" s="2" t="s">
+        <v>701</v>
+      </c>
+      <c r="D256" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A257">
+        <v>255</v>
+      </c>
+      <c r="B257" t="s">
+        <v>825</v>
+      </c>
+      <c r="C257" s="2" t="s">
+        <v>703</v>
+      </c>
+      <c r="D257" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A258">
+        <v>256</v>
+      </c>
+      <c r="B258" t="s">
+        <v>31</v>
+      </c>
+      <c r="C258" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D258" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A259">
+        <v>257</v>
+      </c>
+      <c r="B259" t="s">
+        <v>34</v>
+      </c>
+      <c r="C259" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D259" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A260">
+        <v>258</v>
+      </c>
+      <c r="B260" t="s">
+        <v>38</v>
+      </c>
+      <c r="C260" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="D260" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A261">
+        <v>259</v>
+      </c>
+      <c r="B261" t="s">
+        <v>826</v>
+      </c>
+      <c r="C261" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="D261" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A262">
+        <v>260</v>
+      </c>
+      <c r="B262" t="s">
+        <v>40</v>
+      </c>
+      <c r="C262" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="D262" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A263">
+        <v>261</v>
+      </c>
+      <c r="B263" t="s">
+        <v>41</v>
+      </c>
+      <c r="C263" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="D263" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A264">
+        <v>262</v>
+      </c>
+      <c r="B264" t="s">
+        <v>43</v>
+      </c>
+      <c r="C264" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="D264" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A265">
+        <v>263</v>
+      </c>
+      <c r="B265" t="s">
+        <v>827</v>
+      </c>
+      <c r="C265" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="D265" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A266">
+        <v>264</v>
+      </c>
+      <c r="B266" t="s">
+        <v>828</v>
+      </c>
+      <c r="C266" s="2" t="s">
+        <v>715</v>
+      </c>
+      <c r="D266" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A267">
+        <v>265</v>
+      </c>
+      <c r="B267" t="s">
+        <v>829</v>
+      </c>
+      <c r="C267" s="2" t="s">
+        <v>717</v>
+      </c>
+      <c r="D267" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A268">
+        <v>266</v>
+      </c>
+      <c r="B268" t="s">
+        <v>830</v>
+      </c>
+      <c r="C268" s="2" t="s">
+        <v>719</v>
+      </c>
+      <c r="D268" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A269">
+        <v>267</v>
+      </c>
+      <c r="B269" t="s">
+        <v>831</v>
+      </c>
+      <c r="C269" s="2" t="s">
+        <v>721</v>
+      </c>
+      <c r="D269" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A270">
+        <v>268</v>
+      </c>
+      <c r="B270" t="s">
+        <v>832</v>
+      </c>
+      <c r="C270" s="2" t="s">
+        <v>723</v>
+      </c>
+      <c r="D270" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="271" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A271">
+        <v>269</v>
+      </c>
+      <c r="B271" t="s">
+        <v>833</v>
+      </c>
+      <c r="C271" s="2" t="s">
+        <v>725</v>
+      </c>
+      <c r="D271" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A272">
+        <v>270</v>
+      </c>
+      <c r="B272" t="s">
+        <v>46</v>
+      </c>
+      <c r="C272" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="D272" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A273">
+        <v>271</v>
+      </c>
+      <c r="B273" t="s">
+        <v>47</v>
+      </c>
+      <c r="C273" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="D273" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A274">
+        <v>272</v>
+      </c>
+      <c r="B274" t="s">
+        <v>834</v>
+      </c>
+      <c r="C274" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="D274" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A275">
+        <v>273</v>
+      </c>
+      <c r="B275" t="s">
+        <v>835</v>
+      </c>
+      <c r="C275" s="2" t="s">
+        <v>731</v>
+      </c>
+      <c r="D275" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A276">
+        <v>274</v>
+      </c>
+      <c r="B276" t="s">
+        <v>48</v>
+      </c>
+      <c r="C276" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="D276" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A277">
+        <v>275</v>
+      </c>
+      <c r="B277" t="s">
+        <v>49</v>
+      </c>
+      <c r="C277" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="D277" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A278">
+        <v>276</v>
+      </c>
+      <c r="B278" t="s">
+        <v>836</v>
+      </c>
+      <c r="C278" s="2" t="s">
+        <v>735</v>
+      </c>
+      <c r="D278" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A279">
+        <v>277</v>
+      </c>
+      <c r="B279" t="s">
+        <v>50</v>
+      </c>
+      <c r="C279" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="D279" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A280">
+        <v>278</v>
+      </c>
+      <c r="B280" t="s">
+        <v>53</v>
+      </c>
+      <c r="C280" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="D280" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A281">
+        <v>279</v>
+      </c>
+      <c r="B281" t="s">
+        <v>837</v>
+      </c>
+      <c r="C281" s="2" t="s">
+        <v>739</v>
+      </c>
+      <c r="D281" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A282">
+        <v>280</v>
+      </c>
+      <c r="B282" t="s">
+        <v>838</v>
+      </c>
+      <c r="C282" s="2" t="s">
+        <v>741</v>
+      </c>
+      <c r="D282" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A283">
+        <v>281</v>
+      </c>
+      <c r="B283" t="s">
+        <v>54</v>
+      </c>
+      <c r="C283" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="D283" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A284">
+        <v>282</v>
+      </c>
+      <c r="B284" t="s">
+        <v>839</v>
+      </c>
+      <c r="C284" s="2" t="s">
+        <v>744</v>
+      </c>
+      <c r="D284" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A285">
+        <v>283</v>
+      </c>
+      <c r="B285" t="s">
+        <v>840</v>
+      </c>
+      <c r="C285" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="D285" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A286">
+        <v>284</v>
+      </c>
+      <c r="B286" t="s">
+        <v>841</v>
+      </c>
+      <c r="C286" s="2" t="s">
+        <v>747</v>
+      </c>
+      <c r="D286" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A287">
+        <v>285</v>
+      </c>
+      <c r="B287" t="s">
+        <v>57</v>
+      </c>
+      <c r="C287" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="D287" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A288">
+        <v>286</v>
+      </c>
+      <c r="B288" t="s">
+        <v>842</v>
+      </c>
+      <c r="C288" s="2" t="s">
+        <v>750</v>
+      </c>
+      <c r="D288" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A289">
+        <v>287</v>
+      </c>
+      <c r="B289" t="s">
+        <v>843</v>
+      </c>
+      <c r="C289" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="D289" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A290">
+        <v>288</v>
+      </c>
+      <c r="B290" t="s">
+        <v>844</v>
+      </c>
+      <c r="C290" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="D290" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A291">
+        <v>289</v>
+      </c>
+      <c r="B291" t="s">
+        <v>845</v>
+      </c>
+      <c r="C291" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="D291" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="292" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A292">
+        <v>290</v>
+      </c>
+      <c r="B292" t="s">
+        <v>846</v>
+      </c>
+      <c r="C292" s="2" t="s">
+        <v>757</v>
+      </c>
+      <c r="D292" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="293" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A293">
+        <v>291</v>
+      </c>
+      <c r="B293" t="s">
+        <v>59</v>
+      </c>
+      <c r="C293" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="D293" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="294" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A294">
+        <v>292</v>
+      </c>
+      <c r="B294" t="s">
+        <v>847</v>
+      </c>
+      <c r="C294" s="2" t="s">
+        <v>760</v>
+      </c>
+      <c r="D294" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="295" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A295">
+        <v>293</v>
+      </c>
+      <c r="B295" t="s">
+        <v>848</v>
+      </c>
+      <c r="C295" s="2" t="s">
+        <v>762</v>
+      </c>
+      <c r="D295" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="296" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A296">
+        <v>294</v>
+      </c>
+      <c r="B296" t="s">
+        <v>849</v>
+      </c>
+      <c r="C296" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="D296" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="297" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A297">
+        <v>295</v>
+      </c>
+      <c r="B297" t="s">
+        <v>62</v>
+      </c>
+      <c r="C297" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="298" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A298">
+        <v>296</v>
+      </c>
+      <c r="B298" t="s">
+        <v>63</v>
+      </c>
+      <c r="C298" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="D298" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="299" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A299">
+        <v>297</v>
+      </c>
+      <c r="B299" t="s">
+        <v>64</v>
+      </c>
+      <c r="C299" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="D299" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="300" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A300">
+        <v>298</v>
+      </c>
+      <c r="B300" t="s">
+        <v>65</v>
+      </c>
+      <c r="C300" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="D300" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="301" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A301">
+        <v>299</v>
+      </c>
+      <c r="B301" t="s">
+        <v>850</v>
+      </c>
+      <c r="C301" s="2" t="s">
+        <v>769</v>
+      </c>
+      <c r="D301" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="302" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A302">
+        <v>300</v>
+      </c>
+      <c r="B302" t="s">
+        <v>851</v>
+      </c>
+      <c r="C302" s="2" t="s">
+        <v>771</v>
+      </c>
+      <c r="D302" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="303" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A303">
+        <v>301</v>
+      </c>
+      <c r="B303" t="s">
+        <v>70</v>
+      </c>
+      <c r="C303" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="D303" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="304" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A304">
+        <v>302</v>
+      </c>
+      <c r="B304" t="s">
+        <v>71</v>
+      </c>
+      <c r="C304" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="D304" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="305" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A305">
+        <v>303</v>
+      </c>
+      <c r="B305" t="s">
+        <v>852</v>
+      </c>
+      <c r="C305" s="2" t="s">
+        <v>775</v>
+      </c>
+      <c r="D305" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="306" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A306">
+        <v>304</v>
+      </c>
+      <c r="B306" t="s">
+        <v>72</v>
+      </c>
+      <c r="C306" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D306" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="307" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A307">
+        <v>305</v>
+      </c>
+      <c r="B307" t="s">
+        <v>853</v>
+      </c>
+      <c r="C307" s="2" t="s">
+        <v>778</v>
+      </c>
+      <c r="D307" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="308" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A308">
+        <v>306</v>
+      </c>
+      <c r="B308" t="s">
+        <v>854</v>
+      </c>
+      <c r="C308" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="D308" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="309" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A309">
+        <v>307</v>
+      </c>
+      <c r="B309" t="s">
+        <v>855</v>
+      </c>
+      <c r="C309" s="2" t="s">
+        <v>782</v>
+      </c>
+      <c r="D309" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="310" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A310">
+        <v>308</v>
+      </c>
+      <c r="B310" t="s">
+        <v>74</v>
+      </c>
+      <c r="C310" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="D310" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="311" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A311">
+        <v>309</v>
+      </c>
+      <c r="B311" t="s">
+        <v>76</v>
+      </c>
+      <c r="C311" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="D311" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="312" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A312">
+        <v>310</v>
+      </c>
+      <c r="B312" t="s">
+        <v>77</v>
+      </c>
+      <c r="C312" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="D312" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="313" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A313">
+        <v>311</v>
+      </c>
+      <c r="B313" t="s">
+        <v>79</v>
+      </c>
+      <c r="C313" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="D313" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="314" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A314">
+        <v>312</v>
+      </c>
+      <c r="B314" t="s">
+        <v>82</v>
+      </c>
+      <c r="C314" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="D314" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="315" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A315">
+        <v>313</v>
+      </c>
+      <c r="B315" t="s">
+        <v>83</v>
+      </c>
+      <c r="C315" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="D315" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="316" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A316">
+        <v>314</v>
+      </c>
+      <c r="B316" t="s">
+        <v>856</v>
+      </c>
+      <c r="C316" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="D316" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="317" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A317">
+        <v>315</v>
+      </c>
+      <c r="B317" t="s">
+        <v>857</v>
+      </c>
+      <c r="C317" s="2" t="s">
+        <v>791</v>
+      </c>
+      <c r="D317" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="318" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A318">
+        <v>316</v>
+      </c>
+      <c r="B318" t="s">
+        <v>85</v>
+      </c>
+      <c r="C318" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="D318" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="319" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A319">
+        <v>317</v>
+      </c>
+      <c r="B319" t="s">
+        <v>86</v>
+      </c>
+      <c r="C319" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D319" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="320" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A320">
+        <v>318</v>
+      </c>
+      <c r="B320" t="s">
+        <v>858</v>
+      </c>
+      <c r="C320" s="2" t="s">
+        <v>795</v>
+      </c>
+      <c r="D320" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="321" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A321">
+        <v>319</v>
+      </c>
+      <c r="B321" t="s">
+        <v>859</v>
+      </c>
+      <c r="C321" s="2" t="s">
+        <v>797</v>
+      </c>
+      <c r="D321" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="322" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A322">
+        <v>320</v>
+      </c>
+      <c r="B322" t="s">
+        <v>860</v>
+      </c>
+      <c r="C322" s="2" t="s">
+        <v>799</v>
+      </c>
+      <c r="D322" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="323" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A323">
+        <v>321</v>
+      </c>
+      <c r="B323" t="s">
+        <v>861</v>
+      </c>
+      <c r="C323" s="2" t="s">
+        <v>801</v>
+      </c>
+      <c r="D323" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="324" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A324">
+        <v>322</v>
+      </c>
+      <c r="B324" t="s">
+        <v>89</v>
+      </c>
+      <c r="C324" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D324" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="325" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A325">
+        <v>323</v>
+      </c>
+      <c r="B325" t="s">
+        <v>862</v>
+      </c>
+      <c r="C325" s="2" t="s">
+        <v>804</v>
+      </c>
+      <c r="D325" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="326" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A326">
+        <v>324</v>
+      </c>
+      <c r="B326" t="s">
+        <v>863</v>
+      </c>
+      <c r="C326" s="2" t="s">
+        <v>806</v>
+      </c>
+      <c r="D326" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="327" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A327">
+        <v>325</v>
+      </c>
+      <c r="B327" t="s">
+        <v>92</v>
+      </c>
+      <c r="C327" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="D327" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="328" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A328">
+        <v>326</v>
+      </c>
+      <c r="B328" t="s">
+        <v>93</v>
+      </c>
+      <c r="C328" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="D328" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="329" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A329">
+        <v>327</v>
+      </c>
+      <c r="B329" t="s">
+        <v>864</v>
+      </c>
+      <c r="C329" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="D329" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="330" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A330">
+        <v>328</v>
+      </c>
+      <c r="B330" t="s">
+        <v>865</v>
+      </c>
+      <c r="C330" s="2" t="s">
+        <v>811</v>
+      </c>
+      <c r="D330" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="331" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A331">
+        <v>329</v>
+      </c>
+      <c r="B331" t="s">
+        <v>866</v>
+      </c>
+      <c r="C331" s="2" t="s">
+        <v>867</v>
+      </c>
+      <c r="D331" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="332" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A332">
+        <v>330</v>
+      </c>
+      <c r="B332" t="s">
+        <v>869</v>
+      </c>
+      <c r="C332" s="2" t="s">
+        <v>870</v>
+      </c>
+      <c r="D332" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="333" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A333">
+        <v>331</v>
+      </c>
+      <c r="B333" t="s">
+        <v>872</v>
+      </c>
+      <c r="C333" s="2" t="s">
+        <v>873</v>
+      </c>
+      <c r="D333" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="334" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A334">
+        <v>332</v>
+      </c>
+      <c r="B334" t="s">
+        <v>875</v>
+      </c>
+      <c r="C334" s="2" t="s">
+        <v>876</v>
+      </c>
+      <c r="D334" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="335" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A335">
+        <v>333</v>
+      </c>
+      <c r="B335" t="s">
+        <v>878</v>
+      </c>
+      <c r="C335" s="2" t="s">
+        <v>879</v>
+      </c>
+      <c r="D335" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="336" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A336">
+        <v>334</v>
+      </c>
+      <c r="B336" t="s">
+        <v>881</v>
+      </c>
+      <c r="C336" s="2" t="s">
+        <v>882</v>
+      </c>
+      <c r="D336" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="337" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A337">
+        <v>335</v>
+      </c>
+      <c r="B337" t="s">
+        <v>884</v>
+      </c>
+      <c r="C337" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="D337" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="338" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A338">
+        <v>336</v>
+      </c>
+      <c r="B338" t="s">
+        <v>886</v>
+      </c>
+      <c r="C338" s="2" t="s">
+        <v>887</v>
+      </c>
+      <c r="D338" t="s">
+        <v>888</v>
       </c>
     </row>
   </sheetData>
@@ -6750,6 +9277,112 @@
     <hyperlink ref="C217" r:id="rId222" xr:uid="{B74AB779-4FC0-A14E-9D22-825A7E7598D1}"/>
     <hyperlink ref="C214" r:id="rId223" xr:uid="{B2E3FFBB-8325-8D46-A1A7-CC62A7F739AE}"/>
     <hyperlink ref="C213" r:id="rId224" xr:uid="{D1015901-8155-1244-902C-478625A60F74}"/>
+    <hyperlink ref="C233" r:id="rId225" xr:uid="{73D9C7C6-8FCE-F64C-8337-765A2275F849}"/>
+    <hyperlink ref="C234" r:id="rId226" xr:uid="{6EF066A5-703D-8F40-9CB1-4BBDD9D3ABEF}"/>
+    <hyperlink ref="C235" r:id="rId227" xr:uid="{BD5280AF-0911-A744-B80E-2328386D3E8C}"/>
+    <hyperlink ref="C236" r:id="rId228" xr:uid="{EB6BD41F-D3AD-514B-A4A3-70695105F3D0}"/>
+    <hyperlink ref="C237" r:id="rId229" xr:uid="{BA003BC7-4266-9040-962E-B08584BEED43}"/>
+    <hyperlink ref="C238" r:id="rId230" xr:uid="{51663CBF-6376-0E48-9D14-B1EE652E2758}"/>
+    <hyperlink ref="C239" r:id="rId231" xr:uid="{5E0198A3-5DA5-1B40-8460-41387ACDE18C}"/>
+    <hyperlink ref="C240" r:id="rId232" xr:uid="{B052CBB3-8852-CE43-AF64-719BF4F49081}"/>
+    <hyperlink ref="C241" r:id="rId233" xr:uid="{2C63B8BA-1070-1142-B3CD-9189C966CC39}"/>
+    <hyperlink ref="C242" r:id="rId234" xr:uid="{248F0133-EB13-A044-B90E-FDFCC8E84F43}"/>
+    <hyperlink ref="C243" r:id="rId235" xr:uid="{BC805C06-FA82-2B4E-89D5-9FF927F92917}"/>
+    <hyperlink ref="C244" r:id="rId236" xr:uid="{6EA896F7-0B47-3549-9D8F-D20FD2F39322}"/>
+    <hyperlink ref="C245" r:id="rId237" xr:uid="{2B053253-CB38-F643-AB86-7929C4E03879}"/>
+    <hyperlink ref="C246" r:id="rId238" xr:uid="{05AB7890-F155-544C-850D-810A97C94BFA}"/>
+    <hyperlink ref="C247" r:id="rId239" xr:uid="{A3C1B3C6-6D23-EB40-BA42-BE68E0BDFFFE}"/>
+    <hyperlink ref="C248" r:id="rId240" xr:uid="{35B7F48C-F458-494B-991A-A1ECC5BC0963}"/>
+    <hyperlink ref="C249" r:id="rId241" xr:uid="{77ACC825-153C-4C43-B496-2AB1D9916CA9}"/>
+    <hyperlink ref="C250" r:id="rId242" xr:uid="{F1FBCE59-BFAE-244E-A6E0-ADFBA117DE64}"/>
+    <hyperlink ref="C251" r:id="rId243" xr:uid="{2AF4E4A8-64C9-574E-849E-D6461F6A2A4A}"/>
+    <hyperlink ref="C252" r:id="rId244" xr:uid="{BD2A26A0-FC93-184E-8CF4-DDEFDDF4636F}"/>
+    <hyperlink ref="C253" r:id="rId245" xr:uid="{0B3E9404-4360-1B44-B7CE-9A28CD98388C}"/>
+    <hyperlink ref="C254" r:id="rId246" xr:uid="{E595C7EA-5FC7-E34B-B1DB-FC17DA0E9EC9}"/>
+    <hyperlink ref="C255" r:id="rId247" xr:uid="{591674B9-714C-E34C-B725-57D820A56A00}"/>
+    <hyperlink ref="C256" r:id="rId248" xr:uid="{A079639F-3EE2-0845-845C-EE8416288FB3}"/>
+    <hyperlink ref="C257" r:id="rId249" xr:uid="{182B0FE9-E73D-7045-BCD1-047FA0DB0C18}"/>
+    <hyperlink ref="C258" r:id="rId250" xr:uid="{9A3E67AD-3965-E84B-82A0-952B20285D91}"/>
+    <hyperlink ref="C259" r:id="rId251" xr:uid="{0321A780-F973-8B48-900F-C4FC48165C0F}"/>
+    <hyperlink ref="C260" r:id="rId252" xr:uid="{872FED43-8D4D-D845-9EA8-362C9532D53F}"/>
+    <hyperlink ref="C261" r:id="rId253" xr:uid="{E17503D0-973D-3E4D-99F6-6FE31C1337E1}"/>
+    <hyperlink ref="C262" r:id="rId254" xr:uid="{3EC9E408-8EE6-E24C-BB0A-7DEFF931FE4C}"/>
+    <hyperlink ref="C263" r:id="rId255" xr:uid="{B1C77A8B-5A5E-ED46-B901-093E5507B9FB}"/>
+    <hyperlink ref="C264" r:id="rId256" xr:uid="{BFCBCF07-2CB6-1D45-AE37-14F74A7DDA3D}"/>
+    <hyperlink ref="C265" r:id="rId257" xr:uid="{7114238C-654B-8A4C-AB6D-D41B71B9197C}"/>
+    <hyperlink ref="C266" r:id="rId258" xr:uid="{85487C6B-F4BC-4A40-914E-0EA998A60FC3}"/>
+    <hyperlink ref="C267" r:id="rId259" xr:uid="{AD308052-15D6-2548-A1AC-7AC5AE355645}"/>
+    <hyperlink ref="C268" r:id="rId260" xr:uid="{D742E675-0A22-514E-9F3F-C0321DCC0F2B}"/>
+    <hyperlink ref="C269" r:id="rId261" xr:uid="{3823CAC5-E4DB-9E42-A93C-2542C30C4A9C}"/>
+    <hyperlink ref="C270" r:id="rId262" xr:uid="{D0DD9559-BBE7-5F40-9253-3B915B479783}"/>
+    <hyperlink ref="C271" r:id="rId263" xr:uid="{12FB7102-EEBE-A040-831D-3026639DBF0B}"/>
+    <hyperlink ref="C272" r:id="rId264" xr:uid="{9BDA2911-1BF7-2D45-9396-63F292AA11C4}"/>
+    <hyperlink ref="C273" r:id="rId265" xr:uid="{B8A274CE-AF2F-0A4E-B4EA-53CB6BE0185E}"/>
+    <hyperlink ref="C274" r:id="rId266" xr:uid="{859C166C-8DA9-6640-937D-6B6F8CD9F2FD}"/>
+    <hyperlink ref="C275" r:id="rId267" xr:uid="{D27EDDAE-90C0-AE48-B47D-D985393A26F6}"/>
+    <hyperlink ref="C276" r:id="rId268" xr:uid="{D4FF7345-BAB9-874A-BC81-B30658FFA971}"/>
+    <hyperlink ref="C277" r:id="rId269" xr:uid="{D1B71E5A-3B35-7941-9DEF-1E11CC9969DF}"/>
+    <hyperlink ref="C278" r:id="rId270" xr:uid="{576FDB10-8EF0-9B44-B961-4A080D521722}"/>
+    <hyperlink ref="C279" r:id="rId271" xr:uid="{79E56F24-0C64-C143-9B7A-E35B89700A55}"/>
+    <hyperlink ref="C280" r:id="rId272" xr:uid="{26DCE153-EE00-A04E-A63B-EC14E741BB27}"/>
+    <hyperlink ref="C281" r:id="rId273" xr:uid="{EA98D7A4-7E4A-7E4A-8BAB-290F5BE5CD3D}"/>
+    <hyperlink ref="C282" r:id="rId274" xr:uid="{1332298E-7152-014E-8BBF-77DEF7084DC7}"/>
+    <hyperlink ref="C283" r:id="rId275" xr:uid="{2D2DC994-4CEB-B74F-86E9-6F2569B99403}"/>
+    <hyperlink ref="C284" r:id="rId276" xr:uid="{9B069E54-E899-D94F-9736-05D99BDA3C48}"/>
+    <hyperlink ref="C285" r:id="rId277" xr:uid="{2E4D493B-F78D-B047-A474-8552415347FD}"/>
+    <hyperlink ref="C286" r:id="rId278" xr:uid="{F5C579C3-3481-E147-9987-C3A487CBC014}"/>
+    <hyperlink ref="C287" r:id="rId279" xr:uid="{AC785D0D-BE62-764B-9BBB-B22B2D4E6B75}"/>
+    <hyperlink ref="C288" r:id="rId280" xr:uid="{E8126938-384E-D548-8D89-9F3EB04D1261}"/>
+    <hyperlink ref="C289" r:id="rId281" xr:uid="{34804B9F-A7D7-5144-B79C-DEA7D071D383}"/>
+    <hyperlink ref="C290" r:id="rId282" xr:uid="{4D1E6458-6A72-434D-9E84-127E44194B1B}"/>
+    <hyperlink ref="C291" r:id="rId283" xr:uid="{AE4264DC-0FF5-B849-8F48-0F8C1CD94A41}"/>
+    <hyperlink ref="C292" r:id="rId284" xr:uid="{045DAC65-57E4-C844-B56B-B3658C12C187}"/>
+    <hyperlink ref="C293" r:id="rId285" xr:uid="{656DF242-BEDE-454B-B42E-1DB3F7282C68}"/>
+    <hyperlink ref="C294" r:id="rId286" xr:uid="{DDF2FA47-521E-C14E-BCA5-378001EC9EA0}"/>
+    <hyperlink ref="C295" r:id="rId287" xr:uid="{DF8A08C4-E632-5C4F-8FA4-B14DC291F62D}"/>
+    <hyperlink ref="C296" r:id="rId288" xr:uid="{FE9A81EB-21EB-FE46-8AF2-7D18CCB26966}"/>
+    <hyperlink ref="C297" r:id="rId289" xr:uid="{B106BB1C-0587-B949-AE0E-4D07B5B47A8B}"/>
+    <hyperlink ref="C298" r:id="rId290" xr:uid="{4E2921C4-BC58-B74C-BA33-0D5F08976270}"/>
+    <hyperlink ref="C299" r:id="rId291" xr:uid="{6D938686-AA64-A148-9A73-5B37B4AD82F6}"/>
+    <hyperlink ref="C300" r:id="rId292" xr:uid="{060ABD9A-BC84-9E42-B4DC-737B6A3A721C}"/>
+    <hyperlink ref="C301" r:id="rId293" xr:uid="{82174C6C-47EA-BE49-8AA2-8D3A091A8124}"/>
+    <hyperlink ref="C302" r:id="rId294" xr:uid="{4B475902-B282-EE43-B43A-37C8B69806C3}"/>
+    <hyperlink ref="C303" r:id="rId295" xr:uid="{8A245D74-20D9-6B4A-A99E-B93E1111DE86}"/>
+    <hyperlink ref="C304" r:id="rId296" xr:uid="{5F0298AA-98EA-2F42-91B6-277D4BC8C1CD}"/>
+    <hyperlink ref="C305" r:id="rId297" xr:uid="{3CD92367-A231-3441-A855-1DF8124152C0}"/>
+    <hyperlink ref="C306" r:id="rId298" xr:uid="{483DE20F-74EB-6546-8B8D-82B7E3B7C081}"/>
+    <hyperlink ref="C307" r:id="rId299" xr:uid="{47D0F75E-0A30-8D42-97E6-75B87F2C78EC}"/>
+    <hyperlink ref="C308" r:id="rId300" xr:uid="{40D859F7-E537-4140-AC20-6597A733E072}"/>
+    <hyperlink ref="C309" r:id="rId301" xr:uid="{61E1A65D-D584-7A4C-9B34-5FEB1EF48719}"/>
+    <hyperlink ref="C310" r:id="rId302" xr:uid="{A4BD5F5E-E9DC-3F4C-9656-BED1598D413D}"/>
+    <hyperlink ref="C311" r:id="rId303" xr:uid="{00279377-FD9E-B24F-90F0-986B7CCBCC90}"/>
+    <hyperlink ref="C312" r:id="rId304" xr:uid="{1B6E1A7A-2570-984C-9585-3CA3A99E688F}"/>
+    <hyperlink ref="C313" r:id="rId305" xr:uid="{96EC15E5-979E-AB4F-B417-F062D6BBEF2B}"/>
+    <hyperlink ref="C314" r:id="rId306" xr:uid="{15A9D6FA-E642-E340-B9E5-C82FFFE2569E}"/>
+    <hyperlink ref="C315" r:id="rId307" xr:uid="{159E5513-92BC-9042-B503-2A77A4CD31FD}"/>
+    <hyperlink ref="C316" r:id="rId308" xr:uid="{3A514B95-CA01-A347-BB16-8C0D46337FA8}"/>
+    <hyperlink ref="C317" r:id="rId309" xr:uid="{DA169392-411B-664F-B544-0441EFF5E5E0}"/>
+    <hyperlink ref="C318" r:id="rId310" xr:uid="{B1293505-DBD2-0D45-AF5D-FF1D07E97EDA}"/>
+    <hyperlink ref="C319" r:id="rId311" xr:uid="{B694297E-D38B-604C-BE47-A6890B347B30}"/>
+    <hyperlink ref="C320" r:id="rId312" xr:uid="{8D9CC1D1-FA96-984A-8FBE-12A3227BCEB3}"/>
+    <hyperlink ref="C321" r:id="rId313" xr:uid="{2815443D-01D7-6B43-A162-325AC6D26F4E}"/>
+    <hyperlink ref="C322" r:id="rId314" xr:uid="{64680E4D-23BC-EF47-8797-681811EFF926}"/>
+    <hyperlink ref="C323" r:id="rId315" xr:uid="{8F68E88B-EEE6-B94B-B235-0552E485DF2D}"/>
+    <hyperlink ref="C324" r:id="rId316" xr:uid="{41B84924-FCAD-2D42-BAD2-F45DD5D251D4}"/>
+    <hyperlink ref="C325" r:id="rId317" xr:uid="{BCDCA171-3CEF-A14B-8755-973D49949DC0}"/>
+    <hyperlink ref="C326" r:id="rId318" xr:uid="{40DDFF14-F2A7-2142-A042-9322E59C7F52}"/>
+    <hyperlink ref="C327" r:id="rId319" xr:uid="{B7CE2DB0-CD30-9E41-AA66-2315FE6944DE}"/>
+    <hyperlink ref="C328" r:id="rId320" xr:uid="{3612B26A-8622-A142-9F29-1FBBE3F8724E}"/>
+    <hyperlink ref="C329" r:id="rId321" xr:uid="{9601F953-9D47-0E45-91F2-DE486EC63F5F}"/>
+    <hyperlink ref="C330" r:id="rId322" xr:uid="{DC7EDC9D-5C54-4449-9063-9A40627572C5}"/>
+    <hyperlink ref="C331" r:id="rId323" xr:uid="{21556B13-77DF-8444-B6DA-4BDAFC3BA939}"/>
+    <hyperlink ref="C332" r:id="rId324" xr:uid="{B6CD55B8-CE3F-CF45-8516-26BFECE51711}"/>
+    <hyperlink ref="C333" r:id="rId325" xr:uid="{852AC053-3395-054A-8AFA-30BEFC7BDFC8}"/>
+    <hyperlink ref="C334" r:id="rId326" xr:uid="{BDC020AD-5A51-924C-8756-1031DD5CD347}"/>
+    <hyperlink ref="C335" r:id="rId327" xr:uid="{FB6018DE-949B-2444-AE86-077BDA6391F2}"/>
+    <hyperlink ref="C336" r:id="rId328" xr:uid="{0ADE7B18-0E31-4E4E-A279-ADEB2EC07FA9}"/>
+    <hyperlink ref="C337" r:id="rId329" xr:uid="{2D9E3871-4339-EE4F-BA5E-68FF897A4B7A}"/>
+    <hyperlink ref="C338" r:id="rId330" xr:uid="{11CA4843-1A2F-3D40-BBAC-B2719EB31D7E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>